<commit_message>
Update: Fundamental pages added
</commit_message>
<xml_diff>
--- a/Group C2-3 Scrum documentation.xlsx
+++ b/Group C2-3 Scrum documentation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johna\OneDrive\Documents\University\Year II\CO553 Agile Development and Software Security B\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johna\OneDrive\Documents\University\Year II\CO553 Agile Development and Software Security B\co553-c2-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DFA178E-7DC8-4A6E-8100-698F395ECEB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6C9013A-E3BB-4C35-A462-45775F5A6ECD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3810" yWindow="3810" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{0CC9FE5D-919A-41CA-B32D-5FFC3808111C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{0CC9FE5D-919A-41CA-B32D-5FFC3808111C}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -234,7 +234,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -256,8 +256,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -274,6 +295,21 @@
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -405,10 +441,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -430,37 +469,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="8" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="2" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2169,8 +2214,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1498325-30FB-42AD-97E8-3EAEC03F161C}">
   <dimension ref="B2:V24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2180,37 +2225,37 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="28"/>
-      <c r="O2" s="28"/>
-      <c r="P2" s="28"/>
-      <c r="Q2" s="28"/>
-      <c r="R2" s="28"/>
-      <c r="S2" s="28"/>
-      <c r="T2" s="28"/>
-      <c r="U2" s="28"/>
-      <c r="V2" s="28"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="23"/>
+      <c r="O2" s="23"/>
+      <c r="P2" s="23"/>
+      <c r="Q2" s="23"/>
+      <c r="R2" s="23"/>
+      <c r="S2" s="23"/>
+      <c r="T2" s="23"/>
+      <c r="U2" s="23"/>
+      <c r="V2" s="23"/>
     </row>
     <row r="3" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
       <c r="D3" s="9">
         <v>44221</v>
       </c>
@@ -2270,31 +2315,31 @@
       </c>
     </row>
     <row r="4" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="21" t="s">
         <v>22</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="18">
-        <v>0</v>
-      </c>
-      <c r="E4" s="11">
+      <c r="D4" s="13">
+        <v>0</v>
+      </c>
+      <c r="E4" s="27">
         <v>0.25</v>
       </c>
-      <c r="F4" s="3">
-        <v>0</v>
-      </c>
-      <c r="G4" s="3">
-        <v>0</v>
-      </c>
-      <c r="H4" s="3">
-        <v>0</v>
-      </c>
-      <c r="I4" s="3">
-        <v>0</v>
-      </c>
-      <c r="J4" s="3">
+      <c r="F4" s="30">
+        <v>0</v>
+      </c>
+      <c r="G4" s="30">
+        <v>0</v>
+      </c>
+      <c r="H4" s="30">
+        <v>0</v>
+      </c>
+      <c r="I4" s="30">
+        <v>0</v>
+      </c>
+      <c r="J4" s="30">
         <v>0</v>
       </c>
       <c r="K4" s="3">
@@ -2330,34 +2375,34 @@
       <c r="U4" s="3">
         <v>0</v>
       </c>
-      <c r="V4" s="21">
+      <c r="V4" s="16">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B5" s="30"/>
+      <c r="B5" s="24"/>
       <c r="C5" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="D5" s="19">
-        <v>0</v>
-      </c>
-      <c r="E5" s="11">
+      <c r="D5" s="14">
+        <v>0</v>
+      </c>
+      <c r="E5" s="27">
         <v>0.25</v>
       </c>
-      <c r="F5" s="3">
-        <v>0</v>
-      </c>
-      <c r="G5" s="3">
-        <v>0</v>
-      </c>
-      <c r="H5" s="3">
-        <v>0</v>
-      </c>
-      <c r="I5" s="3">
-        <v>0</v>
-      </c>
-      <c r="J5" s="3">
+      <c r="F5" s="30">
+        <v>0</v>
+      </c>
+      <c r="G5" s="30">
+        <v>0</v>
+      </c>
+      <c r="H5" s="30">
+        <v>0</v>
+      </c>
+      <c r="I5" s="30">
+        <v>0</v>
+      </c>
+      <c r="J5" s="30">
         <v>0</v>
       </c>
       <c r="K5" s="3">
@@ -2393,34 +2438,34 @@
       <c r="U5" s="3">
         <v>0</v>
       </c>
-      <c r="V5" s="22">
+      <c r="V5" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B6" s="30"/>
+      <c r="B6" s="24"/>
       <c r="C6" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D6" s="19">
-        <v>0</v>
-      </c>
-      <c r="E6" s="11">
+      <c r="D6" s="14">
+        <v>0</v>
+      </c>
+      <c r="E6" s="25">
         <v>0.25</v>
       </c>
-      <c r="F6" s="3">
-        <v>0</v>
-      </c>
-      <c r="G6" s="3">
-        <v>0</v>
-      </c>
-      <c r="H6" s="3">
-        <v>0</v>
-      </c>
-      <c r="I6" s="3">
-        <v>0</v>
-      </c>
-      <c r="J6" s="3">
+      <c r="F6" s="30">
+        <v>0</v>
+      </c>
+      <c r="G6" s="30">
+        <v>0</v>
+      </c>
+      <c r="H6" s="30">
+        <v>0</v>
+      </c>
+      <c r="I6" s="30">
+        <v>0</v>
+      </c>
+      <c r="J6" s="30">
         <v>0</v>
       </c>
       <c r="K6" s="3">
@@ -2456,34 +2501,34 @@
       <c r="U6" s="3">
         <v>0</v>
       </c>
-      <c r="V6" s="22">
+      <c r="V6" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B7" s="31"/>
+      <c r="B7" s="22"/>
       <c r="C7" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="20">
-        <v>0</v>
-      </c>
-      <c r="E7" s="12">
+      <c r="D7" s="15">
+        <v>0</v>
+      </c>
+      <c r="E7" s="26">
         <v>0.25</v>
       </c>
-      <c r="F7" s="4">
-        <v>0</v>
-      </c>
-      <c r="G7" s="4">
-        <v>0</v>
-      </c>
-      <c r="H7" s="4">
-        <v>0</v>
-      </c>
-      <c r="I7" s="4">
-        <v>0</v>
-      </c>
-      <c r="J7" s="4">
+      <c r="F7" s="31">
+        <v>0</v>
+      </c>
+      <c r="G7" s="31">
+        <v>0</v>
+      </c>
+      <c r="H7" s="31">
+        <v>0</v>
+      </c>
+      <c r="I7" s="31">
+        <v>0</v>
+      </c>
+      <c r="J7" s="31">
         <v>0</v>
       </c>
       <c r="K7" s="4">
@@ -2519,99 +2564,99 @@
       <c r="U7" s="4">
         <v>0</v>
       </c>
-      <c r="V7" s="23">
+      <c r="V7" s="18">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="18">
-        <v>0</v>
-      </c>
-      <c r="E8" s="14">
-        <v>0</v>
-      </c>
-      <c r="F8" s="15">
+      <c r="D8" s="13">
+        <v>0</v>
+      </c>
+      <c r="E8" s="29">
+        <v>0</v>
+      </c>
+      <c r="F8" s="28">
         <v>1</v>
       </c>
-      <c r="G8" s="14">
-        <v>0</v>
-      </c>
-      <c r="H8" s="14">
-        <v>0</v>
-      </c>
-      <c r="I8" s="14">
-        <v>0</v>
-      </c>
-      <c r="J8" s="14">
-        <v>0</v>
-      </c>
-      <c r="K8" s="14">
-        <v>0</v>
-      </c>
-      <c r="L8" s="14">
-        <v>0</v>
-      </c>
-      <c r="M8" s="14">
-        <v>0</v>
-      </c>
-      <c r="N8" s="14">
-        <v>0</v>
-      </c>
-      <c r="O8" s="14">
-        <v>0</v>
-      </c>
-      <c r="P8" s="14">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="14">
-        <v>0</v>
-      </c>
-      <c r="R8" s="14">
-        <v>0</v>
-      </c>
-      <c r="S8" s="14">
-        <v>0</v>
-      </c>
-      <c r="T8" s="14">
-        <v>0</v>
-      </c>
-      <c r="U8" s="14">
-        <v>0</v>
-      </c>
-      <c r="V8" s="21">
+      <c r="G8" s="29">
+        <v>0</v>
+      </c>
+      <c r="H8" s="29">
+        <v>0</v>
+      </c>
+      <c r="I8" s="29">
+        <v>0</v>
+      </c>
+      <c r="J8" s="29">
+        <v>0</v>
+      </c>
+      <c r="K8" s="12">
+        <v>0</v>
+      </c>
+      <c r="L8" s="12">
+        <v>0</v>
+      </c>
+      <c r="M8" s="12">
+        <v>0</v>
+      </c>
+      <c r="N8" s="12">
+        <v>0</v>
+      </c>
+      <c r="O8" s="12">
+        <v>0</v>
+      </c>
+      <c r="P8" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="12">
+        <v>0</v>
+      </c>
+      <c r="R8" s="12">
+        <v>0</v>
+      </c>
+      <c r="S8" s="12">
+        <v>0</v>
+      </c>
+      <c r="T8" s="12">
+        <v>0</v>
+      </c>
+      <c r="U8" s="12">
+        <v>0</v>
+      </c>
+      <c r="V8" s="16">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B9" s="30"/>
+      <c r="B9" s="24"/>
       <c r="C9" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="19">
-        <v>0</v>
-      </c>
-      <c r="E9" s="3">
-        <v>0</v>
-      </c>
-      <c r="F9" s="3">
-        <v>0</v>
-      </c>
-      <c r="G9" s="11">
+      <c r="D9" s="14">
+        <v>0</v>
+      </c>
+      <c r="E9" s="30">
+        <v>0</v>
+      </c>
+      <c r="F9" s="30">
+        <v>0</v>
+      </c>
+      <c r="G9" s="25">
         <v>2</v>
       </c>
-      <c r="H9" s="3">
-        <v>0</v>
-      </c>
-      <c r="I9" s="3">
-        <v>0</v>
-      </c>
-      <c r="J9" s="3">
+      <c r="H9" s="30">
+        <v>0</v>
+      </c>
+      <c r="I9" s="30">
+        <v>0</v>
+      </c>
+      <c r="J9" s="30">
         <v>0</v>
       </c>
       <c r="K9" s="3">
@@ -2647,34 +2692,34 @@
       <c r="U9" s="3">
         <v>0</v>
       </c>
-      <c r="V9" s="22">
+      <c r="V9" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B10" s="30"/>
+      <c r="B10" s="24"/>
       <c r="C10" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="19">
-        <v>0</v>
-      </c>
-      <c r="E10" s="3">
-        <v>0</v>
-      </c>
-      <c r="F10" s="3">
-        <v>0</v>
-      </c>
-      <c r="G10" s="3">
-        <v>0</v>
-      </c>
-      <c r="H10" s="11">
+      <c r="D10" s="14">
+        <v>0</v>
+      </c>
+      <c r="E10" s="30">
+        <v>0</v>
+      </c>
+      <c r="F10" s="30">
+        <v>0</v>
+      </c>
+      <c r="G10" s="30">
+        <v>0</v>
+      </c>
+      <c r="H10" s="25">
         <v>1</v>
       </c>
-      <c r="I10" s="3">
-        <v>0</v>
-      </c>
-      <c r="J10" s="3">
+      <c r="I10" s="30">
+        <v>0</v>
+      </c>
+      <c r="J10" s="30">
         <v>0</v>
       </c>
       <c r="K10" s="3">
@@ -2710,34 +2755,34 @@
       <c r="U10" s="3">
         <v>0</v>
       </c>
-      <c r="V10" s="22">
+      <c r="V10" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B11" s="30"/>
+      <c r="B11" s="24"/>
       <c r="C11" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="19">
-        <v>0</v>
-      </c>
-      <c r="E11" s="3">
-        <v>0</v>
-      </c>
-      <c r="F11" s="3">
-        <v>0</v>
-      </c>
-      <c r="G11" s="3">
-        <v>0</v>
-      </c>
-      <c r="H11" s="3">
-        <v>0</v>
-      </c>
-      <c r="I11" s="11">
+      <c r="D11" s="14">
+        <v>0</v>
+      </c>
+      <c r="E11" s="30">
+        <v>0</v>
+      </c>
+      <c r="F11" s="30">
+        <v>0</v>
+      </c>
+      <c r="G11" s="30">
+        <v>0</v>
+      </c>
+      <c r="H11" s="30">
+        <v>0</v>
+      </c>
+      <c r="I11" s="25">
         <v>2</v>
       </c>
-      <c r="J11" s="3">
+      <c r="J11" s="30">
         <v>0</v>
       </c>
       <c r="K11" s="3">
@@ -2773,34 +2818,34 @@
       <c r="U11" s="3">
         <v>0</v>
       </c>
-      <c r="V11" s="22">
+      <c r="V11" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B12" s="31"/>
+      <c r="B12" s="22"/>
       <c r="C12" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="20">
-        <v>0</v>
-      </c>
-      <c r="E12" s="4">
-        <v>0</v>
-      </c>
-      <c r="F12" s="4">
-        <v>0</v>
-      </c>
-      <c r="G12" s="4">
-        <v>0</v>
-      </c>
-      <c r="H12" s="4">
-        <v>0</v>
-      </c>
-      <c r="I12" s="4">
-        <v>0</v>
-      </c>
-      <c r="J12" s="12">
+      <c r="D12" s="15">
+        <v>0</v>
+      </c>
+      <c r="E12" s="31">
+        <v>0</v>
+      </c>
+      <c r="F12" s="31">
+        <v>0</v>
+      </c>
+      <c r="G12" s="31">
+        <v>0</v>
+      </c>
+      <c r="H12" s="31">
+        <v>0</v>
+      </c>
+      <c r="I12" s="31">
+        <v>0</v>
+      </c>
+      <c r="J12" s="26">
         <v>2</v>
       </c>
       <c r="K12" s="4">
@@ -2836,81 +2881,81 @@
       <c r="U12" s="4">
         <v>0</v>
       </c>
-      <c r="V12" s="23">
+      <c r="V12" s="18">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B13" s="29" t="s">
+      <c r="B13" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="18">
-        <v>0</v>
-      </c>
-      <c r="E13" s="14">
-        <v>0</v>
-      </c>
-      <c r="F13" s="14">
-        <v>0</v>
-      </c>
-      <c r="G13" s="14">
-        <v>0</v>
-      </c>
-      <c r="H13" s="14">
-        <v>0</v>
-      </c>
-      <c r="I13" s="14">
-        <v>0</v>
-      </c>
-      <c r="J13" s="14">
-        <v>0</v>
-      </c>
-      <c r="K13" s="15">
+      <c r="D13" s="13">
+        <v>0</v>
+      </c>
+      <c r="E13" s="12">
+        <v>0</v>
+      </c>
+      <c r="F13" s="12">
+        <v>0</v>
+      </c>
+      <c r="G13" s="12">
+        <v>0</v>
+      </c>
+      <c r="H13" s="12">
+        <v>0</v>
+      </c>
+      <c r="I13" s="12">
+        <v>0</v>
+      </c>
+      <c r="J13" s="12">
+        <v>0</v>
+      </c>
+      <c r="K13" s="29">
         <v>2</v>
       </c>
-      <c r="L13" s="15">
+      <c r="L13" s="29">
         <v>1</v>
       </c>
-      <c r="M13" s="14">
-        <v>0</v>
-      </c>
-      <c r="N13" s="14">
-        <v>0</v>
-      </c>
-      <c r="O13" s="14">
-        <v>0</v>
-      </c>
-      <c r="P13" s="14">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="14">
-        <v>0</v>
-      </c>
-      <c r="R13" s="14">
-        <v>0</v>
-      </c>
-      <c r="S13" s="14">
-        <v>0</v>
-      </c>
-      <c r="T13" s="14">
-        <v>0</v>
-      </c>
-      <c r="U13" s="14">
-        <v>0</v>
-      </c>
-      <c r="V13" s="21">
+      <c r="M13" s="29">
+        <v>0</v>
+      </c>
+      <c r="N13" s="29">
+        <v>0</v>
+      </c>
+      <c r="O13" s="29">
+        <v>0</v>
+      </c>
+      <c r="P13" s="29">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="29">
+        <v>0</v>
+      </c>
+      <c r="R13" s="29">
+        <v>0</v>
+      </c>
+      <c r="S13" s="12">
+        <v>0</v>
+      </c>
+      <c r="T13" s="12">
+        <v>0</v>
+      </c>
+      <c r="U13" s="12">
+        <v>0</v>
+      </c>
+      <c r="V13" s="16">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B14" s="30"/>
+      <c r="B14" s="24"/>
       <c r="C14" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="19">
+      <c r="D14" s="14">
         <v>0</v>
       </c>
       <c r="E14" s="3">
@@ -2931,28 +2976,28 @@
       <c r="J14" s="3">
         <v>0</v>
       </c>
-      <c r="K14" s="3">
-        <v>0</v>
-      </c>
-      <c r="L14" s="3">
-        <v>0</v>
-      </c>
-      <c r="M14" s="11">
+      <c r="K14" s="30">
+        <v>0</v>
+      </c>
+      <c r="L14" s="30">
+        <v>0</v>
+      </c>
+      <c r="M14" s="30">
         <v>1</v>
       </c>
-      <c r="N14" s="3">
-        <v>0</v>
-      </c>
-      <c r="O14" s="3">
-        <v>0</v>
-      </c>
-      <c r="P14" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="3">
-        <v>0</v>
-      </c>
-      <c r="R14" s="3">
+      <c r="N14" s="30">
+        <v>0</v>
+      </c>
+      <c r="O14" s="30">
+        <v>0</v>
+      </c>
+      <c r="P14" s="30">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="30">
+        <v>0</v>
+      </c>
+      <c r="R14" s="30">
         <v>0</v>
       </c>
       <c r="S14" s="3">
@@ -2964,16 +3009,16 @@
       <c r="U14" s="3">
         <v>0</v>
       </c>
-      <c r="V14" s="22">
+      <c r="V14" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B15" s="30"/>
+      <c r="B15" s="24"/>
       <c r="C15" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="19">
+      <c r="D15" s="14">
         <v>0</v>
       </c>
       <c r="E15" s="3">
@@ -2994,28 +3039,28 @@
       <c r="J15" s="3">
         <v>0</v>
       </c>
-      <c r="K15" s="3">
-        <v>0</v>
-      </c>
-      <c r="L15" s="3">
-        <v>0</v>
-      </c>
-      <c r="M15" s="3">
-        <v>0</v>
-      </c>
-      <c r="N15" s="11">
+      <c r="K15" s="30">
+        <v>0</v>
+      </c>
+      <c r="L15" s="30">
+        <v>0</v>
+      </c>
+      <c r="M15" s="30">
+        <v>0</v>
+      </c>
+      <c r="N15" s="30">
         <v>2</v>
       </c>
-      <c r="O15" s="11">
+      <c r="O15" s="30">
         <v>1</v>
       </c>
-      <c r="P15" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="3">
-        <v>0</v>
-      </c>
-      <c r="R15" s="3">
+      <c r="P15" s="30">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="30">
+        <v>0</v>
+      </c>
+      <c r="R15" s="30">
         <v>0</v>
       </c>
       <c r="S15" s="3">
@@ -3027,16 +3072,16 @@
       <c r="U15" s="3">
         <v>0</v>
       </c>
-      <c r="V15" s="22">
+      <c r="V15" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B16" s="31"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="20">
+      <c r="D16" s="15">
         <v>0</v>
       </c>
       <c r="E16" s="4">
@@ -3057,28 +3102,28 @@
       <c r="J16" s="4">
         <v>0</v>
       </c>
-      <c r="K16" s="4">
-        <v>0</v>
-      </c>
-      <c r="L16" s="4">
-        <v>0</v>
-      </c>
-      <c r="M16" s="4">
-        <v>0</v>
-      </c>
-      <c r="N16" s="4">
-        <v>0</v>
-      </c>
-      <c r="O16" s="4">
-        <v>0</v>
-      </c>
-      <c r="P16" s="12">
+      <c r="K16" s="31">
+        <v>0</v>
+      </c>
+      <c r="L16" s="31">
+        <v>0</v>
+      </c>
+      <c r="M16" s="31">
+        <v>0</v>
+      </c>
+      <c r="N16" s="31">
+        <v>0</v>
+      </c>
+      <c r="O16" s="31">
+        <v>0</v>
+      </c>
+      <c r="P16" s="31">
         <v>1</v>
       </c>
-      <c r="Q16" s="12">
+      <c r="Q16" s="31">
         <v>1</v>
       </c>
-      <c r="R16" s="12">
+      <c r="R16" s="31">
         <v>1</v>
       </c>
       <c r="S16" s="4">
@@ -3090,81 +3135,81 @@
       <c r="U16" s="4">
         <v>0</v>
       </c>
-      <c r="V16" s="23">
+      <c r="V16" s="18">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B17" s="29" t="s">
+      <c r="B17" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D17" s="18">
-        <v>0</v>
-      </c>
-      <c r="E17" s="14">
-        <v>0</v>
-      </c>
-      <c r="F17" s="14">
-        <v>0</v>
-      </c>
-      <c r="G17" s="14">
-        <v>0</v>
-      </c>
-      <c r="H17" s="14">
-        <v>0</v>
-      </c>
-      <c r="I17" s="14">
-        <v>0</v>
-      </c>
-      <c r="J17" s="14">
-        <v>0</v>
-      </c>
-      <c r="K17" s="14">
-        <v>0</v>
-      </c>
-      <c r="L17" s="14">
-        <v>0</v>
-      </c>
-      <c r="M17" s="14">
-        <v>0</v>
-      </c>
-      <c r="N17" s="14">
-        <v>0</v>
-      </c>
-      <c r="O17" s="14">
-        <v>0</v>
-      </c>
-      <c r="P17" s="14">
-        <v>0</v>
-      </c>
-      <c r="Q17" s="14">
-        <v>0</v>
-      </c>
-      <c r="R17" s="14">
-        <v>0</v>
-      </c>
-      <c r="S17" s="15">
+      <c r="D17" s="13">
+        <v>0</v>
+      </c>
+      <c r="E17" s="12">
+        <v>0</v>
+      </c>
+      <c r="F17" s="12">
+        <v>0</v>
+      </c>
+      <c r="G17" s="12">
+        <v>0</v>
+      </c>
+      <c r="H17" s="12">
+        <v>0</v>
+      </c>
+      <c r="I17" s="12">
+        <v>0</v>
+      </c>
+      <c r="J17" s="12">
+        <v>0</v>
+      </c>
+      <c r="K17" s="12">
+        <v>0</v>
+      </c>
+      <c r="L17" s="12">
+        <v>0</v>
+      </c>
+      <c r="M17" s="12">
+        <v>0</v>
+      </c>
+      <c r="N17" s="12">
+        <v>0</v>
+      </c>
+      <c r="O17" s="12">
+        <v>0</v>
+      </c>
+      <c r="P17" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="12">
+        <v>0</v>
+      </c>
+      <c r="R17" s="12">
+        <v>0</v>
+      </c>
+      <c r="S17" s="28">
         <v>0.5</v>
       </c>
-      <c r="T17" s="14">
-        <v>0</v>
-      </c>
-      <c r="U17" s="14">
-        <v>0</v>
-      </c>
-      <c r="V17" s="21">
+      <c r="T17" s="29">
+        <v>0</v>
+      </c>
+      <c r="U17" s="29">
+        <v>0</v>
+      </c>
+      <c r="V17" s="32">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B18" s="30"/>
+      <c r="B18" s="24"/>
       <c r="C18" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D18" s="19">
+      <c r="D18" s="14">
         <v>0</v>
       </c>
       <c r="E18" s="3">
@@ -3209,25 +3254,25 @@
       <c r="R18" s="3">
         <v>0</v>
       </c>
-      <c r="S18" s="11">
+      <c r="S18" s="30">
         <v>0.5</v>
       </c>
-      <c r="T18" s="3">
-        <v>0</v>
-      </c>
-      <c r="U18" s="3">
-        <v>0</v>
-      </c>
-      <c r="V18" s="22">
+      <c r="T18" s="30">
+        <v>0</v>
+      </c>
+      <c r="U18" s="30">
+        <v>0</v>
+      </c>
+      <c r="V18" s="33">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B19" s="31"/>
+      <c r="B19" s="22"/>
       <c r="C19" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="20">
+      <c r="D19" s="15">
         <v>0</v>
       </c>
       <c r="E19" s="4">
@@ -3272,90 +3317,90 @@
       <c r="R19" s="4">
         <v>0</v>
       </c>
-      <c r="S19" s="4">
-        <v>0</v>
-      </c>
-      <c r="T19" s="12">
+      <c r="S19" s="31">
+        <v>0</v>
+      </c>
+      <c r="T19" s="31">
         <v>1</v>
       </c>
-      <c r="U19" s="4">
-        <v>0</v>
-      </c>
-      <c r="V19" s="23">
+      <c r="U19" s="31">
+        <v>0</v>
+      </c>
+      <c r="V19" s="34">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B20" s="29" t="s">
+      <c r="B20" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="D20" s="18">
-        <v>0</v>
-      </c>
-      <c r="E20" s="14">
-        <v>0</v>
-      </c>
-      <c r="F20" s="14">
-        <v>0</v>
-      </c>
-      <c r="G20" s="14">
-        <v>0</v>
-      </c>
-      <c r="H20" s="14">
-        <v>0</v>
-      </c>
-      <c r="I20" s="14">
-        <v>0</v>
-      </c>
-      <c r="J20" s="14">
-        <v>0</v>
-      </c>
-      <c r="K20" s="14">
-        <v>0</v>
-      </c>
-      <c r="L20" s="14">
-        <v>0</v>
-      </c>
-      <c r="M20" s="14">
-        <v>0</v>
-      </c>
-      <c r="N20" s="14">
-        <v>0</v>
-      </c>
-      <c r="O20" s="14">
-        <v>0</v>
-      </c>
-      <c r="P20" s="14">
-        <v>0</v>
-      </c>
-      <c r="Q20" s="14">
-        <v>0</v>
-      </c>
-      <c r="R20" s="14">
-        <v>0</v>
-      </c>
-      <c r="S20" s="14">
-        <v>0</v>
-      </c>
-      <c r="T20" s="14">
-        <v>0</v>
-      </c>
-      <c r="U20" s="15">
+      <c r="D20" s="13">
+        <v>0</v>
+      </c>
+      <c r="E20" s="12">
+        <v>0</v>
+      </c>
+      <c r="F20" s="12">
+        <v>0</v>
+      </c>
+      <c r="G20" s="12">
+        <v>0</v>
+      </c>
+      <c r="H20" s="12">
+        <v>0</v>
+      </c>
+      <c r="I20" s="12">
+        <v>0</v>
+      </c>
+      <c r="J20" s="12">
+        <v>0</v>
+      </c>
+      <c r="K20" s="12">
+        <v>0</v>
+      </c>
+      <c r="L20" s="12">
+        <v>0</v>
+      </c>
+      <c r="M20" s="12">
+        <v>0</v>
+      </c>
+      <c r="N20" s="12">
+        <v>0</v>
+      </c>
+      <c r="O20" s="12">
+        <v>0</v>
+      </c>
+      <c r="P20" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="12">
+        <v>0</v>
+      </c>
+      <c r="R20" s="12">
+        <v>0</v>
+      </c>
+      <c r="S20" s="29">
+        <v>0</v>
+      </c>
+      <c r="T20" s="29">
+        <v>0</v>
+      </c>
+      <c r="U20" s="28">
         <v>0.5</v>
       </c>
-      <c r="V20" s="21">
+      <c r="V20" s="32">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B21" s="31"/>
+      <c r="B21" s="22"/>
       <c r="C21" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D21" s="20">
+      <c r="D21" s="15">
         <v>0</v>
       </c>
       <c r="E21" s="4">
@@ -3400,90 +3445,90 @@
       <c r="R21" s="4">
         <v>0</v>
       </c>
-      <c r="S21" s="4">
-        <v>0</v>
-      </c>
-      <c r="T21" s="4">
-        <v>0</v>
-      </c>
-      <c r="U21" s="12">
+      <c r="S21" s="31">
+        <v>0</v>
+      </c>
+      <c r="T21" s="31">
+        <v>0</v>
+      </c>
+      <c r="U21" s="31">
         <v>0.5</v>
       </c>
-      <c r="V21" s="23">
+      <c r="V21" s="34">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B22" s="29" t="s">
+      <c r="B22" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="14" t="s">
+      <c r="C22" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="D22" s="18">
-        <v>0</v>
-      </c>
-      <c r="E22" s="14">
-        <v>0</v>
-      </c>
-      <c r="F22" s="14">
-        <v>0</v>
-      </c>
-      <c r="G22" s="14">
-        <v>0</v>
-      </c>
-      <c r="H22" s="14">
-        <v>0</v>
-      </c>
-      <c r="I22" s="14">
-        <v>0</v>
-      </c>
-      <c r="J22" s="14">
-        <v>0</v>
-      </c>
-      <c r="K22" s="14">
-        <v>0</v>
-      </c>
-      <c r="L22" s="14">
-        <v>0</v>
-      </c>
-      <c r="M22" s="14">
-        <v>0</v>
-      </c>
-      <c r="N22" s="14">
-        <v>0</v>
-      </c>
-      <c r="O22" s="14">
-        <v>0</v>
-      </c>
-      <c r="P22" s="14">
-        <v>0</v>
-      </c>
-      <c r="Q22" s="14">
-        <v>0</v>
-      </c>
-      <c r="R22" s="14">
-        <v>0</v>
-      </c>
-      <c r="S22" s="14">
-        <v>0</v>
-      </c>
-      <c r="T22" s="14">
-        <v>0</v>
-      </c>
-      <c r="U22" s="16">
-        <v>0</v>
-      </c>
-      <c r="V22" s="24">
+      <c r="D22" s="13">
+        <v>0</v>
+      </c>
+      <c r="E22" s="12">
+        <v>0</v>
+      </c>
+      <c r="F22" s="12">
+        <v>0</v>
+      </c>
+      <c r="G22" s="12">
+        <v>0</v>
+      </c>
+      <c r="H22" s="12">
+        <v>0</v>
+      </c>
+      <c r="I22" s="12">
+        <v>0</v>
+      </c>
+      <c r="J22" s="12">
+        <v>0</v>
+      </c>
+      <c r="K22" s="12">
+        <v>0</v>
+      </c>
+      <c r="L22" s="12">
+        <v>0</v>
+      </c>
+      <c r="M22" s="12">
+        <v>0</v>
+      </c>
+      <c r="N22" s="12">
+        <v>0</v>
+      </c>
+      <c r="O22" s="12">
+        <v>0</v>
+      </c>
+      <c r="P22" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="12">
+        <v>0</v>
+      </c>
+      <c r="R22" s="12">
+        <v>0</v>
+      </c>
+      <c r="S22" s="29">
+        <v>0</v>
+      </c>
+      <c r="T22" s="29">
+        <v>0</v>
+      </c>
+      <c r="U22" s="29">
+        <v>0</v>
+      </c>
+      <c r="V22" s="32">
         <v>0.5</v>
       </c>
     </row>
     <row r="23" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B23" s="31"/>
+      <c r="B23" s="22"/>
       <c r="C23" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D23" s="20">
+      <c r="D23" s="15">
         <v>0</v>
       </c>
       <c r="E23" s="4">
@@ -3528,92 +3573,92 @@
       <c r="R23" s="4">
         <v>0</v>
       </c>
-      <c r="S23" s="4">
-        <v>0</v>
-      </c>
-      <c r="T23" s="4">
-        <v>0</v>
-      </c>
-      <c r="U23" s="17">
-        <v>0</v>
-      </c>
-      <c r="V23" s="25">
+      <c r="S23" s="31">
+        <v>0</v>
+      </c>
+      <c r="T23" s="31">
+        <v>0</v>
+      </c>
+      <c r="U23" s="31">
+        <v>0</v>
+      </c>
+      <c r="V23" s="34">
         <v>0.5</v>
       </c>
     </row>
     <row r="24" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="D24" s="18">
+      <c r="D24" s="13">
         <v>23</v>
       </c>
-      <c r="E24" s="18">
+      <c r="E24" s="13">
         <f>D24-SUM(E4:E23)</f>
         <v>22</v>
       </c>
-      <c r="F24" s="18">
+      <c r="F24" s="13">
         <f>E24-SUM(F4:F23)</f>
         <v>21</v>
       </c>
-      <c r="G24" s="18">
+      <c r="G24" s="13">
         <f>F24-SUM(G4:G23)</f>
         <v>19</v>
       </c>
-      <c r="H24" s="18">
+      <c r="H24" s="13">
         <f t="shared" ref="H24:V24" si="0">G24-SUM(H4:H23)</f>
         <v>18</v>
       </c>
-      <c r="I24" s="18">
+      <c r="I24" s="13">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="J24" s="18">
+      <c r="J24" s="13">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="K24" s="18">
+      <c r="K24" s="13">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="L24" s="18">
+      <c r="L24" s="13">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="M24" s="18">
+      <c r="M24" s="13">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="N24" s="18">
+      <c r="N24" s="13">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="O24" s="18">
+      <c r="O24" s="13">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="P24" s="18">
+      <c r="P24" s="13">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="Q24" s="18">
+      <c r="Q24" s="13">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="R24" s="18">
+      <c r="R24" s="13">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="S24" s="18">
+      <c r="S24" s="13">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="T24" s="18">
+      <c r="T24" s="13">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="U24" s="18">
+      <c r="U24" s="13">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="V24" s="26">
+      <c r="V24" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Sprint 1 - W2
</commit_message>
<xml_diff>
--- a/Group C2-3 Scrum documentation.xlsx
+++ b/Group C2-3 Scrum documentation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johna\OneDrive\Documents\University\Year II\CO553 Agile Development and Software Security B\co553-c2-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6C9013A-E3BB-4C35-A462-45775F5A6ECD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60A1F294-FD20-47D3-81EA-6401AD42E9CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{0CC9FE5D-919A-41CA-B32D-5FFC3808111C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0CC9FE5D-919A-41CA-B32D-5FFC3808111C}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -447,19 +447,13 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -479,6 +473,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="8" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -491,16 +495,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="8" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1983,8 +1986,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F2ABAF1-62E6-41B4-BC47-CFBA7BD3B611}">
   <dimension ref="B2:D21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1993,211 +1996,211 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="8" t="s">
+      <c r="B2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="6" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="5">
+      <c r="B3" s="33">
         <v>1</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="33">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="6">
+      <c r="B4" s="34">
         <v>2</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="34">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="6">
+      <c r="B5" s="34">
         <v>3</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="34">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="6">
+      <c r="B6" s="34">
         <v>4</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="34">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="6">
+      <c r="B7" s="34">
         <v>5</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="34">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="6">
+      <c r="B8" s="34">
         <v>6</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="34">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="6">
+      <c r="B9" s="4">
         <v>7</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="4">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="6">
+      <c r="B10" s="4">
         <v>8</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="4">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="6">
+      <c r="B11" s="4">
         <v>9</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="4">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="6">
+      <c r="B12" s="4">
         <v>10</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="4">
         <v>3</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="6">
+      <c r="B13" s="4">
         <v>11</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="6">
+      <c r="B14" s="4">
         <v>12</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="6">
+      <c r="B15" s="4">
         <v>13</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D15" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="6">
+      <c r="B16" s="4">
         <v>14</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D16" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="6">
+      <c r="B17" s="4">
         <v>15</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D17" s="4">
         <v>3</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="6">
+      <c r="B18" s="4">
         <v>16</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D18" s="4">
         <v>5</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="6">
+      <c r="B19" s="4">
         <v>17</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="6">
+      <c r="D19" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="6">
+      <c r="B20" s="4">
         <v>18</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D20" s="6">
+      <c r="D20" s="4">
         <v>1</v>
       </c>
     </row>
@@ -2214,8 +2217,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1498325-30FB-42AD-97E8-3EAEC03F161C}">
   <dimension ref="B2:V24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2225,1440 +2228,1440 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
-      <c r="O2" s="23"/>
-      <c r="P2" s="23"/>
-      <c r="Q2" s="23"/>
-      <c r="R2" s="23"/>
-      <c r="S2" s="23"/>
-      <c r="T2" s="23"/>
-      <c r="U2" s="23"/>
-      <c r="V2" s="23"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="31"/>
+      <c r="P2" s="31"/>
+      <c r="Q2" s="31"/>
+      <c r="R2" s="31"/>
+      <c r="S2" s="31"/>
+      <c r="T2" s="31"/>
+      <c r="U2" s="31"/>
+      <c r="V2" s="31"/>
     </row>
     <row r="3" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="9">
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="7">
         <v>44221</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="7">
         <v>44222</v>
       </c>
-      <c r="F3" s="9">
+      <c r="F3" s="7">
         <v>44223</v>
       </c>
-      <c r="G3" s="9">
+      <c r="G3" s="7">
         <v>44224</v>
       </c>
-      <c r="H3" s="9">
+      <c r="H3" s="7">
         <v>44225</v>
       </c>
-      <c r="I3" s="9">
+      <c r="I3" s="7">
         <v>44226</v>
       </c>
-      <c r="J3" s="9">
+      <c r="J3" s="7">
         <v>44227</v>
       </c>
-      <c r="K3" s="9">
+      <c r="K3" s="7">
         <v>44228</v>
       </c>
-      <c r="L3" s="9">
+      <c r="L3" s="7">
         <v>44229</v>
       </c>
-      <c r="M3" s="9">
+      <c r="M3" s="7">
         <v>44230</v>
       </c>
-      <c r="N3" s="9">
+      <c r="N3" s="7">
         <v>44231</v>
       </c>
-      <c r="O3" s="9">
+      <c r="O3" s="7">
         <v>44232</v>
       </c>
-      <c r="P3" s="9">
+      <c r="P3" s="7">
         <v>44233</v>
       </c>
-      <c r="Q3" s="9">
+      <c r="Q3" s="7">
         <v>44234</v>
       </c>
-      <c r="R3" s="9">
+      <c r="R3" s="7">
         <v>44235</v>
       </c>
-      <c r="S3" s="9">
+      <c r="S3" s="7">
         <v>44236</v>
       </c>
-      <c r="T3" s="9">
+      <c r="T3" s="7">
         <v>44237</v>
       </c>
-      <c r="U3" s="9">
+      <c r="U3" s="7">
         <v>44238</v>
       </c>
-      <c r="V3" s="9">
+      <c r="V3" s="7">
         <v>44239</v>
       </c>
     </row>
     <row r="4" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="13">
-        <v>0</v>
-      </c>
-      <c r="E4" s="27">
+      <c r="D4" s="11">
+        <v>0</v>
+      </c>
+      <c r="E4" s="21">
         <v>0.25</v>
       </c>
-      <c r="F4" s="30">
-        <v>0</v>
-      </c>
-      <c r="G4" s="30">
-        <v>0</v>
-      </c>
-      <c r="H4" s="30">
-        <v>0</v>
-      </c>
-      <c r="I4" s="30">
-        <v>0</v>
-      </c>
-      <c r="J4" s="30">
-        <v>0</v>
-      </c>
-      <c r="K4" s="3">
-        <v>0</v>
-      </c>
-      <c r="L4" s="3">
-        <v>0</v>
-      </c>
-      <c r="M4" s="3">
-        <v>0</v>
-      </c>
-      <c r="N4" s="3">
-        <v>0</v>
-      </c>
-      <c r="O4" s="3">
-        <v>0</v>
-      </c>
-      <c r="P4" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="3">
-        <v>0</v>
-      </c>
-      <c r="R4" s="3">
-        <v>0</v>
-      </c>
-      <c r="S4" s="3">
-        <v>0</v>
-      </c>
-      <c r="T4" s="3">
-        <v>0</v>
-      </c>
-      <c r="U4" s="3">
-        <v>0</v>
-      </c>
-      <c r="V4" s="16">
+      <c r="F4" s="24">
+        <v>0</v>
+      </c>
+      <c r="G4" s="24">
+        <v>0</v>
+      </c>
+      <c r="H4" s="24">
+        <v>0</v>
+      </c>
+      <c r="I4" s="24">
+        <v>0</v>
+      </c>
+      <c r="J4" s="24">
+        <v>0</v>
+      </c>
+      <c r="K4" s="2">
+        <v>0</v>
+      </c>
+      <c r="L4" s="2">
+        <v>0</v>
+      </c>
+      <c r="M4" s="2">
+        <v>0</v>
+      </c>
+      <c r="N4" s="2">
+        <v>0</v>
+      </c>
+      <c r="O4" s="2">
+        <v>0</v>
+      </c>
+      <c r="P4" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>0</v>
+      </c>
+      <c r="R4" s="2">
+        <v>0</v>
+      </c>
+      <c r="S4" s="2">
+        <v>0</v>
+      </c>
+      <c r="T4" s="2">
+        <v>0</v>
+      </c>
+      <c r="U4" s="2">
+        <v>0</v>
+      </c>
+      <c r="V4" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B5" s="24"/>
-      <c r="C5" s="10" t="s">
+      <c r="B5" s="32"/>
+      <c r="C5" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D5" s="14">
-        <v>0</v>
-      </c>
-      <c r="E5" s="27">
+      <c r="D5" s="12">
+        <v>0</v>
+      </c>
+      <c r="E5" s="21">
         <v>0.25</v>
       </c>
-      <c r="F5" s="30">
-        <v>0</v>
-      </c>
-      <c r="G5" s="30">
-        <v>0</v>
-      </c>
-      <c r="H5" s="30">
-        <v>0</v>
-      </c>
-      <c r="I5" s="30">
-        <v>0</v>
-      </c>
-      <c r="J5" s="30">
-        <v>0</v>
-      </c>
-      <c r="K5" s="3">
-        <v>0</v>
-      </c>
-      <c r="L5" s="3">
-        <v>0</v>
-      </c>
-      <c r="M5" s="3">
-        <v>0</v>
-      </c>
-      <c r="N5" s="3">
-        <v>0</v>
-      </c>
-      <c r="O5" s="3">
-        <v>0</v>
-      </c>
-      <c r="P5" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="3">
-        <v>0</v>
-      </c>
-      <c r="R5" s="3">
-        <v>0</v>
-      </c>
-      <c r="S5" s="3">
-        <v>0</v>
-      </c>
-      <c r="T5" s="3">
-        <v>0</v>
-      </c>
-      <c r="U5" s="3">
-        <v>0</v>
-      </c>
-      <c r="V5" s="17">
+      <c r="F5" s="24">
+        <v>0</v>
+      </c>
+      <c r="G5" s="24">
+        <v>0</v>
+      </c>
+      <c r="H5" s="24">
+        <v>0</v>
+      </c>
+      <c r="I5" s="24">
+        <v>0</v>
+      </c>
+      <c r="J5" s="24">
+        <v>0</v>
+      </c>
+      <c r="K5" s="2">
+        <v>0</v>
+      </c>
+      <c r="L5" s="2">
+        <v>0</v>
+      </c>
+      <c r="M5" s="2">
+        <v>0</v>
+      </c>
+      <c r="N5" s="2">
+        <v>0</v>
+      </c>
+      <c r="O5" s="2">
+        <v>0</v>
+      </c>
+      <c r="P5" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>0</v>
+      </c>
+      <c r="R5" s="2">
+        <v>0</v>
+      </c>
+      <c r="S5" s="2">
+        <v>0</v>
+      </c>
+      <c r="T5" s="2">
+        <v>0</v>
+      </c>
+      <c r="U5" s="2">
+        <v>0</v>
+      </c>
+      <c r="V5" s="15">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B6" s="24"/>
-      <c r="C6" s="3" t="s">
+      <c r="B6" s="32"/>
+      <c r="C6" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D6" s="14">
-        <v>0</v>
-      </c>
-      <c r="E6" s="25">
+      <c r="D6" s="12">
+        <v>0</v>
+      </c>
+      <c r="E6" s="19">
         <v>0.25</v>
       </c>
-      <c r="F6" s="30">
-        <v>0</v>
-      </c>
-      <c r="G6" s="30">
-        <v>0</v>
-      </c>
-      <c r="H6" s="30">
-        <v>0</v>
-      </c>
-      <c r="I6" s="30">
-        <v>0</v>
-      </c>
-      <c r="J6" s="30">
-        <v>0</v>
-      </c>
-      <c r="K6" s="3">
-        <v>0</v>
-      </c>
-      <c r="L6" s="3">
-        <v>0</v>
-      </c>
-      <c r="M6" s="3">
-        <v>0</v>
-      </c>
-      <c r="N6" s="3">
-        <v>0</v>
-      </c>
-      <c r="O6" s="3">
-        <v>0</v>
-      </c>
-      <c r="P6" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="3">
-        <v>0</v>
-      </c>
-      <c r="R6" s="3">
-        <v>0</v>
-      </c>
-      <c r="S6" s="3">
-        <v>0</v>
-      </c>
-      <c r="T6" s="3">
-        <v>0</v>
-      </c>
-      <c r="U6" s="3">
-        <v>0</v>
-      </c>
-      <c r="V6" s="17">
+      <c r="F6" s="24">
+        <v>0</v>
+      </c>
+      <c r="G6" s="24">
+        <v>0</v>
+      </c>
+      <c r="H6" s="24">
+        <v>0</v>
+      </c>
+      <c r="I6" s="24">
+        <v>0</v>
+      </c>
+      <c r="J6" s="24">
+        <v>0</v>
+      </c>
+      <c r="K6" s="2">
+        <v>0</v>
+      </c>
+      <c r="L6" s="2">
+        <v>0</v>
+      </c>
+      <c r="M6" s="2">
+        <v>0</v>
+      </c>
+      <c r="N6" s="2">
+        <v>0</v>
+      </c>
+      <c r="O6" s="2">
+        <v>0</v>
+      </c>
+      <c r="P6" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>0</v>
+      </c>
+      <c r="R6" s="2">
+        <v>0</v>
+      </c>
+      <c r="S6" s="2">
+        <v>0</v>
+      </c>
+      <c r="T6" s="2">
+        <v>0</v>
+      </c>
+      <c r="U6" s="2">
+        <v>0</v>
+      </c>
+      <c r="V6" s="15">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B7" s="22"/>
-      <c r="C7" s="4" t="s">
+      <c r="B7" s="30"/>
+      <c r="C7" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="15">
-        <v>0</v>
-      </c>
-      <c r="E7" s="26">
+      <c r="D7" s="13">
+        <v>0</v>
+      </c>
+      <c r="E7" s="20">
         <v>0.25</v>
       </c>
-      <c r="F7" s="31">
-        <v>0</v>
-      </c>
-      <c r="G7" s="31">
-        <v>0</v>
-      </c>
-      <c r="H7" s="31">
-        <v>0</v>
-      </c>
-      <c r="I7" s="31">
-        <v>0</v>
-      </c>
-      <c r="J7" s="31">
-        <v>0</v>
-      </c>
-      <c r="K7" s="4">
-        <v>0</v>
-      </c>
-      <c r="L7" s="4">
-        <v>0</v>
-      </c>
-      <c r="M7" s="4">
-        <v>0</v>
-      </c>
-      <c r="N7" s="4">
-        <v>0</v>
-      </c>
-      <c r="O7" s="4">
-        <v>0</v>
-      </c>
-      <c r="P7" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="4">
-        <v>0</v>
-      </c>
-      <c r="R7" s="4">
-        <v>0</v>
-      </c>
-      <c r="S7" s="4">
-        <v>0</v>
-      </c>
-      <c r="T7" s="4">
-        <v>0</v>
-      </c>
-      <c r="U7" s="4">
-        <v>0</v>
-      </c>
-      <c r="V7" s="18">
+      <c r="F7" s="25">
+        <v>0</v>
+      </c>
+      <c r="G7" s="25">
+        <v>0</v>
+      </c>
+      <c r="H7" s="25">
+        <v>0</v>
+      </c>
+      <c r="I7" s="25">
+        <v>0</v>
+      </c>
+      <c r="J7" s="25">
+        <v>0</v>
+      </c>
+      <c r="K7" s="3">
+        <v>0</v>
+      </c>
+      <c r="L7" s="3">
+        <v>0</v>
+      </c>
+      <c r="M7" s="3">
+        <v>0</v>
+      </c>
+      <c r="N7" s="3">
+        <v>0</v>
+      </c>
+      <c r="O7" s="3">
+        <v>0</v>
+      </c>
+      <c r="P7" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>0</v>
+      </c>
+      <c r="R7" s="3">
+        <v>0</v>
+      </c>
+      <c r="S7" s="3">
+        <v>0</v>
+      </c>
+      <c r="T7" s="3">
+        <v>0</v>
+      </c>
+      <c r="U7" s="3">
+        <v>0</v>
+      </c>
+      <c r="V7" s="16">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="13">
-        <v>0</v>
-      </c>
-      <c r="E8" s="29">
-        <v>0</v>
-      </c>
-      <c r="F8" s="28">
+      <c r="D8" s="11">
+        <v>0</v>
+      </c>
+      <c r="E8" s="23">
+        <v>0</v>
+      </c>
+      <c r="F8" s="22">
         <v>1</v>
       </c>
-      <c r="G8" s="29">
-        <v>0</v>
-      </c>
-      <c r="H8" s="29">
-        <v>0</v>
-      </c>
-      <c r="I8" s="29">
-        <v>0</v>
-      </c>
-      <c r="J8" s="29">
-        <v>0</v>
-      </c>
-      <c r="K8" s="12">
-        <v>0</v>
-      </c>
-      <c r="L8" s="12">
-        <v>0</v>
-      </c>
-      <c r="M8" s="12">
-        <v>0</v>
-      </c>
-      <c r="N8" s="12">
-        <v>0</v>
-      </c>
-      <c r="O8" s="12">
-        <v>0</v>
-      </c>
-      <c r="P8" s="12">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="12">
-        <v>0</v>
-      </c>
-      <c r="R8" s="12">
-        <v>0</v>
-      </c>
-      <c r="S8" s="12">
-        <v>0</v>
-      </c>
-      <c r="T8" s="12">
-        <v>0</v>
-      </c>
-      <c r="U8" s="12">
-        <v>0</v>
-      </c>
-      <c r="V8" s="16">
+      <c r="G8" s="23">
+        <v>0</v>
+      </c>
+      <c r="H8" s="23">
+        <v>0</v>
+      </c>
+      <c r="I8" s="23">
+        <v>0</v>
+      </c>
+      <c r="J8" s="23">
+        <v>0</v>
+      </c>
+      <c r="K8" s="10">
+        <v>0</v>
+      </c>
+      <c r="L8" s="10">
+        <v>0</v>
+      </c>
+      <c r="M8" s="10">
+        <v>0</v>
+      </c>
+      <c r="N8" s="10">
+        <v>0</v>
+      </c>
+      <c r="O8" s="10">
+        <v>0</v>
+      </c>
+      <c r="P8" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="10">
+        <v>0</v>
+      </c>
+      <c r="R8" s="10">
+        <v>0</v>
+      </c>
+      <c r="S8" s="10">
+        <v>0</v>
+      </c>
+      <c r="T8" s="10">
+        <v>0</v>
+      </c>
+      <c r="U8" s="10">
+        <v>0</v>
+      </c>
+      <c r="V8" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B9" s="24"/>
-      <c r="C9" s="3" t="s">
+      <c r="B9" s="32"/>
+      <c r="C9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="14">
-        <v>0</v>
-      </c>
-      <c r="E9" s="30">
-        <v>0</v>
-      </c>
-      <c r="F9" s="30">
-        <v>0</v>
-      </c>
-      <c r="G9" s="25">
+      <c r="D9" s="12">
+        <v>0</v>
+      </c>
+      <c r="E9" s="24">
+        <v>0</v>
+      </c>
+      <c r="F9" s="24">
+        <v>0</v>
+      </c>
+      <c r="G9" s="19">
         <v>2</v>
       </c>
-      <c r="H9" s="30">
-        <v>0</v>
-      </c>
-      <c r="I9" s="30">
-        <v>0</v>
-      </c>
-      <c r="J9" s="30">
-        <v>0</v>
-      </c>
-      <c r="K9" s="3">
-        <v>0</v>
-      </c>
-      <c r="L9" s="3">
-        <v>0</v>
-      </c>
-      <c r="M9" s="3">
-        <v>0</v>
-      </c>
-      <c r="N9" s="3">
-        <v>0</v>
-      </c>
-      <c r="O9" s="3">
-        <v>0</v>
-      </c>
-      <c r="P9" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="3">
-        <v>0</v>
-      </c>
-      <c r="R9" s="3">
-        <v>0</v>
-      </c>
-      <c r="S9" s="3">
-        <v>0</v>
-      </c>
-      <c r="T9" s="3">
-        <v>0</v>
-      </c>
-      <c r="U9" s="3">
-        <v>0</v>
-      </c>
-      <c r="V9" s="17">
+      <c r="H9" s="24">
+        <v>0</v>
+      </c>
+      <c r="I9" s="24">
+        <v>0</v>
+      </c>
+      <c r="J9" s="24">
+        <v>0</v>
+      </c>
+      <c r="K9" s="2">
+        <v>0</v>
+      </c>
+      <c r="L9" s="2">
+        <v>0</v>
+      </c>
+      <c r="M9" s="2">
+        <v>0</v>
+      </c>
+      <c r="N9" s="2">
+        <v>0</v>
+      </c>
+      <c r="O9" s="2">
+        <v>0</v>
+      </c>
+      <c r="P9" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="2">
+        <v>0</v>
+      </c>
+      <c r="R9" s="2">
+        <v>0</v>
+      </c>
+      <c r="S9" s="2">
+        <v>0</v>
+      </c>
+      <c r="T9" s="2">
+        <v>0</v>
+      </c>
+      <c r="U9" s="2">
+        <v>0</v>
+      </c>
+      <c r="V9" s="15">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B10" s="24"/>
-      <c r="C10" s="3" t="s">
+      <c r="B10" s="32"/>
+      <c r="C10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="14">
-        <v>0</v>
-      </c>
-      <c r="E10" s="30">
-        <v>0</v>
-      </c>
-      <c r="F10" s="30">
-        <v>0</v>
-      </c>
-      <c r="G10" s="30">
-        <v>0</v>
-      </c>
-      <c r="H10" s="25">
+      <c r="D10" s="12">
+        <v>0</v>
+      </c>
+      <c r="E10" s="24">
+        <v>0</v>
+      </c>
+      <c r="F10" s="24">
+        <v>0</v>
+      </c>
+      <c r="G10" s="24">
+        <v>0</v>
+      </c>
+      <c r="H10" s="19">
         <v>1</v>
       </c>
-      <c r="I10" s="30">
-        <v>0</v>
-      </c>
-      <c r="J10" s="30">
-        <v>0</v>
-      </c>
-      <c r="K10" s="3">
-        <v>0</v>
-      </c>
-      <c r="L10" s="3">
-        <v>0</v>
-      </c>
-      <c r="M10" s="3">
-        <v>0</v>
-      </c>
-      <c r="N10" s="3">
-        <v>0</v>
-      </c>
-      <c r="O10" s="3">
-        <v>0</v>
-      </c>
-      <c r="P10" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="3">
-        <v>0</v>
-      </c>
-      <c r="R10" s="3">
-        <v>0</v>
-      </c>
-      <c r="S10" s="3">
-        <v>0</v>
-      </c>
-      <c r="T10" s="3">
-        <v>0</v>
-      </c>
-      <c r="U10" s="3">
-        <v>0</v>
-      </c>
-      <c r="V10" s="17">
+      <c r="I10" s="24">
+        <v>0</v>
+      </c>
+      <c r="J10" s="24">
+        <v>0</v>
+      </c>
+      <c r="K10" s="2">
+        <v>0</v>
+      </c>
+      <c r="L10" s="2">
+        <v>0</v>
+      </c>
+      <c r="M10" s="2">
+        <v>0</v>
+      </c>
+      <c r="N10" s="2">
+        <v>0</v>
+      </c>
+      <c r="O10" s="2">
+        <v>0</v>
+      </c>
+      <c r="P10" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="2">
+        <v>0</v>
+      </c>
+      <c r="R10" s="2">
+        <v>0</v>
+      </c>
+      <c r="S10" s="2">
+        <v>0</v>
+      </c>
+      <c r="T10" s="2">
+        <v>0</v>
+      </c>
+      <c r="U10" s="2">
+        <v>0</v>
+      </c>
+      <c r="V10" s="15">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B11" s="24"/>
-      <c r="C11" s="3" t="s">
+      <c r="B11" s="32"/>
+      <c r="C11" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="14">
-        <v>0</v>
-      </c>
-      <c r="E11" s="30">
-        <v>0</v>
-      </c>
-      <c r="F11" s="30">
-        <v>0</v>
-      </c>
-      <c r="G11" s="30">
-        <v>0</v>
-      </c>
-      <c r="H11" s="30">
-        <v>0</v>
-      </c>
-      <c r="I11" s="25">
+      <c r="D11" s="12">
+        <v>0</v>
+      </c>
+      <c r="E11" s="24">
+        <v>0</v>
+      </c>
+      <c r="F11" s="24">
+        <v>0</v>
+      </c>
+      <c r="G11" s="24">
+        <v>0</v>
+      </c>
+      <c r="H11" s="24">
+        <v>0</v>
+      </c>
+      <c r="I11" s="19">
         <v>2</v>
       </c>
-      <c r="J11" s="30">
-        <v>0</v>
-      </c>
-      <c r="K11" s="3">
-        <v>0</v>
-      </c>
-      <c r="L11" s="3">
-        <v>0</v>
-      </c>
-      <c r="M11" s="3">
-        <v>0</v>
-      </c>
-      <c r="N11" s="3">
-        <v>0</v>
-      </c>
-      <c r="O11" s="3">
-        <v>0</v>
-      </c>
-      <c r="P11" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="3">
-        <v>0</v>
-      </c>
-      <c r="R11" s="3">
-        <v>0</v>
-      </c>
-      <c r="S11" s="3">
-        <v>0</v>
-      </c>
-      <c r="T11" s="3">
-        <v>0</v>
-      </c>
-      <c r="U11" s="3">
-        <v>0</v>
-      </c>
-      <c r="V11" s="17">
+      <c r="J11" s="24">
+        <v>0</v>
+      </c>
+      <c r="K11" s="2">
+        <v>0</v>
+      </c>
+      <c r="L11" s="2">
+        <v>0</v>
+      </c>
+      <c r="M11" s="2">
+        <v>0</v>
+      </c>
+      <c r="N11" s="2">
+        <v>0</v>
+      </c>
+      <c r="O11" s="2">
+        <v>0</v>
+      </c>
+      <c r="P11" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>0</v>
+      </c>
+      <c r="R11" s="2">
+        <v>0</v>
+      </c>
+      <c r="S11" s="2">
+        <v>0</v>
+      </c>
+      <c r="T11" s="2">
+        <v>0</v>
+      </c>
+      <c r="U11" s="2">
+        <v>0</v>
+      </c>
+      <c r="V11" s="15">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B12" s="22"/>
-      <c r="C12" s="4" t="s">
+      <c r="B12" s="30"/>
+      <c r="C12" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="15">
-        <v>0</v>
-      </c>
-      <c r="E12" s="31">
-        <v>0</v>
-      </c>
-      <c r="F12" s="31">
-        <v>0</v>
-      </c>
-      <c r="G12" s="31">
-        <v>0</v>
-      </c>
-      <c r="H12" s="31">
-        <v>0</v>
-      </c>
-      <c r="I12" s="31">
-        <v>0</v>
-      </c>
-      <c r="J12" s="26">
+      <c r="D12" s="13">
+        <v>0</v>
+      </c>
+      <c r="E12" s="25">
+        <v>0</v>
+      </c>
+      <c r="F12" s="25">
+        <v>0</v>
+      </c>
+      <c r="G12" s="25">
+        <v>0</v>
+      </c>
+      <c r="H12" s="25">
+        <v>0</v>
+      </c>
+      <c r="I12" s="25">
+        <v>0</v>
+      </c>
+      <c r="J12" s="20">
         <v>2</v>
       </c>
-      <c r="K12" s="4">
-        <v>0</v>
-      </c>
-      <c r="L12" s="4">
-        <v>0</v>
-      </c>
-      <c r="M12" s="4">
-        <v>0</v>
-      </c>
-      <c r="N12" s="4">
-        <v>0</v>
-      </c>
-      <c r="O12" s="4">
-        <v>0</v>
-      </c>
-      <c r="P12" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="4">
-        <v>0</v>
-      </c>
-      <c r="R12" s="4">
-        <v>0</v>
-      </c>
-      <c r="S12" s="4">
-        <v>0</v>
-      </c>
-      <c r="T12" s="4">
-        <v>0</v>
-      </c>
-      <c r="U12" s="4">
-        <v>0</v>
-      </c>
-      <c r="V12" s="18">
+      <c r="K12" s="3">
+        <v>0</v>
+      </c>
+      <c r="L12" s="3">
+        <v>0</v>
+      </c>
+      <c r="M12" s="3">
+        <v>0</v>
+      </c>
+      <c r="N12" s="3">
+        <v>0</v>
+      </c>
+      <c r="O12" s="3">
+        <v>0</v>
+      </c>
+      <c r="P12" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="3">
+        <v>0</v>
+      </c>
+      <c r="R12" s="3">
+        <v>0</v>
+      </c>
+      <c r="S12" s="3">
+        <v>0</v>
+      </c>
+      <c r="T12" s="3">
+        <v>0</v>
+      </c>
+      <c r="U12" s="3">
+        <v>0</v>
+      </c>
+      <c r="V12" s="16">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="13">
-        <v>0</v>
-      </c>
-      <c r="E13" s="12">
-        <v>0</v>
-      </c>
-      <c r="F13" s="12">
-        <v>0</v>
-      </c>
-      <c r="G13" s="12">
-        <v>0</v>
-      </c>
-      <c r="H13" s="12">
-        <v>0</v>
-      </c>
-      <c r="I13" s="12">
-        <v>0</v>
-      </c>
-      <c r="J13" s="12">
-        <v>0</v>
-      </c>
-      <c r="K13" s="29">
+      <c r="D13" s="11">
+        <v>0</v>
+      </c>
+      <c r="E13" s="10">
+        <v>0</v>
+      </c>
+      <c r="F13" s="10">
+        <v>0</v>
+      </c>
+      <c r="G13" s="10">
+        <v>0</v>
+      </c>
+      <c r="H13" s="10">
+        <v>0</v>
+      </c>
+      <c r="I13" s="10">
+        <v>0</v>
+      </c>
+      <c r="J13" s="10">
+        <v>0</v>
+      </c>
+      <c r="K13" s="23">
         <v>2</v>
       </c>
-      <c r="L13" s="29">
+      <c r="L13" s="23">
         <v>1</v>
       </c>
-      <c r="M13" s="29">
-        <v>0</v>
-      </c>
-      <c r="N13" s="29">
-        <v>0</v>
-      </c>
-      <c r="O13" s="29">
-        <v>0</v>
-      </c>
-      <c r="P13" s="29">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="29">
-        <v>0</v>
-      </c>
-      <c r="R13" s="29">
-        <v>0</v>
-      </c>
-      <c r="S13" s="12">
-        <v>0</v>
-      </c>
-      <c r="T13" s="12">
-        <v>0</v>
-      </c>
-      <c r="U13" s="12">
-        <v>0</v>
-      </c>
-      <c r="V13" s="16">
+      <c r="M13" s="23">
+        <v>0</v>
+      </c>
+      <c r="N13" s="23">
+        <v>0</v>
+      </c>
+      <c r="O13" s="23">
+        <v>0</v>
+      </c>
+      <c r="P13" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="23">
+        <v>0</v>
+      </c>
+      <c r="R13" s="23">
+        <v>0</v>
+      </c>
+      <c r="S13" s="10">
+        <v>0</v>
+      </c>
+      <c r="T13" s="10">
+        <v>0</v>
+      </c>
+      <c r="U13" s="10">
+        <v>0</v>
+      </c>
+      <c r="V13" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B14" s="24"/>
-      <c r="C14" s="3" t="s">
+      <c r="B14" s="32"/>
+      <c r="C14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="14">
-        <v>0</v>
-      </c>
-      <c r="E14" s="3">
-        <v>0</v>
-      </c>
-      <c r="F14" s="3">
-        <v>0</v>
-      </c>
-      <c r="G14" s="3">
-        <v>0</v>
-      </c>
-      <c r="H14" s="3">
-        <v>0</v>
-      </c>
-      <c r="I14" s="3">
-        <v>0</v>
-      </c>
-      <c r="J14" s="3">
-        <v>0</v>
-      </c>
-      <c r="K14" s="30">
-        <v>0</v>
-      </c>
-      <c r="L14" s="30">
-        <v>0</v>
-      </c>
-      <c r="M14" s="30">
+      <c r="D14" s="12">
+        <v>0</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0</v>
+      </c>
+      <c r="F14" s="2">
+        <v>0</v>
+      </c>
+      <c r="G14" s="2">
+        <v>0</v>
+      </c>
+      <c r="H14" s="2">
+        <v>0</v>
+      </c>
+      <c r="I14" s="2">
+        <v>0</v>
+      </c>
+      <c r="J14" s="2">
+        <v>0</v>
+      </c>
+      <c r="K14" s="24">
+        <v>0</v>
+      </c>
+      <c r="L14" s="24">
+        <v>0</v>
+      </c>
+      <c r="M14" s="24">
         <v>1</v>
       </c>
-      <c r="N14" s="30">
-        <v>0</v>
-      </c>
-      <c r="O14" s="30">
-        <v>0</v>
-      </c>
-      <c r="P14" s="30">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="30">
-        <v>0</v>
-      </c>
-      <c r="R14" s="30">
-        <v>0</v>
-      </c>
-      <c r="S14" s="3">
-        <v>0</v>
-      </c>
-      <c r="T14" s="3">
-        <v>0</v>
-      </c>
-      <c r="U14" s="3">
-        <v>0</v>
-      </c>
-      <c r="V14" s="17">
+      <c r="N14" s="24">
+        <v>0</v>
+      </c>
+      <c r="O14" s="24">
+        <v>0</v>
+      </c>
+      <c r="P14" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="24">
+        <v>0</v>
+      </c>
+      <c r="R14" s="24">
+        <v>0</v>
+      </c>
+      <c r="S14" s="2">
+        <v>0</v>
+      </c>
+      <c r="T14" s="2">
+        <v>0</v>
+      </c>
+      <c r="U14" s="2">
+        <v>0</v>
+      </c>
+      <c r="V14" s="15">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B15" s="24"/>
-      <c r="C15" s="3" t="s">
+      <c r="B15" s="32"/>
+      <c r="C15" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="14">
-        <v>0</v>
-      </c>
-      <c r="E15" s="3">
-        <v>0</v>
-      </c>
-      <c r="F15" s="3">
-        <v>0</v>
-      </c>
-      <c r="G15" s="3">
-        <v>0</v>
-      </c>
-      <c r="H15" s="3">
-        <v>0</v>
-      </c>
-      <c r="I15" s="3">
-        <v>0</v>
-      </c>
-      <c r="J15" s="3">
-        <v>0</v>
-      </c>
-      <c r="K15" s="30">
-        <v>0</v>
-      </c>
-      <c r="L15" s="30">
-        <v>0</v>
-      </c>
-      <c r="M15" s="30">
-        <v>0</v>
-      </c>
-      <c r="N15" s="30">
+      <c r="D15" s="12">
+        <v>0</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0</v>
+      </c>
+      <c r="F15" s="2">
+        <v>0</v>
+      </c>
+      <c r="G15" s="2">
+        <v>0</v>
+      </c>
+      <c r="H15" s="2">
+        <v>0</v>
+      </c>
+      <c r="I15" s="2">
+        <v>0</v>
+      </c>
+      <c r="J15" s="2">
+        <v>0</v>
+      </c>
+      <c r="K15" s="24">
+        <v>0</v>
+      </c>
+      <c r="L15" s="24">
+        <v>0</v>
+      </c>
+      <c r="M15" s="24">
+        <v>0</v>
+      </c>
+      <c r="N15" s="24">
         <v>2</v>
       </c>
-      <c r="O15" s="30">
+      <c r="O15" s="24">
         <v>1</v>
       </c>
-      <c r="P15" s="30">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="30">
-        <v>0</v>
-      </c>
-      <c r="R15" s="30">
-        <v>0</v>
-      </c>
-      <c r="S15" s="3">
-        <v>0</v>
-      </c>
-      <c r="T15" s="3">
-        <v>0</v>
-      </c>
-      <c r="U15" s="3">
-        <v>0</v>
-      </c>
-      <c r="V15" s="17">
+      <c r="P15" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="24">
+        <v>0</v>
+      </c>
+      <c r="R15" s="24">
+        <v>0</v>
+      </c>
+      <c r="S15" s="2">
+        <v>0</v>
+      </c>
+      <c r="T15" s="2">
+        <v>0</v>
+      </c>
+      <c r="U15" s="2">
+        <v>0</v>
+      </c>
+      <c r="V15" s="15">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B16" s="22"/>
-      <c r="C16" s="4" t="s">
+      <c r="B16" s="30"/>
+      <c r="C16" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="15">
-        <v>0</v>
-      </c>
-      <c r="E16" s="4">
-        <v>0</v>
-      </c>
-      <c r="F16" s="4">
-        <v>0</v>
-      </c>
-      <c r="G16" s="4">
-        <v>0</v>
-      </c>
-      <c r="H16" s="4">
-        <v>0</v>
-      </c>
-      <c r="I16" s="4">
-        <v>0</v>
-      </c>
-      <c r="J16" s="4">
-        <v>0</v>
-      </c>
-      <c r="K16" s="31">
-        <v>0</v>
-      </c>
-      <c r="L16" s="31">
-        <v>0</v>
-      </c>
-      <c r="M16" s="31">
-        <v>0</v>
-      </c>
-      <c r="N16" s="31">
-        <v>0</v>
-      </c>
-      <c r="O16" s="31">
-        <v>0</v>
-      </c>
-      <c r="P16" s="31">
+      <c r="D16" s="13">
+        <v>0</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0</v>
+      </c>
+      <c r="F16" s="3">
+        <v>0</v>
+      </c>
+      <c r="G16" s="3">
+        <v>0</v>
+      </c>
+      <c r="H16" s="3">
+        <v>0</v>
+      </c>
+      <c r="I16" s="3">
+        <v>0</v>
+      </c>
+      <c r="J16" s="3">
+        <v>0</v>
+      </c>
+      <c r="K16" s="25">
+        <v>0</v>
+      </c>
+      <c r="L16" s="25">
+        <v>0</v>
+      </c>
+      <c r="M16" s="25">
+        <v>0</v>
+      </c>
+      <c r="N16" s="25">
+        <v>0</v>
+      </c>
+      <c r="O16" s="25">
+        <v>0</v>
+      </c>
+      <c r="P16" s="25">
         <v>1</v>
       </c>
-      <c r="Q16" s="31">
+      <c r="Q16" s="25">
         <v>1</v>
       </c>
-      <c r="R16" s="31">
+      <c r="R16" s="25">
         <v>1</v>
       </c>
-      <c r="S16" s="4">
-        <v>0</v>
-      </c>
-      <c r="T16" s="4">
-        <v>0</v>
-      </c>
-      <c r="U16" s="4">
-        <v>0</v>
-      </c>
-      <c r="V16" s="18">
+      <c r="S16" s="3">
+        <v>0</v>
+      </c>
+      <c r="T16" s="3">
+        <v>0</v>
+      </c>
+      <c r="U16" s="3">
+        <v>0</v>
+      </c>
+      <c r="V16" s="16">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B17" s="21" t="s">
+      <c r="B17" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D17" s="13">
-        <v>0</v>
-      </c>
-      <c r="E17" s="12">
-        <v>0</v>
-      </c>
-      <c r="F17" s="12">
-        <v>0</v>
-      </c>
-      <c r="G17" s="12">
-        <v>0</v>
-      </c>
-      <c r="H17" s="12">
-        <v>0</v>
-      </c>
-      <c r="I17" s="12">
-        <v>0</v>
-      </c>
-      <c r="J17" s="12">
-        <v>0</v>
-      </c>
-      <c r="K17" s="12">
-        <v>0</v>
-      </c>
-      <c r="L17" s="12">
-        <v>0</v>
-      </c>
-      <c r="M17" s="12">
-        <v>0</v>
-      </c>
-      <c r="N17" s="12">
-        <v>0</v>
-      </c>
-      <c r="O17" s="12">
-        <v>0</v>
-      </c>
-      <c r="P17" s="12">
-        <v>0</v>
-      </c>
-      <c r="Q17" s="12">
-        <v>0</v>
-      </c>
-      <c r="R17" s="12">
-        <v>0</v>
-      </c>
-      <c r="S17" s="28">
+      <c r="D17" s="11">
+        <v>0</v>
+      </c>
+      <c r="E17" s="10">
+        <v>0</v>
+      </c>
+      <c r="F17" s="10">
+        <v>0</v>
+      </c>
+      <c r="G17" s="10">
+        <v>0</v>
+      </c>
+      <c r="H17" s="10">
+        <v>0</v>
+      </c>
+      <c r="I17" s="10">
+        <v>0</v>
+      </c>
+      <c r="J17" s="10">
+        <v>0</v>
+      </c>
+      <c r="K17" s="10">
+        <v>0</v>
+      </c>
+      <c r="L17" s="10">
+        <v>0</v>
+      </c>
+      <c r="M17" s="10">
+        <v>0</v>
+      </c>
+      <c r="N17" s="10">
+        <v>0</v>
+      </c>
+      <c r="O17" s="10">
+        <v>0</v>
+      </c>
+      <c r="P17" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="10">
+        <v>0</v>
+      </c>
+      <c r="R17" s="10">
+        <v>0</v>
+      </c>
+      <c r="S17" s="22">
         <v>0.5</v>
       </c>
-      <c r="T17" s="29">
-        <v>0</v>
-      </c>
-      <c r="U17" s="29">
-        <v>0</v>
-      </c>
-      <c r="V17" s="32">
+      <c r="T17" s="23">
+        <v>0</v>
+      </c>
+      <c r="U17" s="23">
+        <v>0</v>
+      </c>
+      <c r="V17" s="26">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B18" s="24"/>
-      <c r="C18" s="3" t="s">
+      <c r="B18" s="32"/>
+      <c r="C18" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D18" s="14">
-        <v>0</v>
-      </c>
-      <c r="E18" s="3">
-        <v>0</v>
-      </c>
-      <c r="F18" s="3">
-        <v>0</v>
-      </c>
-      <c r="G18" s="3">
-        <v>0</v>
-      </c>
-      <c r="H18" s="3">
-        <v>0</v>
-      </c>
-      <c r="I18" s="3">
-        <v>0</v>
-      </c>
-      <c r="J18" s="3">
-        <v>0</v>
-      </c>
-      <c r="K18" s="3">
-        <v>0</v>
-      </c>
-      <c r="L18" s="3">
-        <v>0</v>
-      </c>
-      <c r="M18" s="3">
-        <v>0</v>
-      </c>
-      <c r="N18" s="3">
-        <v>0</v>
-      </c>
-      <c r="O18" s="3">
-        <v>0</v>
-      </c>
-      <c r="P18" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q18" s="3">
-        <v>0</v>
-      </c>
-      <c r="R18" s="3">
-        <v>0</v>
-      </c>
-      <c r="S18" s="30">
+      <c r="D18" s="12">
+        <v>0</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0</v>
+      </c>
+      <c r="F18" s="2">
+        <v>0</v>
+      </c>
+      <c r="G18" s="2">
+        <v>0</v>
+      </c>
+      <c r="H18" s="2">
+        <v>0</v>
+      </c>
+      <c r="I18" s="2">
+        <v>0</v>
+      </c>
+      <c r="J18" s="2">
+        <v>0</v>
+      </c>
+      <c r="K18" s="2">
+        <v>0</v>
+      </c>
+      <c r="L18" s="2">
+        <v>0</v>
+      </c>
+      <c r="M18" s="2">
+        <v>0</v>
+      </c>
+      <c r="N18" s="2">
+        <v>0</v>
+      </c>
+      <c r="O18" s="2">
+        <v>0</v>
+      </c>
+      <c r="P18" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="2">
+        <v>0</v>
+      </c>
+      <c r="R18" s="2">
+        <v>0</v>
+      </c>
+      <c r="S18" s="24">
         <v>0.5</v>
       </c>
-      <c r="T18" s="30">
-        <v>0</v>
-      </c>
-      <c r="U18" s="30">
-        <v>0</v>
-      </c>
-      <c r="V18" s="33">
+      <c r="T18" s="24">
+        <v>0</v>
+      </c>
+      <c r="U18" s="24">
+        <v>0</v>
+      </c>
+      <c r="V18" s="27">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B19" s="22"/>
-      <c r="C19" s="4" t="s">
+      <c r="B19" s="30"/>
+      <c r="C19" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="15">
-        <v>0</v>
-      </c>
-      <c r="E19" s="4">
-        <v>0</v>
-      </c>
-      <c r="F19" s="4">
-        <v>0</v>
-      </c>
-      <c r="G19" s="4">
-        <v>0</v>
-      </c>
-      <c r="H19" s="4">
-        <v>0</v>
-      </c>
-      <c r="I19" s="4">
-        <v>0</v>
-      </c>
-      <c r="J19" s="4">
-        <v>0</v>
-      </c>
-      <c r="K19" s="4">
-        <v>0</v>
-      </c>
-      <c r="L19" s="4">
-        <v>0</v>
-      </c>
-      <c r="M19" s="4">
-        <v>0</v>
-      </c>
-      <c r="N19" s="4">
-        <v>0</v>
-      </c>
-      <c r="O19" s="4">
-        <v>0</v>
-      </c>
-      <c r="P19" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q19" s="4">
-        <v>0</v>
-      </c>
-      <c r="R19" s="4">
-        <v>0</v>
-      </c>
-      <c r="S19" s="31">
-        <v>0</v>
-      </c>
-      <c r="T19" s="31">
+      <c r="D19" s="13">
+        <v>0</v>
+      </c>
+      <c r="E19" s="3">
+        <v>0</v>
+      </c>
+      <c r="F19" s="3">
+        <v>0</v>
+      </c>
+      <c r="G19" s="3">
+        <v>0</v>
+      </c>
+      <c r="H19" s="3">
+        <v>0</v>
+      </c>
+      <c r="I19" s="3">
+        <v>0</v>
+      </c>
+      <c r="J19" s="3">
+        <v>0</v>
+      </c>
+      <c r="K19" s="3">
+        <v>0</v>
+      </c>
+      <c r="L19" s="3">
+        <v>0</v>
+      </c>
+      <c r="M19" s="3">
+        <v>0</v>
+      </c>
+      <c r="N19" s="3">
+        <v>0</v>
+      </c>
+      <c r="O19" s="3">
+        <v>0</v>
+      </c>
+      <c r="P19" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="3">
+        <v>0</v>
+      </c>
+      <c r="R19" s="3">
+        <v>0</v>
+      </c>
+      <c r="S19" s="25">
+        <v>0</v>
+      </c>
+      <c r="T19" s="25">
         <v>1</v>
       </c>
-      <c r="U19" s="31">
-        <v>0</v>
-      </c>
-      <c r="V19" s="34">
+      <c r="U19" s="25">
+        <v>0</v>
+      </c>
+      <c r="V19" s="28">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B20" s="21" t="s">
+      <c r="B20" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="D20" s="13">
-        <v>0</v>
-      </c>
-      <c r="E20" s="12">
-        <v>0</v>
-      </c>
-      <c r="F20" s="12">
-        <v>0</v>
-      </c>
-      <c r="G20" s="12">
-        <v>0</v>
-      </c>
-      <c r="H20" s="12">
-        <v>0</v>
-      </c>
-      <c r="I20" s="12">
-        <v>0</v>
-      </c>
-      <c r="J20" s="12">
-        <v>0</v>
-      </c>
-      <c r="K20" s="12">
-        <v>0</v>
-      </c>
-      <c r="L20" s="12">
-        <v>0</v>
-      </c>
-      <c r="M20" s="12">
-        <v>0</v>
-      </c>
-      <c r="N20" s="12">
-        <v>0</v>
-      </c>
-      <c r="O20" s="12">
-        <v>0</v>
-      </c>
-      <c r="P20" s="12">
-        <v>0</v>
-      </c>
-      <c r="Q20" s="12">
-        <v>0</v>
-      </c>
-      <c r="R20" s="12">
-        <v>0</v>
-      </c>
-      <c r="S20" s="29">
-        <v>0</v>
-      </c>
-      <c r="T20" s="29">
-        <v>0</v>
-      </c>
-      <c r="U20" s="28">
+      <c r="D20" s="11">
+        <v>0</v>
+      </c>
+      <c r="E20" s="10">
+        <v>0</v>
+      </c>
+      <c r="F20" s="10">
+        <v>0</v>
+      </c>
+      <c r="G20" s="10">
+        <v>0</v>
+      </c>
+      <c r="H20" s="10">
+        <v>0</v>
+      </c>
+      <c r="I20" s="10">
+        <v>0</v>
+      </c>
+      <c r="J20" s="10">
+        <v>0</v>
+      </c>
+      <c r="K20" s="10">
+        <v>0</v>
+      </c>
+      <c r="L20" s="10">
+        <v>0</v>
+      </c>
+      <c r="M20" s="10">
+        <v>0</v>
+      </c>
+      <c r="N20" s="10">
+        <v>0</v>
+      </c>
+      <c r="O20" s="10">
+        <v>0</v>
+      </c>
+      <c r="P20" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="10">
+        <v>0</v>
+      </c>
+      <c r="R20" s="10">
+        <v>0</v>
+      </c>
+      <c r="S20" s="23">
+        <v>0</v>
+      </c>
+      <c r="T20" s="23">
+        <v>0</v>
+      </c>
+      <c r="U20" s="22">
         <v>0.5</v>
       </c>
-      <c r="V20" s="32">
+      <c r="V20" s="26">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B21" s="22"/>
-      <c r="C21" s="4" t="s">
+      <c r="B21" s="30"/>
+      <c r="C21" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D21" s="15">
-        <v>0</v>
-      </c>
-      <c r="E21" s="4">
-        <v>0</v>
-      </c>
-      <c r="F21" s="4">
-        <v>0</v>
-      </c>
-      <c r="G21" s="4">
-        <v>0</v>
-      </c>
-      <c r="H21" s="4">
-        <v>0</v>
-      </c>
-      <c r="I21" s="4">
-        <v>0</v>
-      </c>
-      <c r="J21" s="4">
-        <v>0</v>
-      </c>
-      <c r="K21" s="4">
-        <v>0</v>
-      </c>
-      <c r="L21" s="4">
-        <v>0</v>
-      </c>
-      <c r="M21" s="4">
-        <v>0</v>
-      </c>
-      <c r="N21" s="4">
-        <v>0</v>
-      </c>
-      <c r="O21" s="4">
-        <v>0</v>
-      </c>
-      <c r="P21" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q21" s="4">
-        <v>0</v>
-      </c>
-      <c r="R21" s="4">
-        <v>0</v>
-      </c>
-      <c r="S21" s="31">
-        <v>0</v>
-      </c>
-      <c r="T21" s="31">
-        <v>0</v>
-      </c>
-      <c r="U21" s="31">
+      <c r="D21" s="13">
+        <v>0</v>
+      </c>
+      <c r="E21" s="3">
+        <v>0</v>
+      </c>
+      <c r="F21" s="3">
+        <v>0</v>
+      </c>
+      <c r="G21" s="3">
+        <v>0</v>
+      </c>
+      <c r="H21" s="3">
+        <v>0</v>
+      </c>
+      <c r="I21" s="3">
+        <v>0</v>
+      </c>
+      <c r="J21" s="3">
+        <v>0</v>
+      </c>
+      <c r="K21" s="3">
+        <v>0</v>
+      </c>
+      <c r="L21" s="3">
+        <v>0</v>
+      </c>
+      <c r="M21" s="3">
+        <v>0</v>
+      </c>
+      <c r="N21" s="3">
+        <v>0</v>
+      </c>
+      <c r="O21" s="3">
+        <v>0</v>
+      </c>
+      <c r="P21" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="3">
+        <v>0</v>
+      </c>
+      <c r="R21" s="3">
+        <v>0</v>
+      </c>
+      <c r="S21" s="25">
+        <v>0</v>
+      </c>
+      <c r="T21" s="25">
+        <v>0</v>
+      </c>
+      <c r="U21" s="25">
         <v>0.5</v>
       </c>
-      <c r="V21" s="34">
+      <c r="V21" s="28">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B22" s="21" t="s">
+      <c r="B22" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C22" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="D22" s="13">
-        <v>0</v>
-      </c>
-      <c r="E22" s="12">
-        <v>0</v>
-      </c>
-      <c r="F22" s="12">
-        <v>0</v>
-      </c>
-      <c r="G22" s="12">
-        <v>0</v>
-      </c>
-      <c r="H22" s="12">
-        <v>0</v>
-      </c>
-      <c r="I22" s="12">
-        <v>0</v>
-      </c>
-      <c r="J22" s="12">
-        <v>0</v>
-      </c>
-      <c r="K22" s="12">
-        <v>0</v>
-      </c>
-      <c r="L22" s="12">
-        <v>0</v>
-      </c>
-      <c r="M22" s="12">
-        <v>0</v>
-      </c>
-      <c r="N22" s="12">
-        <v>0</v>
-      </c>
-      <c r="O22" s="12">
-        <v>0</v>
-      </c>
-      <c r="P22" s="12">
-        <v>0</v>
-      </c>
-      <c r="Q22" s="12">
-        <v>0</v>
-      </c>
-      <c r="R22" s="12">
-        <v>0</v>
-      </c>
-      <c r="S22" s="29">
-        <v>0</v>
-      </c>
-      <c r="T22" s="29">
-        <v>0</v>
-      </c>
-      <c r="U22" s="29">
-        <v>0</v>
-      </c>
-      <c r="V22" s="32">
+      <c r="D22" s="11">
+        <v>0</v>
+      </c>
+      <c r="E22" s="10">
+        <v>0</v>
+      </c>
+      <c r="F22" s="10">
+        <v>0</v>
+      </c>
+      <c r="G22" s="10">
+        <v>0</v>
+      </c>
+      <c r="H22" s="10">
+        <v>0</v>
+      </c>
+      <c r="I22" s="10">
+        <v>0</v>
+      </c>
+      <c r="J22" s="10">
+        <v>0</v>
+      </c>
+      <c r="K22" s="10">
+        <v>0</v>
+      </c>
+      <c r="L22" s="10">
+        <v>0</v>
+      </c>
+      <c r="M22" s="10">
+        <v>0</v>
+      </c>
+      <c r="N22" s="10">
+        <v>0</v>
+      </c>
+      <c r="O22" s="10">
+        <v>0</v>
+      </c>
+      <c r="P22" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="10">
+        <v>0</v>
+      </c>
+      <c r="R22" s="10">
+        <v>0</v>
+      </c>
+      <c r="S22" s="23">
+        <v>0</v>
+      </c>
+      <c r="T22" s="23">
+        <v>0</v>
+      </c>
+      <c r="U22" s="23">
+        <v>0</v>
+      </c>
+      <c r="V22" s="26">
         <v>0.5</v>
       </c>
     </row>
     <row r="23" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B23" s="22"/>
-      <c r="C23" s="4" t="s">
+      <c r="B23" s="30"/>
+      <c r="C23" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D23" s="15">
-        <v>0</v>
-      </c>
-      <c r="E23" s="4">
-        <v>0</v>
-      </c>
-      <c r="F23" s="4">
-        <v>0</v>
-      </c>
-      <c r="G23" s="4">
-        <v>0</v>
-      </c>
-      <c r="H23" s="4">
-        <v>0</v>
-      </c>
-      <c r="I23" s="4">
-        <v>0</v>
-      </c>
-      <c r="J23" s="4">
-        <v>0</v>
-      </c>
-      <c r="K23" s="4">
-        <v>0</v>
-      </c>
-      <c r="L23" s="4">
-        <v>0</v>
-      </c>
-      <c r="M23" s="4">
-        <v>0</v>
-      </c>
-      <c r="N23" s="4">
-        <v>0</v>
-      </c>
-      <c r="O23" s="4">
-        <v>0</v>
-      </c>
-      <c r="P23" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q23" s="4">
-        <v>0</v>
-      </c>
-      <c r="R23" s="4">
-        <v>0</v>
-      </c>
-      <c r="S23" s="31">
-        <v>0</v>
-      </c>
-      <c r="T23" s="31">
-        <v>0</v>
-      </c>
-      <c r="U23" s="31">
-        <v>0</v>
-      </c>
-      <c r="V23" s="34">
+      <c r="D23" s="13">
+        <v>0</v>
+      </c>
+      <c r="E23" s="3">
+        <v>0</v>
+      </c>
+      <c r="F23" s="3">
+        <v>0</v>
+      </c>
+      <c r="G23" s="3">
+        <v>0</v>
+      </c>
+      <c r="H23" s="3">
+        <v>0</v>
+      </c>
+      <c r="I23" s="3">
+        <v>0</v>
+      </c>
+      <c r="J23" s="3">
+        <v>0</v>
+      </c>
+      <c r="K23" s="3">
+        <v>0</v>
+      </c>
+      <c r="L23" s="3">
+        <v>0</v>
+      </c>
+      <c r="M23" s="3">
+        <v>0</v>
+      </c>
+      <c r="N23" s="3">
+        <v>0</v>
+      </c>
+      <c r="O23" s="3">
+        <v>0</v>
+      </c>
+      <c r="P23" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="3">
+        <v>0</v>
+      </c>
+      <c r="R23" s="3">
+        <v>0</v>
+      </c>
+      <c r="S23" s="25">
+        <v>0</v>
+      </c>
+      <c r="T23" s="25">
+        <v>0</v>
+      </c>
+      <c r="U23" s="25">
+        <v>0</v>
+      </c>
+      <c r="V23" s="28">
         <v>0.5</v>
       </c>
     </row>
     <row r="24" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="D24" s="13">
+      <c r="D24" s="11">
         <v>23</v>
       </c>
-      <c r="E24" s="13">
+      <c r="E24" s="11">
         <f>D24-SUM(E4:E23)</f>
         <v>22</v>
       </c>
-      <c r="F24" s="13">
+      <c r="F24" s="11">
         <f>E24-SUM(F4:F23)</f>
         <v>21</v>
       </c>
-      <c r="G24" s="13">
+      <c r="G24" s="11">
         <f>F24-SUM(G4:G23)</f>
         <v>19</v>
       </c>
-      <c r="H24" s="13">
+      <c r="H24" s="11">
         <f t="shared" ref="H24:V24" si="0">G24-SUM(H4:H23)</f>
         <v>18</v>
       </c>
-      <c r="I24" s="13">
+      <c r="I24" s="11">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="J24" s="13">
+      <c r="J24" s="11">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="K24" s="13">
+      <c r="K24" s="11">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="L24" s="13">
+      <c r="L24" s="11">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="M24" s="13">
+      <c r="M24" s="11">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="N24" s="13">
+      <c r="N24" s="11">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="O24" s="13">
+      <c r="O24" s="11">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="P24" s="13">
+      <c r="P24" s="11">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="Q24" s="13">
+      <c r="Q24" s="11">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="R24" s="13">
+      <c r="R24" s="11">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="S24" s="13">
+      <c r="S24" s="11">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="T24" s="13">
+      <c r="T24" s="11">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="U24" s="13">
+      <c r="U24" s="11">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="V24" s="19">
+      <c r="V24" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Update: annotated sprint 1 + homepage CI
</commit_message>
<xml_diff>
--- a/Group C2-3 Scrum documentation.xlsx
+++ b/Group C2-3 Scrum documentation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johna\OneDrive\Documents\University\Year II\CO553 Agile Development and Software Security B\co553-c2-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60A1F294-FD20-47D3-81EA-6401AD42E9CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48497EA2-FCBC-44D0-88A2-85AA02879323}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0CC9FE5D-919A-41CA-B32D-5FFC3808111C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{0CC9FE5D-919A-41CA-B32D-5FFC3808111C}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -150,9 +150,6 @@
     <t>Display the available ticket options and prices [3]</t>
   </si>
   <si>
-    <t>Create a registration form that asks for forename, surname, email, password (twice) [0.5]</t>
-  </si>
-  <si>
     <t>Validate the fields (check if they are filled and the email and password meet criteria) [0.5]</t>
   </si>
   <si>
@@ -229,12 +226,15 @@
       <t>[0.25]</t>
     </r>
   </si>
+  <si>
+    <t>Create a registration form that asks for forename, surname, email, password [0.5]</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -277,8 +277,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -312,8 +319,13 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -440,14 +452,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -480,9 +508,15 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -495,19 +529,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="12" xfId="4"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Input" xfId="4" builtinId="20"/>
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1986,7 +2014,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F2ABAF1-62E6-41B4-BC47-CFBA7BD3B611}">
   <dimension ref="B2:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
@@ -2007,68 +2035,68 @@
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="33">
+      <c r="B3" s="26">
         <v>1</v>
       </c>
-      <c r="C3" s="33" t="s">
+      <c r="C3" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="33">
+      <c r="D3" s="26">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="34">
+      <c r="B4" s="27">
         <v>2</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="34">
+      <c r="D4" s="27">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="34">
+      <c r="B5" s="27">
         <v>3</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="34">
+      <c r="D5" s="27">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="34">
+      <c r="B6" s="27">
         <v>4</v>
       </c>
-      <c r="C6" s="35" t="s">
+      <c r="C6" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="34">
+      <c r="D6" s="27">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="34">
+      <c r="B7" s="27">
         <v>5</v>
       </c>
-      <c r="C7" s="34" t="s">
+      <c r="C7" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="34">
+      <c r="D7" s="27">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="34">
+      <c r="B8" s="27">
         <v>6</v>
       </c>
-      <c r="C8" s="34" t="s">
+      <c r="C8" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="34">
+      <c r="D8" s="27">
         <v>1</v>
       </c>
     </row>
@@ -2217,8 +2245,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1498325-30FB-42AD-97E8-3EAEC03F161C}">
   <dimension ref="B2:V24"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13:P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2235,7 +2263,7 @@
         <v>21</v>
       </c>
       <c r="D2" s="31" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E2" s="31"/>
       <c r="F2" s="31"/>
@@ -2322,7 +2350,7 @@
         <v>22</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D4" s="11">
         <v>0</v>
@@ -2330,19 +2358,19 @@
       <c r="E4" s="21">
         <v>0.25</v>
       </c>
-      <c r="F4" s="24">
-        <v>0</v>
-      </c>
-      <c r="G4" s="24">
-        <v>0</v>
-      </c>
-      <c r="H4" s="24">
-        <v>0</v>
-      </c>
-      <c r="I4" s="24">
-        <v>0</v>
-      </c>
-      <c r="J4" s="24">
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
         <v>0</v>
       </c>
       <c r="K4" s="2">
@@ -2385,7 +2413,7 @@
     <row r="5" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B5" s="32"/>
       <c r="C5" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D5" s="12">
         <v>0</v>
@@ -2393,19 +2421,19 @@
       <c r="E5" s="21">
         <v>0.25</v>
       </c>
-      <c r="F5" s="24">
-        <v>0</v>
-      </c>
-      <c r="G5" s="24">
-        <v>0</v>
-      </c>
-      <c r="H5" s="24">
-        <v>0</v>
-      </c>
-      <c r="I5" s="24">
-        <v>0</v>
-      </c>
-      <c r="J5" s="24">
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
         <v>0</v>
       </c>
       <c r="K5" s="2">
@@ -2448,27 +2476,27 @@
     <row r="6" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B6" s="32"/>
       <c r="C6" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D6" s="12">
         <v>0</v>
       </c>
-      <c r="E6" s="19">
+      <c r="E6" s="21">
         <v>0.25</v>
       </c>
-      <c r="F6" s="24">
-        <v>0</v>
-      </c>
-      <c r="G6" s="24">
-        <v>0</v>
-      </c>
-      <c r="H6" s="24">
-        <v>0</v>
-      </c>
-      <c r="I6" s="24">
-        <v>0</v>
-      </c>
-      <c r="J6" s="24">
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
         <v>0</v>
       </c>
       <c r="K6" s="2">
@@ -2511,27 +2539,27 @@
     <row r="7" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B7" s="30"/>
       <c r="C7" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D7" s="13">
         <v>0</v>
       </c>
-      <c r="E7" s="20">
+      <c r="E7" s="33">
         <v>0.25</v>
       </c>
-      <c r="F7" s="25">
-        <v>0</v>
-      </c>
-      <c r="G7" s="25">
-        <v>0</v>
-      </c>
-      <c r="H7" s="25">
-        <v>0</v>
-      </c>
-      <c r="I7" s="25">
-        <v>0</v>
-      </c>
-      <c r="J7" s="25">
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
         <v>0</v>
       </c>
       <c r="K7" s="3">
@@ -2581,22 +2609,22 @@
       <c r="D8" s="11">
         <v>0</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8">
         <v>0</v>
       </c>
       <c r="F8" s="22">
         <v>1</v>
       </c>
-      <c r="G8" s="23">
-        <v>0</v>
-      </c>
-      <c r="H8" s="23">
-        <v>0</v>
-      </c>
-      <c r="I8" s="23">
-        <v>0</v>
-      </c>
-      <c r="J8" s="23">
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
         <v>0</v>
       </c>
       <c r="K8" s="10">
@@ -2644,22 +2672,22 @@
       <c r="D9" s="12">
         <v>0</v>
       </c>
-      <c r="E9" s="24">
-        <v>0</v>
-      </c>
-      <c r="F9" s="24">
-        <v>0</v>
-      </c>
-      <c r="G9" s="19">
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9" s="21">
         <v>2</v>
       </c>
-      <c r="H9" s="24">
-        <v>0</v>
-      </c>
-      <c r="I9" s="24">
-        <v>0</v>
-      </c>
-      <c r="J9" s="24">
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
         <v>0</v>
       </c>
       <c r="K9" s="2">
@@ -2707,22 +2735,22 @@
       <c r="D10" s="12">
         <v>0</v>
       </c>
-      <c r="E10" s="24">
-        <v>0</v>
-      </c>
-      <c r="F10" s="24">
-        <v>0</v>
-      </c>
-      <c r="G10" s="24">
-        <v>0</v>
-      </c>
-      <c r="H10" s="19">
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10" s="21">
         <v>1</v>
       </c>
-      <c r="I10" s="24">
-        <v>0</v>
-      </c>
-      <c r="J10" s="24">
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
         <v>0</v>
       </c>
       <c r="K10" s="2">
@@ -2770,22 +2798,22 @@
       <c r="D11" s="12">
         <v>0</v>
       </c>
-      <c r="E11" s="24">
-        <v>0</v>
-      </c>
-      <c r="F11" s="24">
-        <v>0</v>
-      </c>
-      <c r="G11" s="24">
-        <v>0</v>
-      </c>
-      <c r="H11" s="24">
-        <v>0</v>
-      </c>
-      <c r="I11" s="19">
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11" s="21">
         <v>2</v>
       </c>
-      <c r="J11" s="24">
+      <c r="J11">
         <v>0</v>
       </c>
       <c r="K11" s="2">
@@ -2833,22 +2861,22 @@
       <c r="D12" s="13">
         <v>0</v>
       </c>
-      <c r="E12" s="25">
-        <v>0</v>
-      </c>
-      <c r="F12" s="25">
-        <v>0</v>
-      </c>
-      <c r="G12" s="25">
-        <v>0</v>
-      </c>
-      <c r="H12" s="25">
-        <v>0</v>
-      </c>
-      <c r="I12" s="25">
-        <v>0</v>
-      </c>
-      <c r="J12" s="20">
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12" s="33">
         <v>2</v>
       </c>
       <c r="K12" s="3">
@@ -2922,22 +2950,22 @@
       <c r="L13" s="23">
         <v>1</v>
       </c>
-      <c r="M13" s="23">
-        <v>0</v>
-      </c>
-      <c r="N13" s="23">
-        <v>0</v>
-      </c>
-      <c r="O13" s="23">
-        <v>0</v>
-      </c>
-      <c r="P13" s="23">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="23">
-        <v>0</v>
-      </c>
-      <c r="R13" s="23">
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13">
         <v>0</v>
       </c>
       <c r="S13" s="10">
@@ -2979,28 +3007,28 @@
       <c r="J14" s="2">
         <v>0</v>
       </c>
-      <c r="K14" s="24">
-        <v>0</v>
-      </c>
-      <c r="L14" s="24">
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
         <v>0</v>
       </c>
       <c r="M14" s="24">
         <v>1</v>
       </c>
-      <c r="N14" s="24">
-        <v>0</v>
-      </c>
-      <c r="O14" s="24">
-        <v>0</v>
-      </c>
-      <c r="P14" s="24">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="24">
-        <v>0</v>
-      </c>
-      <c r="R14" s="24">
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+      <c r="R14">
         <v>0</v>
       </c>
       <c r="S14" s="2">
@@ -3042,13 +3070,13 @@
       <c r="J15" s="2">
         <v>0</v>
       </c>
-      <c r="K15" s="24">
-        <v>0</v>
-      </c>
-      <c r="L15" s="24">
-        <v>0</v>
-      </c>
-      <c r="M15" s="24">
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
         <v>0</v>
       </c>
       <c r="N15" s="24">
@@ -3057,13 +3085,13 @@
       <c r="O15" s="24">
         <v>1</v>
       </c>
-      <c r="P15" s="24">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="24">
-        <v>0</v>
-      </c>
-      <c r="R15" s="24">
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+      <c r="R15">
         <v>0</v>
       </c>
       <c r="S15" s="2">
@@ -3105,19 +3133,19 @@
       <c r="J16" s="3">
         <v>0</v>
       </c>
-      <c r="K16" s="25">
-        <v>0</v>
-      </c>
-      <c r="L16" s="25">
-        <v>0</v>
-      </c>
-      <c r="M16" s="25">
-        <v>0</v>
-      </c>
-      <c r="N16" s="25">
-        <v>0</v>
-      </c>
-      <c r="O16" s="25">
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
         <v>0</v>
       </c>
       <c r="P16" s="25">
@@ -3147,7 +3175,7 @@
         <v>26</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="D17" s="11">
         <v>0</v>
@@ -3197,20 +3225,20 @@
       <c r="S17" s="22">
         <v>0.5</v>
       </c>
-      <c r="T17" s="23">
-        <v>0</v>
-      </c>
-      <c r="U17" s="23">
-        <v>0</v>
-      </c>
-      <c r="V17" s="26">
+      <c r="T17">
+        <v>0</v>
+      </c>
+      <c r="U17">
+        <v>0</v>
+      </c>
+      <c r="V17">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B18" s="32"/>
       <c r="C18" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D18" s="12">
         <v>0</v>
@@ -3257,23 +3285,23 @@
       <c r="R18" s="2">
         <v>0</v>
       </c>
-      <c r="S18" s="24">
+      <c r="S18" s="19">
         <v>0.5</v>
       </c>
-      <c r="T18" s="24">
-        <v>0</v>
-      </c>
-      <c r="U18" s="24">
-        <v>0</v>
-      </c>
-      <c r="V18" s="27">
+      <c r="T18">
+        <v>0</v>
+      </c>
+      <c r="U18">
+        <v>0</v>
+      </c>
+      <c r="V18">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B19" s="30"/>
       <c r="C19" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D19" s="13">
         <v>0</v>
@@ -3320,16 +3348,16 @@
       <c r="R19" s="3">
         <v>0</v>
       </c>
-      <c r="S19" s="25">
-        <v>0</v>
-      </c>
-      <c r="T19" s="25">
+      <c r="S19" s="3">
+        <v>0</v>
+      </c>
+      <c r="T19" s="20">
         <v>1</v>
       </c>
-      <c r="U19" s="25">
-        <v>0</v>
-      </c>
-      <c r="V19" s="28">
+      <c r="U19">
+        <v>0</v>
+      </c>
+      <c r="V19">
         <v>0</v>
       </c>
     </row>
@@ -3338,7 +3366,7 @@
         <v>27</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D20" s="11">
         <v>0</v>
@@ -3385,23 +3413,23 @@
       <c r="R20" s="10">
         <v>0</v>
       </c>
-      <c r="S20" s="23">
-        <v>0</v>
-      </c>
-      <c r="T20" s="23">
+      <c r="S20">
+        <v>0</v>
+      </c>
+      <c r="T20">
         <v>0</v>
       </c>
       <c r="U20" s="22">
         <v>0.5</v>
       </c>
-      <c r="V20" s="26">
+      <c r="V20">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B21" s="30"/>
       <c r="C21" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D21" s="13">
         <v>0</v>
@@ -3448,16 +3476,16 @@
       <c r="R21" s="3">
         <v>0</v>
       </c>
-      <c r="S21" s="25">
-        <v>0</v>
-      </c>
-      <c r="T21" s="25">
-        <v>0</v>
-      </c>
-      <c r="U21" s="25">
+      <c r="S21" s="3">
+        <v>0</v>
+      </c>
+      <c r="T21" s="3">
+        <v>0</v>
+      </c>
+      <c r="U21" s="20">
         <v>0.5</v>
       </c>
-      <c r="V21" s="28">
+      <c r="V21">
         <v>0</v>
       </c>
     </row>
@@ -3466,7 +3494,7 @@
         <v>28</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D22" s="11">
         <v>0</v>
@@ -3513,23 +3541,23 @@
       <c r="R22" s="10">
         <v>0</v>
       </c>
-      <c r="S22" s="23">
-        <v>0</v>
-      </c>
-      <c r="T22" s="23">
-        <v>0</v>
-      </c>
-      <c r="U22" s="23">
-        <v>0</v>
-      </c>
-      <c r="V22" s="26">
+      <c r="S22">
+        <v>0</v>
+      </c>
+      <c r="T22">
+        <v>0</v>
+      </c>
+      <c r="U22">
+        <v>0</v>
+      </c>
+      <c r="V22" s="34">
         <v>0.5</v>
       </c>
     </row>
     <row r="23" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B23" s="30"/>
       <c r="C23" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D23" s="13">
         <v>0</v>
@@ -3576,16 +3604,16 @@
       <c r="R23" s="3">
         <v>0</v>
       </c>
-      <c r="S23" s="25">
-        <v>0</v>
-      </c>
-      <c r="T23" s="25">
-        <v>0</v>
-      </c>
-      <c r="U23" s="25">
-        <v>0</v>
-      </c>
-      <c r="V23" s="28">
+      <c r="S23">
+        <v>0</v>
+      </c>
+      <c r="T23">
+        <v>0</v>
+      </c>
+      <c r="U23">
+        <v>0</v>
+      </c>
+      <c r="V23" s="34">
         <v>0.5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update: Sprint retrospective and review
</commit_message>
<xml_diff>
--- a/Group C2-3 Scrum documentation.xlsx
+++ b/Group C2-3 Scrum documentation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johna\OneDrive\Documents\University\Year II\CO553 Agile Development and Software Security B\co553-c2-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFB1F87B-16BE-4A7B-AD45-F5AEBF80658E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D57C522C-4C34-43AC-8051-B2485FFF1A7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{0CC9FE5D-919A-41CA-B32D-5FFC3808111C}"/>
   </bookViews>
@@ -234,7 +234,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -270,22 +270,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="8">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -312,16 +298,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
       </patternFill>
     </fill>
   </fills>
@@ -468,14 +444,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -501,8 +475,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="8" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="2" applyBorder="1"/>
@@ -517,6 +489,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -529,14 +502,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="12" xfId="4"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Input" xfId="4" builtinId="20"/>
-    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2015,7 +1985,7 @@
   <dimension ref="B2:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2035,68 +2005,68 @@
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="26">
+      <c r="B3" s="24">
         <v>1</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="26">
+      <c r="D3" s="24">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="27">
+      <c r="B4" s="25">
         <v>2</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="27">
+      <c r="D4" s="25">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="27">
+      <c r="B5" s="25">
         <v>3</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="27">
+      <c r="D5" s="25">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="27">
+      <c r="B6" s="25">
         <v>4</v>
       </c>
-      <c r="C6" s="28" t="s">
+      <c r="C6" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="27">
+      <c r="D6" s="25">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="27">
+      <c r="B7" s="25">
         <v>5</v>
       </c>
-      <c r="C7" s="27" t="s">
+      <c r="C7" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="27">
+      <c r="D7" s="25">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="27">
+      <c r="B8" s="25">
         <v>6</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="27">
+      <c r="D8" s="25">
         <v>1</v>
       </c>
     </row>
@@ -2245,8 +2215,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1498325-30FB-42AD-97E8-3EAEC03F161C}">
   <dimension ref="B2:V24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W37" sqref="W37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2262,27 +2232,27 @@
       <c r="C2" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="31" t="s">
+      <c r="D2" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="31"/>
-      <c r="O2" s="31"/>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="31"/>
-      <c r="R2" s="31"/>
-      <c r="S2" s="31"/>
-      <c r="T2" s="31"/>
-      <c r="U2" s="31"/>
-      <c r="V2" s="31"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="30"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="30"/>
+      <c r="R2" s="30"/>
+      <c r="S2" s="30"/>
+      <c r="T2" s="30"/>
+      <c r="U2" s="30"/>
+      <c r="V2" s="30"/>
     </row>
     <row r="3" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B3" s="18"/>
@@ -2346,7 +2316,7 @@
       </c>
     </row>
     <row r="4" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="28" t="s">
         <v>22</v>
       </c>
       <c r="C4" s="8" t="s">
@@ -2355,7 +2325,7 @@
       <c r="D4" s="11">
         <v>0</v>
       </c>
-      <c r="E4" s="21">
+      <c r="E4" s="19">
         <v>0.25</v>
       </c>
       <c r="F4">
@@ -2411,14 +2381,14 @@
       </c>
     </row>
     <row r="5" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B5" s="32"/>
+      <c r="B5" s="31"/>
       <c r="C5" s="8" t="s">
         <v>47</v>
       </c>
       <c r="D5" s="12">
         <v>0</v>
       </c>
-      <c r="E5" s="21">
+      <c r="E5" s="19">
         <v>0.25</v>
       </c>
       <c r="F5">
@@ -2474,14 +2444,14 @@
       </c>
     </row>
     <row r="6" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B6" s="32"/>
+      <c r="B6" s="31"/>
       <c r="C6" s="2" t="s">
         <v>46</v>
       </c>
       <c r="D6" s="12">
         <v>0</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="19">
         <v>0.25</v>
       </c>
       <c r="F6">
@@ -2537,14 +2507,14 @@
       </c>
     </row>
     <row r="7" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B7" s="30"/>
+      <c r="B7" s="29"/>
       <c r="C7" s="3" t="s">
         <v>45</v>
       </c>
       <c r="D7" s="13">
         <v>0</v>
       </c>
-      <c r="E7" s="33">
+      <c r="E7" s="27">
         <v>0.25</v>
       </c>
       <c r="F7">
@@ -2600,7 +2570,7 @@
       </c>
     </row>
     <row r="8" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="28" t="s">
         <v>23</v>
       </c>
       <c r="C8" s="10" t="s">
@@ -2612,7 +2582,7 @@
       <c r="E8">
         <v>0</v>
       </c>
-      <c r="F8" s="22">
+      <c r="F8" s="20">
         <v>1</v>
       </c>
       <c r="G8">
@@ -2665,7 +2635,7 @@
       </c>
     </row>
     <row r="9" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B9" s="32"/>
+      <c r="B9" s="31"/>
       <c r="C9" s="2" t="s">
         <v>30</v>
       </c>
@@ -2678,7 +2648,7 @@
       <c r="F9">
         <v>0</v>
       </c>
-      <c r="G9" s="21">
+      <c r="G9" s="19">
         <v>2</v>
       </c>
       <c r="H9">
@@ -2728,7 +2698,7 @@
       </c>
     </row>
     <row r="10" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B10" s="32"/>
+      <c r="B10" s="31"/>
       <c r="C10" s="2" t="s">
         <v>31</v>
       </c>
@@ -2744,7 +2714,7 @@
       <c r="G10">
         <v>0</v>
       </c>
-      <c r="H10" s="21">
+      <c r="H10" s="19">
         <v>1</v>
       </c>
       <c r="I10">
@@ -2791,7 +2761,7 @@
       </c>
     </row>
     <row r="11" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B11" s="32"/>
+      <c r="B11" s="31"/>
       <c r="C11" s="2" t="s">
         <v>32</v>
       </c>
@@ -2810,7 +2780,7 @@
       <c r="H11">
         <v>0</v>
       </c>
-      <c r="I11" s="21">
+      <c r="I11" s="19">
         <v>2</v>
       </c>
       <c r="J11">
@@ -2854,7 +2824,7 @@
       </c>
     </row>
     <row r="12" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B12" s="30"/>
+      <c r="B12" s="29"/>
       <c r="C12" s="3" t="s">
         <v>33</v>
       </c>
@@ -2876,7 +2846,7 @@
       <c r="I12">
         <v>0</v>
       </c>
-      <c r="J12" s="33">
+      <c r="J12" s="27">
         <v>2</v>
       </c>
       <c r="K12" s="3">
@@ -2917,7 +2887,7 @@
       </c>
     </row>
     <row r="13" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B13" s="29" t="s">
+      <c r="B13" s="28" t="s">
         <v>24</v>
       </c>
       <c r="C13" s="10" t="s">
@@ -2944,10 +2914,10 @@
       <c r="J13" s="10">
         <v>0</v>
       </c>
-      <c r="K13" s="23">
+      <c r="K13" s="21">
         <v>2</v>
       </c>
-      <c r="L13" s="23">
+      <c r="L13" s="21">
         <v>1</v>
       </c>
       <c r="M13">
@@ -2982,7 +2952,7 @@
       </c>
     </row>
     <row r="14" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B14" s="32"/>
+      <c r="B14" s="31"/>
       <c r="C14" s="2" t="s">
         <v>35</v>
       </c>
@@ -3013,7 +2983,7 @@
       <c r="L14">
         <v>0</v>
       </c>
-      <c r="M14" s="24">
+      <c r="M14" s="22">
         <v>1</v>
       </c>
       <c r="N14">
@@ -3045,7 +3015,7 @@
       </c>
     </row>
     <row r="15" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B15" s="32"/>
+      <c r="B15" s="31"/>
       <c r="C15" s="2" t="s">
         <v>36</v>
       </c>
@@ -3079,10 +3049,10 @@
       <c r="M15">
         <v>0</v>
       </c>
-      <c r="N15" s="24">
+      <c r="N15" s="22">
         <v>2</v>
       </c>
-      <c r="O15" s="24">
+      <c r="O15" s="22">
         <v>1</v>
       </c>
       <c r="P15">
@@ -3108,7 +3078,7 @@
       </c>
     </row>
     <row r="16" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B16" s="30"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="3" t="s">
         <v>37</v>
       </c>
@@ -3148,13 +3118,13 @@
       <c r="O16">
         <v>0</v>
       </c>
-      <c r="P16" s="25">
+      <c r="P16" s="23">
         <v>1</v>
       </c>
-      <c r="Q16" s="25">
+      <c r="Q16" s="23">
         <v>1</v>
       </c>
-      <c r="R16" s="25">
+      <c r="R16" s="23">
         <v>1</v>
       </c>
       <c r="S16" s="3">
@@ -3171,7 +3141,7 @@
       </c>
     </row>
     <row r="17" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B17" s="29" t="s">
+      <c r="B17" s="28" t="s">
         <v>26</v>
       </c>
       <c r="C17" s="10" t="s">
@@ -3222,7 +3192,7 @@
       <c r="R17" s="10">
         <v>0</v>
       </c>
-      <c r="S17" s="22">
+      <c r="S17" s="20">
         <v>0.5</v>
       </c>
       <c r="T17">
@@ -3236,7 +3206,7 @@
       </c>
     </row>
     <row r="18" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B18" s="32"/>
+      <c r="B18" s="31"/>
       <c r="C18" s="2" t="s">
         <v>38</v>
       </c>
@@ -3299,7 +3269,7 @@
       </c>
     </row>
     <row r="19" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B19" s="30"/>
+      <c r="B19" s="29"/>
       <c r="C19" s="3" t="s">
         <v>39</v>
       </c>
@@ -3351,7 +3321,7 @@
       <c r="S19" s="3">
         <v>0</v>
       </c>
-      <c r="T19" s="20">
+      <c r="T19" s="27">
         <v>1</v>
       </c>
       <c r="U19">
@@ -3362,7 +3332,7 @@
       </c>
     </row>
     <row r="20" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B20" s="29" t="s">
+      <c r="B20" s="28" t="s">
         <v>27</v>
       </c>
       <c r="C20" s="10" t="s">
@@ -3419,7 +3389,7 @@
       <c r="T20">
         <v>0</v>
       </c>
-      <c r="U20" s="22">
+      <c r="U20" s="20">
         <v>0.5</v>
       </c>
       <c r="V20">
@@ -3427,7 +3397,7 @@
       </c>
     </row>
     <row r="21" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B21" s="30"/>
+      <c r="B21" s="29"/>
       <c r="C21" s="3" t="s">
         <v>41</v>
       </c>
@@ -3482,7 +3452,7 @@
       <c r="T21" s="3">
         <v>0</v>
       </c>
-      <c r="U21" s="20">
+      <c r="U21" s="27">
         <v>0.5</v>
       </c>
       <c r="V21">
@@ -3490,7 +3460,7 @@
       </c>
     </row>
     <row r="22" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B22" s="29" t="s">
+      <c r="B22" s="28" t="s">
         <v>28</v>
       </c>
       <c r="C22" s="10" t="s">
@@ -3550,12 +3520,12 @@
       <c r="U22">
         <v>0</v>
       </c>
-      <c r="V22" s="34">
+      <c r="V22" s="32">
         <v>0.5</v>
       </c>
     </row>
     <row r="23" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B23" s="30"/>
+      <c r="B23" s="29"/>
       <c r="C23" s="3" t="s">
         <v>43</v>
       </c>
@@ -3613,7 +3583,7 @@
       <c r="U23">
         <v>0</v>
       </c>
-      <c r="V23" s="34">
+      <c r="V23" s="32">
         <v>0.5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update: Scrum documentation sprint 2
</commit_message>
<xml_diff>
--- a/Group C2-3 Scrum documentation.xlsx
+++ b/Group C2-3 Scrum documentation.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johna\OneDrive\Documents\University\Year II\CO553 Agile Development and Software Security B\co553-c2-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D57C522C-4C34-43AC-8051-B2485FFF1A7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AF0A7555-A1B7-4946-8409-67A4A43647BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{0CC9FE5D-919A-41CA-B32D-5FFC3808111C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{0CC9FE5D-919A-41CA-B32D-5FFC3808111C}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
     <sheet name="Group C2-3 Sprint 1" sheetId="2" r:id="rId2"/>
+    <sheet name="Group C2-3 Sprint 2" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="66">
   <si>
     <t>ID</t>
   </si>
@@ -229,12 +230,60 @@
   <si>
     <t>Create a registration form that asks for forename, surname, email, password [0.5]</t>
   </si>
+  <si>
+    <t>As a customer I would like to be able to buy tickets, so that I can watch movies [10 points]</t>
+  </si>
+  <si>
+    <t>As a customer i would like to select my seat/seats so that i know where i will sit when i enter the screening room [10 points]</t>
+  </si>
+  <si>
+    <t>As a customer i want to have a payment selection section so that i can pay for my tickets [6 points]</t>
+  </si>
+  <si>
+    <t>Create a drop down box so the user can select from the available screening time [3] [Evgeni]</t>
+  </si>
+  <si>
+    <t>Display the available ticket options and prices [3] [Evgeni]</t>
+  </si>
+  <si>
+    <t>Create a seats page [2] [Sukh]</t>
+  </si>
+  <si>
+    <t>Check the seat availability by comparing to the table [2.5] [Amit]</t>
+  </si>
+  <si>
+    <t>Use AJAX to turn the seat green /red(availability) [4] [Evgeni/Amit]</t>
+  </si>
+  <si>
+    <t>Proceed button that redirects to payment page [0.5] [Kezia]</t>
+  </si>
+  <si>
+    <t>Update the seat table with the availability and update the booking page with the seat number [1] [Amit]</t>
+  </si>
+  <si>
+    <t>Create payment page [1] [Kezia]</t>
+  </si>
+  <si>
+    <t>Validate payment input fields [1.5] [Sukh/Kezia]</t>
+  </si>
+  <si>
+    <t>Proceed with the booking confirmation [0.5] [Sukh]</t>
+  </si>
+  <si>
+    <t>Create table with the information inputted [3] [Evgeni]</t>
+  </si>
+  <si>
+    <t>Access the ticket stock database and check the availability [3] [Amit]</t>
+  </si>
+  <si>
+    <t>Display 'sold out' if no tickets are available [1] [Kezia]</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -270,8 +319,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -298,6 +361,16 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
       </patternFill>
     </fill>
   </fills>
@@ -444,22 +517,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -490,6 +561,22 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="10" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="12" xfId="4" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="12" xfId="4"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -502,11 +589,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Input" xfId="4" builtinId="20"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -608,7 +699,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="C00000"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1088,7 +1179,661 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" b="1"/>
+              <a:t>Burndown Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Group C2-3 Sprint 2'!$D$3:$AC$3</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>44242</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44243</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44244</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44245</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44246</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44247</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44248</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44249</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44250</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44251</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44252</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44253</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>44254</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>44255</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>44256</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>44257</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>44258</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>44259</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>44260</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>44261</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>44262</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>44263</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>44264</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>44265</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>44266</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>44267</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Group C2-3 Sprint 2'!$D$17:$AC$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0182-4ECF-8344-C617F4982977}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="668577120"/>
+        <c:axId val="668577448"/>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="668577120"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Sprint</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> Duration</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.49371158094218992"/>
+              <c:y val="0.92824013749550338"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="668577448"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="668577448"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Points Remaining</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="1.0741688844810507E-2"/>
+              <c:y val="0.4091653010378779"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="668577120"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1644,20 +2389,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>379318</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>4162104</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>36700</xdr:rowOff>
+      <xdr:rowOff>145558</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>414619</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>6565047</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>67236</xdr:rowOff>
+      <xdr:rowOff>176094</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1665,6 +2926,47 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2484B4E8-EB42-4F13-ADFE-2D02AF74C521}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2000252</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2952751</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5BB29EC8-177A-4E09-8AEC-69D24545A920}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1985,7 +3287,7 @@
   <dimension ref="B2:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1994,211 +3296,211 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="6" t="s">
+      <c r="B2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="24">
+      <c r="B3" s="22">
         <v>1</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="24">
+      <c r="D3" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="25">
+      <c r="B4" s="23">
         <v>2</v>
       </c>
-      <c r="C4" s="25" t="s">
+      <c r="C4" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="25">
+      <c r="D4" s="23">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="25">
+      <c r="B5" s="28">
         <v>3</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="25">
+      <c r="D5" s="28">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="25">
+      <c r="B6" s="23">
         <v>4</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="25">
+      <c r="D6" s="23">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="25">
+      <c r="B7" s="23">
         <v>5</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="25">
+      <c r="D7" s="23">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="25">
+      <c r="B8" s="23">
         <v>6</v>
       </c>
-      <c r="C8" s="25" t="s">
+      <c r="C8" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="25">
+      <c r="D8" s="23">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="4">
+      <c r="B9" s="28">
         <v>7</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="28">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="4">
+      <c r="B10" s="28">
         <v>8</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="28">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="4">
+      <c r="B11" s="29">
         <v>9</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="29">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="4">
+      <c r="B12" s="29">
         <v>10</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="29">
         <v>3</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="4">
+      <c r="B13" s="29">
         <v>11</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="29">
         <v>2</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="4">
+      <c r="B14" s="29">
         <v>12</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D14" s="29">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="4">
+      <c r="B15" s="29">
         <v>13</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D15" s="29">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="4">
+      <c r="B16" s="29">
         <v>14</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D16" s="29">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="4">
+      <c r="B17" s="30">
         <v>15</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D17" s="30">
         <v>3</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="4">
+      <c r="B18" s="29">
         <v>16</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="4">
+      <c r="D18" s="29">
         <v>5</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="4">
+      <c r="B19" s="30">
         <v>17</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="4">
+      <c r="D19" s="30">
         <v>2</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="4">
+      <c r="B20" s="30">
         <v>18</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="D20" s="4">
+      <c r="D20" s="30">
         <v>1</v>
       </c>
     </row>
@@ -2215,8 +3517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1498325-30FB-42AD-97E8-3EAEC03F161C}">
   <dimension ref="B2:V24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W37" sqref="W37"/>
+    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O29" sqref="O29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2226,106 +3528,106 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="30" t="s">
+      <c r="D2" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="30"/>
-      <c r="Q2" s="30"/>
-      <c r="R2" s="30"/>
-      <c r="S2" s="30"/>
-      <c r="T2" s="30"/>
-      <c r="U2" s="30"/>
-      <c r="V2" s="30"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="36"/>
+      <c r="O2" s="36"/>
+      <c r="P2" s="36"/>
+      <c r="Q2" s="36"/>
+      <c r="R2" s="36"/>
+      <c r="S2" s="36"/>
+      <c r="T2" s="36"/>
+      <c r="U2" s="36"/>
+      <c r="V2" s="36"/>
     </row>
     <row r="3" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="7">
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="5">
         <v>44221</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="5">
         <v>44222</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="5">
         <v>44223</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="5">
         <v>44224</v>
       </c>
-      <c r="H3" s="7">
+      <c r="H3" s="5">
         <v>44225</v>
       </c>
-      <c r="I3" s="7">
+      <c r="I3" s="5">
         <v>44226</v>
       </c>
-      <c r="J3" s="7">
+      <c r="J3" s="5">
         <v>44227</v>
       </c>
-      <c r="K3" s="7">
+      <c r="K3" s="5">
         <v>44228</v>
       </c>
-      <c r="L3" s="7">
+      <c r="L3" s="5">
         <v>44229</v>
       </c>
-      <c r="M3" s="7">
+      <c r="M3" s="5">
         <v>44230</v>
       </c>
-      <c r="N3" s="7">
+      <c r="N3" s="5">
         <v>44231</v>
       </c>
-      <c r="O3" s="7">
+      <c r="O3" s="5">
         <v>44232</v>
       </c>
-      <c r="P3" s="7">
+      <c r="P3" s="5">
         <v>44233</v>
       </c>
-      <c r="Q3" s="7">
+      <c r="Q3" s="5">
         <v>44234</v>
       </c>
-      <c r="R3" s="7">
+      <c r="R3" s="5">
         <v>44235</v>
       </c>
-      <c r="S3" s="7">
+      <c r="S3" s="5">
         <v>44236</v>
       </c>
-      <c r="T3" s="7">
+      <c r="T3" s="5">
         <v>44237</v>
       </c>
-      <c r="U3" s="7">
+      <c r="U3" s="5">
         <v>44238</v>
       </c>
-      <c r="V3" s="7">
+      <c r="V3" s="5">
         <v>44239</v>
       </c>
     </row>
     <row r="4" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="11">
-        <v>0</v>
-      </c>
-      <c r="E4" s="19">
+      <c r="D4" s="9">
+        <v>0</v>
+      </c>
+      <c r="E4" s="17">
         <v>0.25</v>
       </c>
       <c r="F4">
@@ -2376,19 +3678,19 @@
       <c r="U4" s="2">
         <v>0</v>
       </c>
-      <c r="V4" s="14">
+      <c r="V4" s="12">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B5" s="31"/>
-      <c r="C5" s="8" t="s">
+      <c r="B5" s="37"/>
+      <c r="C5" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D5" s="12">
-        <v>0</v>
-      </c>
-      <c r="E5" s="19">
+      <c r="D5" s="10">
+        <v>0</v>
+      </c>
+      <c r="E5" s="17">
         <v>0.25</v>
       </c>
       <c r="F5">
@@ -2439,19 +3741,19 @@
       <c r="U5" s="2">
         <v>0</v>
       </c>
-      <c r="V5" s="15">
+      <c r="V5" s="13">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B6" s="31"/>
+      <c r="B6" s="37"/>
       <c r="C6" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D6" s="12">
-        <v>0</v>
-      </c>
-      <c r="E6" s="19">
+      <c r="D6" s="10">
+        <v>0</v>
+      </c>
+      <c r="E6" s="17">
         <v>0.25</v>
       </c>
       <c r="F6">
@@ -2502,19 +3804,19 @@
       <c r="U6" s="2">
         <v>0</v>
       </c>
-      <c r="V6" s="15">
+      <c r="V6" s="13">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B7" s="29"/>
+      <c r="B7" s="35"/>
       <c r="C7" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D7" s="13">
-        <v>0</v>
-      </c>
-      <c r="E7" s="27">
+      <c r="D7" s="11">
+        <v>0</v>
+      </c>
+      <c r="E7" s="25">
         <v>0.25</v>
       </c>
       <c r="F7">
@@ -2565,24 +3867,24 @@
       <c r="U7" s="3">
         <v>0</v>
       </c>
-      <c r="V7" s="16">
+      <c r="V7" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="9">
         <v>0</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
-      <c r="F8" s="20">
+      <c r="F8" s="18">
         <v>1</v>
       </c>
       <c r="G8">
@@ -2597,49 +3899,49 @@
       <c r="J8">
         <v>0</v>
       </c>
-      <c r="K8" s="10">
-        <v>0</v>
-      </c>
-      <c r="L8" s="10">
-        <v>0</v>
-      </c>
-      <c r="M8" s="10">
-        <v>0</v>
-      </c>
-      <c r="N8" s="10">
-        <v>0</v>
-      </c>
-      <c r="O8" s="10">
-        <v>0</v>
-      </c>
-      <c r="P8" s="10">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="10">
-        <v>0</v>
-      </c>
-      <c r="R8" s="10">
-        <v>0</v>
-      </c>
-      <c r="S8" s="10">
-        <v>0</v>
-      </c>
-      <c r="T8" s="10">
-        <v>0</v>
-      </c>
-      <c r="U8" s="10">
-        <v>0</v>
-      </c>
-      <c r="V8" s="14">
+      <c r="K8" s="8">
+        <v>0</v>
+      </c>
+      <c r="L8" s="8">
+        <v>0</v>
+      </c>
+      <c r="M8" s="8">
+        <v>0</v>
+      </c>
+      <c r="N8" s="8">
+        <v>0</v>
+      </c>
+      <c r="O8" s="8">
+        <v>0</v>
+      </c>
+      <c r="P8" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="8">
+        <v>0</v>
+      </c>
+      <c r="R8" s="8">
+        <v>0</v>
+      </c>
+      <c r="S8" s="8">
+        <v>0</v>
+      </c>
+      <c r="T8" s="8">
+        <v>0</v>
+      </c>
+      <c r="U8" s="8">
+        <v>0</v>
+      </c>
+      <c r="V8" s="12">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B9" s="31"/>
+      <c r="B9" s="37"/>
       <c r="C9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="12">
+      <c r="D9" s="10">
         <v>0</v>
       </c>
       <c r="E9">
@@ -2648,7 +3950,7 @@
       <c r="F9">
         <v>0</v>
       </c>
-      <c r="G9" s="19">
+      <c r="G9" s="17">
         <v>2</v>
       </c>
       <c r="H9">
@@ -2693,16 +3995,16 @@
       <c r="U9" s="2">
         <v>0</v>
       </c>
-      <c r="V9" s="15">
+      <c r="V9" s="13">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B10" s="31"/>
+      <c r="B10" s="37"/>
       <c r="C10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="12">
+      <c r="D10" s="10">
         <v>0</v>
       </c>
       <c r="E10">
@@ -2714,7 +4016,7 @@
       <c r="G10">
         <v>0</v>
       </c>
-      <c r="H10" s="19">
+      <c r="H10" s="17">
         <v>1</v>
       </c>
       <c r="I10">
@@ -2756,16 +4058,16 @@
       <c r="U10" s="2">
         <v>0</v>
       </c>
-      <c r="V10" s="15">
+      <c r="V10" s="13">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B11" s="31"/>
+      <c r="B11" s="37"/>
       <c r="C11" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="12">
+      <c r="D11" s="10">
         <v>0</v>
       </c>
       <c r="E11">
@@ -2780,7 +4082,7 @@
       <c r="H11">
         <v>0</v>
       </c>
-      <c r="I11" s="19">
+      <c r="I11" s="17">
         <v>2</v>
       </c>
       <c r="J11">
@@ -2819,16 +4121,16 @@
       <c r="U11" s="2">
         <v>0</v>
       </c>
-      <c r="V11" s="15">
+      <c r="V11" s="13">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B12" s="29"/>
+      <c r="B12" s="35"/>
       <c r="C12" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="13">
+      <c r="D12" s="11">
         <v>0</v>
       </c>
       <c r="E12">
@@ -2846,7 +4148,7 @@
       <c r="I12">
         <v>0</v>
       </c>
-      <c r="J12" s="27">
+      <c r="J12" s="25">
         <v>2</v>
       </c>
       <c r="K12" s="3">
@@ -2882,42 +4184,42 @@
       <c r="U12" s="3">
         <v>0</v>
       </c>
-      <c r="V12" s="16">
+      <c r="V12" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B13" s="28" t="s">
+      <c r="B13" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="11">
-        <v>0</v>
-      </c>
-      <c r="E13" s="10">
-        <v>0</v>
-      </c>
-      <c r="F13" s="10">
-        <v>0</v>
-      </c>
-      <c r="G13" s="10">
-        <v>0</v>
-      </c>
-      <c r="H13" s="10">
-        <v>0</v>
-      </c>
-      <c r="I13" s="10">
-        <v>0</v>
-      </c>
-      <c r="J13" s="10">
-        <v>0</v>
-      </c>
-      <c r="K13" s="21">
+      <c r="D13" s="9">
+        <v>0</v>
+      </c>
+      <c r="E13" s="8">
+        <v>0</v>
+      </c>
+      <c r="F13" s="8">
+        <v>0</v>
+      </c>
+      <c r="G13" s="8">
+        <v>0</v>
+      </c>
+      <c r="H13" s="8">
+        <v>0</v>
+      </c>
+      <c r="I13" s="8">
+        <v>0</v>
+      </c>
+      <c r="J13" s="8">
+        <v>0</v>
+      </c>
+      <c r="K13" s="19">
         <v>2</v>
       </c>
-      <c r="L13" s="21">
+      <c r="L13" s="19">
         <v>1</v>
       </c>
       <c r="M13">
@@ -2938,25 +4240,25 @@
       <c r="R13">
         <v>0</v>
       </c>
-      <c r="S13" s="10">
-        <v>0</v>
-      </c>
-      <c r="T13" s="10">
-        <v>0</v>
-      </c>
-      <c r="U13" s="10">
-        <v>0</v>
-      </c>
-      <c r="V13" s="14">
+      <c r="S13" s="8">
+        <v>0</v>
+      </c>
+      <c r="T13" s="8">
+        <v>0</v>
+      </c>
+      <c r="U13" s="8">
+        <v>0</v>
+      </c>
+      <c r="V13" s="12">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B14" s="31"/>
+      <c r="B14" s="37"/>
       <c r="C14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="12">
+      <c r="D14" s="10">
         <v>0</v>
       </c>
       <c r="E14" s="2">
@@ -2983,7 +4285,7 @@
       <c r="L14">
         <v>0</v>
       </c>
-      <c r="M14" s="22">
+      <c r="M14" s="20">
         <v>1</v>
       </c>
       <c r="N14">
@@ -3010,16 +4312,16 @@
       <c r="U14" s="2">
         <v>0</v>
       </c>
-      <c r="V14" s="15">
+      <c r="V14" s="13">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B15" s="31"/>
+      <c r="B15" s="37"/>
       <c r="C15" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="12">
+      <c r="D15" s="10">
         <v>0</v>
       </c>
       <c r="E15" s="2">
@@ -3049,10 +4351,10 @@
       <c r="M15">
         <v>0</v>
       </c>
-      <c r="N15" s="22">
+      <c r="N15" s="20">
         <v>2</v>
       </c>
-      <c r="O15" s="22">
+      <c r="O15" s="20">
         <v>1</v>
       </c>
       <c r="P15">
@@ -3073,16 +4375,16 @@
       <c r="U15" s="2">
         <v>0</v>
       </c>
-      <c r="V15" s="15">
+      <c r="V15" s="13">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B16" s="29"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="13">
+      <c r="D16" s="11">
         <v>0</v>
       </c>
       <c r="E16" s="3">
@@ -3118,13 +4420,13 @@
       <c r="O16">
         <v>0</v>
       </c>
-      <c r="P16" s="23">
+      <c r="P16" s="21">
         <v>1</v>
       </c>
-      <c r="Q16" s="23">
+      <c r="Q16" s="21">
         <v>1</v>
       </c>
-      <c r="R16" s="23">
+      <c r="R16" s="21">
         <v>1</v>
       </c>
       <c r="S16" s="3">
@@ -3136,63 +4438,63 @@
       <c r="U16" s="3">
         <v>0</v>
       </c>
-      <c r="V16" s="16">
+      <c r="V16" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B17" s="28" t="s">
+      <c r="B17" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D17" s="11">
-        <v>0</v>
-      </c>
-      <c r="E17" s="10">
-        <v>0</v>
-      </c>
-      <c r="F17" s="10">
-        <v>0</v>
-      </c>
-      <c r="G17" s="10">
-        <v>0</v>
-      </c>
-      <c r="H17" s="10">
-        <v>0</v>
-      </c>
-      <c r="I17" s="10">
-        <v>0</v>
-      </c>
-      <c r="J17" s="10">
-        <v>0</v>
-      </c>
-      <c r="K17" s="10">
-        <v>0</v>
-      </c>
-      <c r="L17" s="10">
-        <v>0</v>
-      </c>
-      <c r="M17" s="10">
-        <v>0</v>
-      </c>
-      <c r="N17" s="10">
-        <v>0</v>
-      </c>
-      <c r="O17" s="10">
-        <v>0</v>
-      </c>
-      <c r="P17" s="10">
-        <v>0</v>
-      </c>
-      <c r="Q17" s="10">
-        <v>0</v>
-      </c>
-      <c r="R17" s="10">
-        <v>0</v>
-      </c>
-      <c r="S17" s="20">
+      <c r="D17" s="9">
+        <v>0</v>
+      </c>
+      <c r="E17" s="8">
+        <v>0</v>
+      </c>
+      <c r="F17" s="8">
+        <v>0</v>
+      </c>
+      <c r="G17" s="8">
+        <v>0</v>
+      </c>
+      <c r="H17" s="8">
+        <v>0</v>
+      </c>
+      <c r="I17" s="8">
+        <v>0</v>
+      </c>
+      <c r="J17" s="8">
+        <v>0</v>
+      </c>
+      <c r="K17" s="8">
+        <v>0</v>
+      </c>
+      <c r="L17" s="8">
+        <v>0</v>
+      </c>
+      <c r="M17" s="8">
+        <v>0</v>
+      </c>
+      <c r="N17" s="8">
+        <v>0</v>
+      </c>
+      <c r="O17" s="8">
+        <v>0</v>
+      </c>
+      <c r="P17" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="8">
+        <v>0</v>
+      </c>
+      <c r="R17" s="8">
+        <v>0</v>
+      </c>
+      <c r="S17" s="18">
         <v>0.5</v>
       </c>
       <c r="T17">
@@ -3206,11 +4508,11 @@
       </c>
     </row>
     <row r="18" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B18" s="31"/>
+      <c r="B18" s="37"/>
       <c r="C18" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="12">
+      <c r="D18" s="10">
         <v>0</v>
       </c>
       <c r="E18" s="2">
@@ -3255,7 +4557,7 @@
       <c r="R18" s="2">
         <v>0</v>
       </c>
-      <c r="S18" s="19">
+      <c r="S18" s="17">
         <v>0.5</v>
       </c>
       <c r="T18">
@@ -3269,11 +4571,11 @@
       </c>
     </row>
     <row r="19" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B19" s="29"/>
+      <c r="B19" s="35"/>
       <c r="C19" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="13">
+      <c r="D19" s="11">
         <v>0</v>
       </c>
       <c r="E19" s="3">
@@ -3321,7 +4623,7 @@
       <c r="S19" s="3">
         <v>0</v>
       </c>
-      <c r="T19" s="27">
+      <c r="T19" s="25">
         <v>1</v>
       </c>
       <c r="U19">
@@ -3332,55 +4634,55 @@
       </c>
     </row>
     <row r="20" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B20" s="28" t="s">
+      <c r="B20" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D20" s="11">
-        <v>0</v>
-      </c>
-      <c r="E20" s="10">
-        <v>0</v>
-      </c>
-      <c r="F20" s="10">
-        <v>0</v>
-      </c>
-      <c r="G20" s="10">
-        <v>0</v>
-      </c>
-      <c r="H20" s="10">
-        <v>0</v>
-      </c>
-      <c r="I20" s="10">
-        <v>0</v>
-      </c>
-      <c r="J20" s="10">
-        <v>0</v>
-      </c>
-      <c r="K20" s="10">
-        <v>0</v>
-      </c>
-      <c r="L20" s="10">
-        <v>0</v>
-      </c>
-      <c r="M20" s="10">
-        <v>0</v>
-      </c>
-      <c r="N20" s="10">
-        <v>0</v>
-      </c>
-      <c r="O20" s="10">
-        <v>0</v>
-      </c>
-      <c r="P20" s="10">
-        <v>0</v>
-      </c>
-      <c r="Q20" s="10">
-        <v>0</v>
-      </c>
-      <c r="R20" s="10">
+      <c r="D20" s="9">
+        <v>0</v>
+      </c>
+      <c r="E20" s="8">
+        <v>0</v>
+      </c>
+      <c r="F20" s="8">
+        <v>0</v>
+      </c>
+      <c r="G20" s="8">
+        <v>0</v>
+      </c>
+      <c r="H20" s="8">
+        <v>0</v>
+      </c>
+      <c r="I20" s="8">
+        <v>0</v>
+      </c>
+      <c r="J20" s="8">
+        <v>0</v>
+      </c>
+      <c r="K20" s="8">
+        <v>0</v>
+      </c>
+      <c r="L20" s="8">
+        <v>0</v>
+      </c>
+      <c r="M20" s="8">
+        <v>0</v>
+      </c>
+      <c r="N20" s="8">
+        <v>0</v>
+      </c>
+      <c r="O20" s="8">
+        <v>0</v>
+      </c>
+      <c r="P20" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="8">
+        <v>0</v>
+      </c>
+      <c r="R20" s="8">
         <v>0</v>
       </c>
       <c r="S20">
@@ -3389,7 +4691,7 @@
       <c r="T20">
         <v>0</v>
       </c>
-      <c r="U20" s="20">
+      <c r="U20" s="18">
         <v>0.5</v>
       </c>
       <c r="V20">
@@ -3397,11 +4699,11 @@
       </c>
     </row>
     <row r="21" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B21" s="29"/>
+      <c r="B21" s="35"/>
       <c r="C21" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D21" s="13">
+      <c r="D21" s="11">
         <v>0</v>
       </c>
       <c r="E21" s="3">
@@ -3452,7 +4754,7 @@
       <c r="T21" s="3">
         <v>0</v>
       </c>
-      <c r="U21" s="27">
+      <c r="U21" s="25">
         <v>0.5</v>
       </c>
       <c r="V21">
@@ -3460,55 +4762,55 @@
       </c>
     </row>
     <row r="22" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B22" s="28" t="s">
+      <c r="B22" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D22" s="11">
-        <v>0</v>
-      </c>
-      <c r="E22" s="10">
-        <v>0</v>
-      </c>
-      <c r="F22" s="10">
-        <v>0</v>
-      </c>
-      <c r="G22" s="10">
-        <v>0</v>
-      </c>
-      <c r="H22" s="10">
-        <v>0</v>
-      </c>
-      <c r="I22" s="10">
-        <v>0</v>
-      </c>
-      <c r="J22" s="10">
-        <v>0</v>
-      </c>
-      <c r="K22" s="10">
-        <v>0</v>
-      </c>
-      <c r="L22" s="10">
-        <v>0</v>
-      </c>
-      <c r="M22" s="10">
-        <v>0</v>
-      </c>
-      <c r="N22" s="10">
-        <v>0</v>
-      </c>
-      <c r="O22" s="10">
-        <v>0</v>
-      </c>
-      <c r="P22" s="10">
-        <v>0</v>
-      </c>
-      <c r="Q22" s="10">
-        <v>0</v>
-      </c>
-      <c r="R22" s="10">
+      <c r="D22" s="9">
+        <v>0</v>
+      </c>
+      <c r="E22" s="8">
+        <v>0</v>
+      </c>
+      <c r="F22" s="8">
+        <v>0</v>
+      </c>
+      <c r="G22" s="8">
+        <v>0</v>
+      </c>
+      <c r="H22" s="8">
+        <v>0</v>
+      </c>
+      <c r="I22" s="8">
+        <v>0</v>
+      </c>
+      <c r="J22" s="8">
+        <v>0</v>
+      </c>
+      <c r="K22" s="8">
+        <v>0</v>
+      </c>
+      <c r="L22" s="8">
+        <v>0</v>
+      </c>
+      <c r="M22" s="8">
+        <v>0</v>
+      </c>
+      <c r="N22" s="8">
+        <v>0</v>
+      </c>
+      <c r="O22" s="8">
+        <v>0</v>
+      </c>
+      <c r="P22" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="8">
+        <v>0</v>
+      </c>
+      <c r="R22" s="8">
         <v>0</v>
       </c>
       <c r="S22">
@@ -3520,16 +4822,16 @@
       <c r="U22">
         <v>0</v>
       </c>
-      <c r="V22" s="32">
+      <c r="V22" s="27">
         <v>0.5</v>
       </c>
     </row>
     <row r="23" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B23" s="29"/>
+      <c r="B23" s="35"/>
       <c r="C23" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D23" s="13">
+      <c r="D23" s="11">
         <v>0</v>
       </c>
       <c r="E23" s="3">
@@ -3583,83 +4885,83 @@
       <c r="U23">
         <v>0</v>
       </c>
-      <c r="V23" s="32">
+      <c r="V23" s="27">
         <v>0.5</v>
       </c>
     </row>
     <row r="24" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="D24" s="11">
+      <c r="D24" s="9">
         <v>23</v>
       </c>
-      <c r="E24" s="11">
+      <c r="E24" s="9">
         <f>D24-SUM(E4:E23)</f>
         <v>22</v>
       </c>
-      <c r="F24" s="11">
+      <c r="F24" s="9">
         <f>E24-SUM(F4:F23)</f>
         <v>21</v>
       </c>
-      <c r="G24" s="11">
+      <c r="G24" s="9">
         <f>F24-SUM(G4:G23)</f>
         <v>19</v>
       </c>
-      <c r="H24" s="11">
+      <c r="H24" s="9">
         <f t="shared" ref="H24:V24" si="0">G24-SUM(H4:H23)</f>
         <v>18</v>
       </c>
-      <c r="I24" s="11">
+      <c r="I24" s="9">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="J24" s="11">
+      <c r="J24" s="9">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="K24" s="11">
+      <c r="K24" s="9">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="L24" s="11">
+      <c r="L24" s="9">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="M24" s="11">
+      <c r="M24" s="9">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="N24" s="11">
+      <c r="N24" s="9">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="O24" s="11">
+      <c r="O24" s="9">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="P24" s="11">
+      <c r="P24" s="9">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="Q24" s="11">
+      <c r="Q24" s="9">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="R24" s="11">
+      <c r="R24" s="9">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="S24" s="11">
+      <c r="S24" s="9">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="T24" s="11">
+      <c r="T24" s="9">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="U24" s="11">
+      <c r="U24" s="9">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="V24" s="17">
+      <c r="V24" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3678,4 +4980,1042 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B40D316F-9AC3-40B6-9034-2229B798232F}">
+  <dimension ref="B2:AC24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="109.85546875" customWidth="1"/>
+    <col min="3" max="3" width="99.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="33"/>
+      <c r="P2" s="33"/>
+      <c r="Q2" s="33"/>
+      <c r="R2" s="33"/>
+      <c r="S2" s="33"/>
+      <c r="T2" s="33"/>
+      <c r="U2" s="33"/>
+      <c r="V2" s="38"/>
+      <c r="W2" s="38"/>
+      <c r="X2" s="38"/>
+      <c r="Y2" s="38"/>
+      <c r="Z2" s="38"/>
+      <c r="AA2" s="38"/>
+      <c r="AB2" s="38"/>
+      <c r="AC2" s="38"/>
+    </row>
+    <row r="3" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="5">
+        <v>44242</v>
+      </c>
+      <c r="E3" s="5">
+        <v>44243</v>
+      </c>
+      <c r="F3" s="5">
+        <v>44244</v>
+      </c>
+      <c r="G3" s="5">
+        <v>44245</v>
+      </c>
+      <c r="H3" s="5">
+        <v>44246</v>
+      </c>
+      <c r="I3" s="5">
+        <v>44247</v>
+      </c>
+      <c r="J3" s="5">
+        <v>44248</v>
+      </c>
+      <c r="K3" s="5">
+        <v>44249</v>
+      </c>
+      <c r="L3" s="5">
+        <v>44250</v>
+      </c>
+      <c r="M3" s="5">
+        <v>44251</v>
+      </c>
+      <c r="N3" s="5">
+        <v>44252</v>
+      </c>
+      <c r="O3" s="5">
+        <v>44253</v>
+      </c>
+      <c r="P3" s="5">
+        <v>44254</v>
+      </c>
+      <c r="Q3" s="5">
+        <v>44255</v>
+      </c>
+      <c r="R3" s="5">
+        <v>44256</v>
+      </c>
+      <c r="S3" s="5">
+        <v>44257</v>
+      </c>
+      <c r="T3" s="5">
+        <v>44258</v>
+      </c>
+      <c r="U3" s="5">
+        <v>44259</v>
+      </c>
+      <c r="V3" s="5">
+        <v>44260</v>
+      </c>
+      <c r="W3" s="5">
+        <v>44261</v>
+      </c>
+      <c r="X3" s="5">
+        <v>44262</v>
+      </c>
+      <c r="Y3" s="5">
+        <v>44263</v>
+      </c>
+      <c r="Z3" s="5">
+        <v>44264</v>
+      </c>
+      <c r="AA3" s="5">
+        <v>44265</v>
+      </c>
+      <c r="AB3" s="5">
+        <v>44266</v>
+      </c>
+      <c r="AC3" s="5">
+        <v>44267</v>
+      </c>
+    </row>
+    <row r="4" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B4" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D4" s="9"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
+      <c r="V4" s="12"/>
+      <c r="W4" s="12"/>
+      <c r="X4" s="12"/>
+      <c r="Y4" s="12"/>
+      <c r="Z4" s="12"/>
+      <c r="AA4" s="12"/>
+      <c r="AB4" s="12"/>
+      <c r="AC4" s="12"/>
+    </row>
+    <row r="5" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B5" s="37"/>
+      <c r="C5" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2"/>
+      <c r="V5" s="13"/>
+      <c r="W5" s="13"/>
+      <c r="X5" s="13"/>
+      <c r="Y5" s="13"/>
+      <c r="Z5" s="13"/>
+      <c r="AA5" s="13"/>
+      <c r="AB5" s="13"/>
+      <c r="AC5" s="13"/>
+    </row>
+    <row r="6" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B6" s="37"/>
+      <c r="C6" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="10"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+      <c r="U6" s="2"/>
+      <c r="V6" s="13"/>
+      <c r="W6" s="13"/>
+      <c r="X6" s="13"/>
+      <c r="Y6" s="13"/>
+      <c r="Z6" s="13"/>
+      <c r="AA6" s="13"/>
+      <c r="AB6" s="13"/>
+      <c r="AC6" s="13"/>
+    </row>
+    <row r="7" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B7" s="35"/>
+      <c r="C7" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="11"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="3"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="14"/>
+      <c r="W7" s="14"/>
+      <c r="X7" s="14"/>
+      <c r="Y7" s="14"/>
+      <c r="Z7" s="14"/>
+      <c r="AA7" s="14"/>
+      <c r="AB7" s="14"/>
+      <c r="AC7" s="14"/>
+    </row>
+    <row r="8" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B8" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="8"/>
+      <c r="Q8" s="8"/>
+      <c r="R8" s="8"/>
+      <c r="S8" s="8"/>
+      <c r="T8" s="8"/>
+      <c r="U8" s="8"/>
+      <c r="V8" s="12"/>
+      <c r="W8" s="12"/>
+      <c r="X8" s="12"/>
+      <c r="Y8" s="12"/>
+      <c r="Z8" s="12"/>
+      <c r="AA8" s="12"/>
+      <c r="AB8" s="12"/>
+      <c r="AC8" s="12"/>
+    </row>
+    <row r="9" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B9" s="37"/>
+      <c r="C9" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" s="10"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+      <c r="U9" s="2"/>
+      <c r="V9" s="13"/>
+      <c r="W9" s="13"/>
+      <c r="X9" s="13"/>
+      <c r="Y9" s="13"/>
+      <c r="Z9" s="13"/>
+      <c r="AA9" s="13"/>
+      <c r="AB9" s="13"/>
+      <c r="AC9" s="13"/>
+    </row>
+    <row r="10" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B10" s="37"/>
+      <c r="C10" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" s="10"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2"/>
+      <c r="T10" s="2"/>
+      <c r="U10" s="2"/>
+      <c r="V10" s="13"/>
+      <c r="W10" s="13"/>
+      <c r="X10" s="13"/>
+      <c r="Y10" s="13"/>
+      <c r="Z10" s="13"/>
+      <c r="AA10" s="13"/>
+      <c r="AB10" s="13"/>
+      <c r="AC10" s="13"/>
+    </row>
+    <row r="11" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B11" s="37"/>
+      <c r="C11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" s="10"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="2"/>
+      <c r="S11" s="2"/>
+      <c r="T11" s="2"/>
+      <c r="U11" s="2"/>
+      <c r="V11" s="13"/>
+      <c r="W11" s="13"/>
+      <c r="X11" s="13"/>
+      <c r="Y11" s="13"/>
+      <c r="Z11" s="13"/>
+      <c r="AA11" s="13"/>
+      <c r="AB11" s="13"/>
+      <c r="AC11" s="13"/>
+    </row>
+    <row r="12" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B12" s="35"/>
+      <c r="C12" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" s="11"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
+      <c r="S12" s="3"/>
+      <c r="T12" s="3"/>
+      <c r="U12" s="3"/>
+      <c r="V12" s="14"/>
+      <c r="W12" s="14"/>
+      <c r="X12" s="14"/>
+      <c r="Y12" s="14"/>
+      <c r="Z12" s="14"/>
+      <c r="AA12" s="14"/>
+      <c r="AB12" s="14"/>
+      <c r="AC12" s="14"/>
+    </row>
+    <row r="13" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B13" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" s="9"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="S13" s="8"/>
+      <c r="T13" s="8"/>
+      <c r="U13" s="8"/>
+      <c r="V13" s="12"/>
+      <c r="W13" s="12"/>
+      <c r="X13" s="12"/>
+      <c r="Y13" s="12"/>
+      <c r="Z13" s="12"/>
+      <c r="AA13" s="12"/>
+      <c r="AB13" s="12"/>
+      <c r="AC13" s="12"/>
+    </row>
+    <row r="14" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B14" s="37"/>
+      <c r="C14" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D14" s="10"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="S14" s="2"/>
+      <c r="T14" s="2"/>
+      <c r="U14" s="2"/>
+      <c r="V14" s="13"/>
+      <c r="W14" s="13"/>
+      <c r="X14" s="13"/>
+      <c r="Y14" s="13"/>
+      <c r="Z14" s="13"/>
+      <c r="AA14" s="13"/>
+      <c r="AB14" s="13"/>
+      <c r="AC14" s="13"/>
+    </row>
+    <row r="15" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B15" s="37"/>
+      <c r="C15" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" s="10"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="S15" s="2"/>
+      <c r="T15" s="2"/>
+      <c r="U15" s="2"/>
+      <c r="V15" s="13"/>
+      <c r="W15" s="13"/>
+      <c r="X15" s="13"/>
+      <c r="Y15" s="13"/>
+      <c r="Z15" s="13"/>
+      <c r="AA15" s="13"/>
+      <c r="AB15" s="13"/>
+      <c r="AC15" s="13"/>
+    </row>
+    <row r="16" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B16" s="37"/>
+      <c r="C16" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D16" s="10"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="S16" s="2"/>
+      <c r="T16" s="2"/>
+      <c r="U16" s="2"/>
+      <c r="V16" s="13"/>
+      <c r="W16" s="13"/>
+      <c r="X16" s="13"/>
+      <c r="Y16" s="13"/>
+      <c r="Z16" s="13"/>
+      <c r="AA16" s="13"/>
+      <c r="AB16" s="13"/>
+      <c r="AC16" s="13"/>
+    </row>
+    <row r="17" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B17" s="8"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="9">
+        <f>26 - SUM(D4:D16)</f>
+        <v>26</v>
+      </c>
+      <c r="E17" s="9">
+        <f>D17-SUM(E4:E16)</f>
+        <v>26</v>
+      </c>
+      <c r="F17" s="9">
+        <f t="shared" ref="F17:V17" si="0">E17-SUM(F4:F16)</f>
+        <v>26</v>
+      </c>
+      <c r="G17" s="9">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="H17" s="9">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="I17" s="9">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="J17" s="9">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="K17" s="9">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="L17" s="9">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="M17" s="9">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="N17" s="9">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="O17" s="9">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="P17" s="9">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="Q17" s="9">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="R17" s="9">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="S17" s="9">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="T17" s="9">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="U17" s="9">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="V17" s="15">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="W17" s="15">
+        <f t="shared" ref="W17" si="1">V17-SUM(W4:W16)</f>
+        <v>26</v>
+      </c>
+      <c r="X17" s="15">
+        <f t="shared" ref="X17" si="2">W17-SUM(X4:X16)</f>
+        <v>26</v>
+      </c>
+      <c r="Y17" s="15">
+        <f t="shared" ref="Y17" si="3">X17-SUM(Y4:Y16)</f>
+        <v>26</v>
+      </c>
+      <c r="Z17" s="15">
+        <f t="shared" ref="Z17" si="4">Y17-SUM(Z4:Z16)</f>
+        <v>26</v>
+      </c>
+      <c r="AA17" s="15">
+        <f t="shared" ref="AA17" si="5">Z17-SUM(AA4:AA16)</f>
+        <v>26</v>
+      </c>
+      <c r="AB17" s="15">
+        <f t="shared" ref="AB17" si="6">AA17-SUM(AB4:AB16)</f>
+        <v>26</v>
+      </c>
+      <c r="AC17" s="15">
+        <f t="shared" ref="AC17" si="7">AB17-SUM(AC4:AC16)</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B18" s="26"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
+      <c r="R18" s="2"/>
+      <c r="S18" s="2"/>
+      <c r="T18" s="2"/>
+      <c r="U18" s="2"/>
+      <c r="V18" s="2"/>
+    </row>
+    <row r="19" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B19" s="26"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="2"/>
+      <c r="R19" s="2"/>
+      <c r="S19" s="2"/>
+      <c r="T19" s="2"/>
+      <c r="U19" s="2"/>
+      <c r="V19" s="2"/>
+    </row>
+    <row r="20" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B20" s="26"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
+      <c r="Q20" s="2"/>
+      <c r="R20" s="2"/>
+      <c r="S20" s="2"/>
+      <c r="T20" s="2"/>
+      <c r="U20" s="2"/>
+      <c r="V20" s="2"/>
+    </row>
+    <row r="21" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B21" s="26"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
+      <c r="Q21" s="2"/>
+      <c r="R21" s="2"/>
+      <c r="S21" s="2"/>
+      <c r="T21" s="2"/>
+      <c r="U21" s="2"/>
+      <c r="V21" s="2"/>
+    </row>
+    <row r="22" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B22" s="26"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="2"/>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="2"/>
+      <c r="R22" s="2"/>
+      <c r="S22" s="2"/>
+      <c r="T22" s="2"/>
+      <c r="U22" s="2"/>
+      <c r="V22" s="2"/>
+    </row>
+    <row r="23" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B23" s="26"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="2"/>
+      <c r="R23" s="2"/>
+      <c r="S23" s="2"/>
+      <c r="T23" s="2"/>
+      <c r="U23" s="2"/>
+      <c r="V23" s="2"/>
+    </row>
+    <row r="24" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
+      <c r="Q24" s="2"/>
+      <c r="R24" s="2"/>
+      <c r="S24" s="2"/>
+      <c r="T24" s="2"/>
+      <c r="U24" s="2"/>
+      <c r="V24" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="B8:B12"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="V2:AC2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010007C60AE6480C8D49900E7A4362DC978A" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2c8c8df2ae4c8b52ea756b3d40f22f1c">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="40d8dcd0-4b95-4e4d-9aa5-be2e8658acc5" xmlns:ns4="3244cbb2-9f52-4273-9113-8cc2cecf4979" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="54d9cecd5b552591da97f0387668823e" ns3:_="" ns4:_="">
+    <xsd:import namespace="40d8dcd0-4b95-4e4d-9aa5-be2e8658acc5"/>
+    <xsd:import namespace="3244cbb2-9f52-4273-9113-8cc2cecf4979"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns3:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns4:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns4:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns4:SharingHintHash" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="40d8dcd0-4b95-4e4d-9aa5-be2e8658acc5" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="10" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="11" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="12" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="13" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="14" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="15" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="16" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="17" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="3244cbb2-9f52-4273-9113-8cc2cecf4979" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="18" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="19" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="SharingHintHash" ma:index="20" nillable="true" ma:displayName="Sharing Hint Hash" ma:hidden="true" ma:internalName="SharingHintHash" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{308378B9-91A3-4988-8873-F75977EABA14}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="40d8dcd0-4b95-4e4d-9aa5-be2e8658acc5"/>
+    <ds:schemaRef ds:uri="3244cbb2-9f52-4273-9113-8cc2cecf4979"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B975CF3D-B020-4216-8822-B9E8F3D97495}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA34204B-E607-45A1-9498-394427B9D986}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="3244cbb2-9f52-4273-9113-8cc2cecf4979"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="40d8dcd0-4b95-4e4d-9aa5-be2e8658acc5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update: Scrum Documentation Sprint 2 corrected
</commit_message>
<xml_diff>
--- a/Group C2-3 Scrum documentation.xlsx
+++ b/Group C2-3 Scrum documentation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johna\OneDrive\Documents\University\Year II\CO553 Agile Development and Software Security B\co553-c2-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AF0A7555-A1B7-4946-8409-67A4A43647BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94F30CF8-4E7B-4C6A-8FCB-70618F6A6639}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{0CC9FE5D-919A-41CA-B32D-5FFC3808111C}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="67">
   <si>
     <t>ID</t>
   </si>
@@ -277,6 +277,9 @@
   </si>
   <si>
     <t>Display 'sold out' if no tickets are available [1] [Kezia]</t>
+  </si>
+  <si>
+    <t>Sprint duration (15/02 - 12/03)</t>
   </si>
 </sst>
 </file>
@@ -4987,7 +4990,7 @@
   <dimension ref="B2:AC24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5004,7 +5007,7 @@
         <v>21</v>
       </c>
       <c r="D2" s="33" t="s">
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="E2" s="33"/>
       <c r="F2" s="33"/>
@@ -5739,6 +5742,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010007C60AE6480C8D49900E7A4362DC978A" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2c8c8df2ae4c8b52ea756b3d40f22f1c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="40d8dcd0-4b95-4e4d-9aa5-be2e8658acc5" xmlns:ns4="3244cbb2-9f52-4273-9113-8cc2cecf4979" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="54d9cecd5b552591da97f0387668823e" ns3:_="" ns4:_="">
     <xsd:import namespace="40d8dcd0-4b95-4e4d-9aa5-be2e8658acc5"/>
@@ -5961,22 +5979,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA34204B-E607-45A1-9498-394427B9D986}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="3244cbb2-9f52-4273-9113-8cc2cecf4979"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="40d8dcd0-4b95-4e4d-9aa5-be2e8658acc5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B975CF3D-B020-4216-8822-B9E8F3D97495}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{308378B9-91A3-4988-8873-F75977EABA14}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5993,29 +6021,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B975CF3D-B020-4216-8822-B9E8F3D97495}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA34204B-E607-45A1-9498-394427B9D986}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="3244cbb2-9f52-4273-9113-8cc2cecf4979"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="40d8dcd0-4b95-4e4d-9aa5-be2e8658acc5"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update: Product backlog correction
</commit_message>
<xml_diff>
--- a/Group C2-3 Scrum documentation.xlsx
+++ b/Group C2-3 Scrum documentation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johna\OneDrive\Documents\University\Year II\CO553 Agile Development and Software Security B\co553-c2-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E591A64A-E5AC-491D-B451-0A15C6561457}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{088E9576-80B0-4D9B-BD66-691305D09DB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{0CC9FE5D-919A-41CA-B32D-5FFC3808111C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0CC9FE5D-919A-41CA-B32D-5FFC3808111C}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -358,7 +358,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -397,8 +397,14 @@
         <fgColor rgb="FFFFCC99"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="15">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -502,17 +508,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -570,9 +565,9 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -592,42 +587,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="10" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="12" xfId="4" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="12" xfId="4"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -640,10 +618,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -653,17 +639,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -3358,8 +3347,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F2ABAF1-62E6-41B4-BC47-CFBA7BD3B611}">
   <dimension ref="B2:D21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3379,200 +3368,200 @@
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="22">
+      <c r="B3" s="46">
         <v>1</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="22">
+      <c r="D3" s="46">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="23">
+      <c r="B4" s="46">
         <v>2</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="23">
+      <c r="D4" s="46">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="28">
+      <c r="B5" s="46">
         <v>3</v>
       </c>
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="28">
+      <c r="D5" s="46">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="23">
+      <c r="B6" s="46">
         <v>4</v>
       </c>
-      <c r="C6" s="24" t="s">
+      <c r="C6" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="23">
+      <c r="D6" s="46">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="23">
+      <c r="B7" s="46">
         <v>5</v>
       </c>
-      <c r="C7" s="23" t="s">
+      <c r="C7" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="23">
+      <c r="D7" s="46">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="23">
+      <c r="B8" s="46">
         <v>6</v>
       </c>
-      <c r="C8" s="23" t="s">
+      <c r="C8" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="23">
+      <c r="D8" s="46">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="28">
+      <c r="B9" s="41">
         <v>7</v>
       </c>
-      <c r="C9" s="28" t="s">
+      <c r="C9" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="28">
+      <c r="D9" s="41">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="28">
+      <c r="B10" s="41">
         <v>8</v>
       </c>
-      <c r="C10" s="28" t="s">
+      <c r="C10" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="28">
+      <c r="D10" s="41">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="29">
+      <c r="B11" s="42">
         <v>9</v>
       </c>
-      <c r="C11" s="29" t="s">
+      <c r="C11" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="29">
+      <c r="D11" s="42">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="29">
+      <c r="B12" s="42">
         <v>10</v>
       </c>
-      <c r="C12" s="29" t="s">
+      <c r="C12" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="29">
+      <c r="D12" s="42">
         <v>3</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="29">
+      <c r="B13" s="42">
         <v>11</v>
       </c>
-      <c r="C13" s="29" t="s">
+      <c r="C13" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="29">
+      <c r="D13" s="42">
         <v>2</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="29">
+      <c r="B14" s="42">
         <v>12</v>
       </c>
-      <c r="C14" s="29" t="s">
+      <c r="C14" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="29">
+      <c r="D14" s="42">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="29">
+      <c r="B15" s="42">
         <v>13</v>
       </c>
-      <c r="C15" s="32" t="s">
+      <c r="C15" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="29">
+      <c r="D15" s="42">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="29">
+      <c r="B16" s="42">
         <v>14</v>
       </c>
-      <c r="C16" s="32" t="s">
+      <c r="C16" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="29">
+      <c r="D16" s="42">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="30">
+      <c r="B17" s="44">
         <v>15</v>
       </c>
-      <c r="C17" s="31" t="s">
+      <c r="C17" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="30">
+      <c r="D17" s="44">
         <v>3</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="29">
+      <c r="B18" s="42">
         <v>16</v>
       </c>
-      <c r="C18" s="32" t="s">
+      <c r="C18" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="29">
+      <c r="D18" s="42">
         <v>5</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="30">
+      <c r="B19" s="44">
         <v>17</v>
       </c>
-      <c r="C19" s="31" t="s">
+      <c r="C19" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="30">
+      <c r="D19" s="44">
         <v>2</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="30">
+      <c r="B20" s="44">
         <v>18</v>
       </c>
-      <c r="C20" s="31" t="s">
+      <c r="C20" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="D20" s="30">
+      <c r="D20" s="44">
         <v>1</v>
       </c>
     </row>
@@ -3606,27 +3595,27 @@
       <c r="C2" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="37" t="s">
+      <c r="D2" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37"/>
-      <c r="O2" s="37"/>
-      <c r="P2" s="37"/>
-      <c r="Q2" s="37"/>
-      <c r="R2" s="37"/>
-      <c r="S2" s="37"/>
-      <c r="T2" s="37"/>
-      <c r="U2" s="37"/>
-      <c r="V2" s="37"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="32"/>
+      <c r="R2" s="32"/>
+      <c r="S2" s="32"/>
+      <c r="T2" s="32"/>
+      <c r="U2" s="32"/>
+      <c r="V2" s="32"/>
     </row>
     <row r="3" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B3" s="16"/>
@@ -3690,7 +3679,7 @@
       </c>
     </row>
     <row r="4" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="30" t="s">
         <v>22</v>
       </c>
       <c r="C4" s="6" t="s">
@@ -3755,7 +3744,7 @@
       </c>
     </row>
     <row r="5" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B5" s="38"/>
+      <c r="B5" s="33"/>
       <c r="C5" s="6" t="s">
         <v>47</v>
       </c>
@@ -3818,7 +3807,7 @@
       </c>
     </row>
     <row r="6" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B6" s="38"/>
+      <c r="B6" s="33"/>
       <c r="C6" s="2" t="s">
         <v>46</v>
       </c>
@@ -3881,14 +3870,14 @@
       </c>
     </row>
     <row r="7" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B7" s="36"/>
+      <c r="B7" s="31"/>
       <c r="C7" s="3" t="s">
         <v>45</v>
       </c>
       <c r="D7" s="11">
         <v>0</v>
       </c>
-      <c r="E7" s="25">
+      <c r="E7" s="22">
         <v>0.25</v>
       </c>
       <c r="F7">
@@ -3944,7 +3933,7 @@
       </c>
     </row>
     <row r="8" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B8" s="35" t="s">
+      <c r="B8" s="30" t="s">
         <v>23</v>
       </c>
       <c r="C8" s="8" t="s">
@@ -4009,7 +3998,7 @@
       </c>
     </row>
     <row r="9" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B9" s="38"/>
+      <c r="B9" s="33"/>
       <c r="C9" s="2" t="s">
         <v>30</v>
       </c>
@@ -4072,7 +4061,7 @@
       </c>
     </row>
     <row r="10" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B10" s="38"/>
+      <c r="B10" s="33"/>
       <c r="C10" s="2" t="s">
         <v>31</v>
       </c>
@@ -4135,7 +4124,7 @@
       </c>
     </row>
     <row r="11" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B11" s="38"/>
+      <c r="B11" s="33"/>
       <c r="C11" s="2" t="s">
         <v>32</v>
       </c>
@@ -4198,7 +4187,7 @@
       </c>
     </row>
     <row r="12" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B12" s="36"/>
+      <c r="B12" s="31"/>
       <c r="C12" s="3" t="s">
         <v>33</v>
       </c>
@@ -4220,7 +4209,7 @@
       <c r="I12">
         <v>0</v>
       </c>
-      <c r="J12" s="25">
+      <c r="J12" s="22">
         <v>2</v>
       </c>
       <c r="K12" s="3">
@@ -4261,7 +4250,7 @@
       </c>
     </row>
     <row r="13" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B13" s="35" t="s">
+      <c r="B13" s="30" t="s">
         <v>24</v>
       </c>
       <c r="C13" s="8" t="s">
@@ -4326,7 +4315,7 @@
       </c>
     </row>
     <row r="14" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B14" s="38"/>
+      <c r="B14" s="33"/>
       <c r="C14" s="2" t="s">
         <v>35</v>
       </c>
@@ -4389,7 +4378,7 @@
       </c>
     </row>
     <row r="15" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B15" s="38"/>
+      <c r="B15" s="33"/>
       <c r="C15" s="2" t="s">
         <v>36</v>
       </c>
@@ -4452,7 +4441,7 @@
       </c>
     </row>
     <row r="16" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B16" s="36"/>
+      <c r="B16" s="31"/>
       <c r="C16" s="3" t="s">
         <v>37</v>
       </c>
@@ -4515,7 +4504,7 @@
       </c>
     </row>
     <row r="17" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B17" s="35" t="s">
+      <c r="B17" s="30" t="s">
         <v>26</v>
       </c>
       <c r="C17" s="8" t="s">
@@ -4580,7 +4569,7 @@
       </c>
     </row>
     <row r="18" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B18" s="38"/>
+      <c r="B18" s="33"/>
       <c r="C18" s="2" t="s">
         <v>38</v>
       </c>
@@ -4643,7 +4632,7 @@
       </c>
     </row>
     <row r="19" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B19" s="36"/>
+      <c r="B19" s="31"/>
       <c r="C19" s="3" t="s">
         <v>39</v>
       </c>
@@ -4695,7 +4684,7 @@
       <c r="S19" s="3">
         <v>0</v>
       </c>
-      <c r="T19" s="25">
+      <c r="T19" s="22">
         <v>1</v>
       </c>
       <c r="U19">
@@ -4706,7 +4695,7 @@
       </c>
     </row>
     <row r="20" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B20" s="35" t="s">
+      <c r="B20" s="30" t="s">
         <v>27</v>
       </c>
       <c r="C20" s="8" t="s">
@@ -4771,7 +4760,7 @@
       </c>
     </row>
     <row r="21" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B21" s="36"/>
+      <c r="B21" s="31"/>
       <c r="C21" s="3" t="s">
         <v>41</v>
       </c>
@@ -4826,7 +4815,7 @@
       <c r="T21" s="3">
         <v>0</v>
       </c>
-      <c r="U21" s="25">
+      <c r="U21" s="22">
         <v>0.5</v>
       </c>
       <c r="V21">
@@ -4834,7 +4823,7 @@
       </c>
     </row>
     <row r="22" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B22" s="35" t="s">
+      <c r="B22" s="30" t="s">
         <v>28</v>
       </c>
       <c r="C22" s="8" t="s">
@@ -4894,12 +4883,12 @@
       <c r="U22">
         <v>0</v>
       </c>
-      <c r="V22" s="27">
+      <c r="V22" s="24">
         <v>0.5</v>
       </c>
     </row>
     <row r="23" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B23" s="36"/>
+      <c r="B23" s="31"/>
       <c r="C23" s="3" t="s">
         <v>43</v>
       </c>
@@ -4957,7 +4946,7 @@
       <c r="U23">
         <v>0</v>
       </c>
-      <c r="V23" s="27">
+      <c r="V23" s="24">
         <v>0.5</v>
       </c>
     </row>
@@ -5058,7 +5047,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B40D316F-9AC3-40B6-9034-2229B798232F}">
   <dimension ref="B2:AE24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
@@ -5083,34 +5072,34 @@
       <c r="E2" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="F2" s="33" t="s">
+      <c r="F2" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
-      <c r="O2" s="33"/>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="33"/>
-      <c r="R2" s="33"/>
-      <c r="S2" s="33"/>
-      <c r="T2" s="33"/>
-      <c r="U2" s="33"/>
-      <c r="V2" s="33"/>
-      <c r="W2" s="33"/>
-      <c r="X2" s="39"/>
-      <c r="Y2" s="39"/>
-      <c r="Z2" s="39"/>
-      <c r="AA2" s="39"/>
-      <c r="AB2" s="39"/>
-      <c r="AC2" s="39"/>
-      <c r="AD2" s="39"/>
-      <c r="AE2" s="39"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="25"/>
+      <c r="N2" s="25"/>
+      <c r="O2" s="25"/>
+      <c r="P2" s="25"/>
+      <c r="Q2" s="25"/>
+      <c r="R2" s="25"/>
+      <c r="S2" s="25"/>
+      <c r="T2" s="25"/>
+      <c r="U2" s="25"/>
+      <c r="V2" s="25"/>
+      <c r="W2" s="25"/>
+      <c r="X2" s="37"/>
+      <c r="Y2" s="37"/>
+      <c r="Z2" s="37"/>
+      <c r="AA2" s="37"/>
+      <c r="AB2" s="37"/>
+      <c r="AC2" s="37"/>
+      <c r="AD2" s="37"/>
+      <c r="AE2" s="37"/>
     </row>
     <row r="3" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B3" s="16"/>
@@ -5197,10 +5186,10 @@
       </c>
     </row>
     <row r="4" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B4" s="44" t="s">
+      <c r="B4" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="41">
+      <c r="C4" s="38">
         <v>10</v>
       </c>
       <c r="D4" s="15" t="s">
@@ -5231,9 +5220,9 @@
       <c r="AE4" s="12"/>
     </row>
     <row r="5" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B5" s="45"/>
-      <c r="C5" s="42"/>
-      <c r="D5" s="47" t="s">
+      <c r="B5" s="35"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="28" t="s">
         <v>62</v>
       </c>
       <c r="E5" s="2" t="s">
@@ -5261,12 +5250,12 @@
       <c r="AE5" s="13"/>
     </row>
     <row r="6" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B6" s="45"/>
-      <c r="C6" s="42"/>
-      <c r="D6" s="47" t="s">
+      <c r="B6" s="35"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="E6" s="40" t="s">
+      <c r="E6" s="27" t="s">
         <v>57</v>
       </c>
       <c r="F6" s="10"/>
@@ -5291,9 +5280,9 @@
       <c r="AE6" s="13"/>
     </row>
     <row r="7" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B7" s="46"/>
-      <c r="C7" s="43"/>
-      <c r="D7" s="48" t="s">
+      <c r="B7" s="36"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="29" t="s">
         <v>64</v>
       </c>
       <c r="E7" s="3" t="s">
@@ -5327,10 +5316,10 @@
       <c r="AE7" s="14"/>
     </row>
     <row r="8" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B8" s="44" t="s">
+      <c r="B8" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="C8" s="41">
+      <c r="C8" s="38">
         <v>10</v>
       </c>
       <c r="D8" s="15" t="s">
@@ -5361,12 +5350,12 @@
       <c r="AE8" s="12"/>
     </row>
     <row r="9" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B9" s="45"/>
-      <c r="C9" s="42"/>
-      <c r="D9" s="47" t="s">
+      <c r="B9" s="35"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="E9" s="40" t="s">
+      <c r="E9" s="27" t="s">
         <v>55</v>
       </c>
       <c r="F9" s="10"/>
@@ -5391,12 +5380,12 @@
       <c r="AE9" s="13"/>
     </row>
     <row r="10" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B10" s="45"/>
-      <c r="C10" s="42"/>
-      <c r="D10" s="47" t="s">
+      <c r="B10" s="35"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="E10" s="40" t="s">
+      <c r="E10" s="27" t="s">
         <v>59</v>
       </c>
       <c r="F10" s="10"/>
@@ -5421,12 +5410,12 @@
       <c r="AE10" s="13"/>
     </row>
     <row r="11" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B11" s="45"/>
-      <c r="C11" s="42"/>
-      <c r="D11" s="47" t="s">
+      <c r="B11" s="35"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="E11" s="40" t="s">
+      <c r="E11" s="27" t="s">
         <v>56</v>
       </c>
       <c r="F11" s="10"/>
@@ -5451,9 +5440,9 @@
       <c r="AE11" s="13"/>
     </row>
     <row r="12" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B12" s="46"/>
-      <c r="C12" s="43"/>
-      <c r="D12" s="48" t="s">
+      <c r="B12" s="36"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="29" t="s">
         <v>69</v>
       </c>
       <c r="E12" s="3" t="s">
@@ -5481,10 +5470,10 @@
       <c r="AE12" s="14"/>
     </row>
     <row r="13" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B13" s="44" t="s">
+      <c r="B13" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="C13" s="41">
+      <c r="C13" s="38">
         <v>6</v>
       </c>
       <c r="D13" s="15" t="s">
@@ -5513,12 +5502,12 @@
       <c r="AE13" s="12"/>
     </row>
     <row r="14" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B14" s="45"/>
-      <c r="C14" s="42"/>
-      <c r="D14" s="47" t="s">
+      <c r="B14" s="35"/>
+      <c r="C14" s="39"/>
+      <c r="D14" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="E14" s="40" t="s">
+      <c r="E14" s="27" t="s">
         <v>60</v>
       </c>
       <c r="F14" s="10"/>
@@ -5541,12 +5530,12 @@
       <c r="AE14" s="13"/>
     </row>
     <row r="15" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B15" s="45"/>
-      <c r="C15" s="42"/>
-      <c r="D15" s="47" t="s">
+      <c r="B15" s="35"/>
+      <c r="C15" s="39"/>
+      <c r="D15" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="E15" s="40" t="s">
+      <c r="E15" s="27" t="s">
         <v>57</v>
       </c>
       <c r="F15" s="10"/>
@@ -5569,12 +5558,12 @@
       <c r="AE15" s="13"/>
     </row>
     <row r="16" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B16" s="46"/>
-      <c r="C16" s="43"/>
-      <c r="D16" s="48" t="s">
+      <c r="B16" s="36"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="E16" s="40" t="s">
+      <c r="E16" s="27" t="s">
         <v>58</v>
       </c>
       <c r="F16" s="10"/>
@@ -5707,8 +5696,8 @@
       </c>
     </row>
     <row r="18" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B18" s="26"/>
-      <c r="C18" s="34"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="26"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
@@ -5732,8 +5721,8 @@
       <c r="X18" s="2"/>
     </row>
     <row r="19" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B19" s="26"/>
-      <c r="C19" s="34"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="26"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
@@ -5757,8 +5746,8 @@
       <c r="X19" s="2"/>
     </row>
     <row r="20" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B20" s="26"/>
-      <c r="C20" s="34"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="26"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
@@ -5782,8 +5771,8 @@
       <c r="X20" s="2"/>
     </row>
     <row r="21" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B21" s="26"/>
-      <c r="C21" s="34"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="26"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
@@ -5807,8 +5796,8 @@
       <c r="X21" s="2"/>
     </row>
     <row r="22" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B22" s="26"/>
-      <c r="C22" s="34"/>
+      <c r="B22" s="23"/>
+      <c r="C22" s="26"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
@@ -5832,8 +5821,8 @@
       <c r="X22" s="2"/>
     </row>
     <row r="23" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B23" s="26"/>
-      <c r="C23" s="34"/>
+      <c r="B23" s="23"/>
+      <c r="C23" s="26"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
@@ -5898,6 +5887,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010007C60AE6480C8D49900E7A4362DC978A" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2c8c8df2ae4c8b52ea756b3d40f22f1c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="40d8dcd0-4b95-4e4d-9aa5-be2e8658acc5" xmlns:ns4="3244cbb2-9f52-4273-9113-8cc2cecf4979" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="54d9cecd5b552591da97f0387668823e" ns3:_="" ns4:_="">
     <xsd:import namespace="40d8dcd0-4b95-4e4d-9aa5-be2e8658acc5"/>
@@ -6120,22 +6124,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA34204B-E607-45A1-9498-394427B9D986}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="3244cbb2-9f52-4273-9113-8cc2cecf4979"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="40d8dcd0-4b95-4e4d-9aa5-be2e8658acc5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B975CF3D-B020-4216-8822-B9E8F3D97495}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{308378B9-91A3-4988-8873-F75977EABA14}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6152,29 +6166,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B975CF3D-B020-4216-8822-B9E8F3D97495}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA34204B-E607-45A1-9498-394427B9D986}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="3244cbb2-9f52-4273-9113-8cc2cecf4979"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="40d8dcd0-4b95-4e4d-9aa5-be2e8658acc5"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update: Revised Burndown chart
</commit_message>
<xml_diff>
--- a/Group C2-3 Scrum documentation.xlsx
+++ b/Group C2-3 Scrum documentation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johna\OneDrive\Documents\University\Year II\CO553 Agile Development and Software Security B\co553-c2-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{088E9576-80B0-4D9B-BD66-691305D09DB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18FA5D80-670D-4336-8E68-DCE011F037B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0CC9FE5D-919A-41CA-B32D-5FFC3808111C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{0CC9FE5D-919A-41CA-B32D-5FFC3808111C}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -606,6 +606,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -638,20 +652,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1427,79 +1427,79 @@
                   <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>26</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>26</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>26</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>26</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>26</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>26</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>26</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>26</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>26</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>26</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>26</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>26</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>26</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>26</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>26</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>26</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>26</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>26</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>26</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>26</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>26</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>26</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>26</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>26</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>26</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3347,7 +3347,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F2ABAF1-62E6-41B4-BC47-CFBA7BD3B611}">
   <dimension ref="B2:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
@@ -3368,200 +3368,200 @@
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="46">
+      <c r="B3" s="35">
         <v>1</v>
       </c>
-      <c r="C3" s="46" t="s">
+      <c r="C3" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="46">
+      <c r="D3" s="35">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="46">
+      <c r="B4" s="35">
         <v>2</v>
       </c>
-      <c r="C4" s="46" t="s">
+      <c r="C4" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="46">
+      <c r="D4" s="35">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="46">
+      <c r="B5" s="35">
         <v>3</v>
       </c>
-      <c r="C5" s="46" t="s">
+      <c r="C5" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="46">
+      <c r="D5" s="35">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="46">
+      <c r="B6" s="35">
         <v>4</v>
       </c>
-      <c r="C6" s="46" t="s">
+      <c r="C6" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="46">
+      <c r="D6" s="35">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="46">
+      <c r="B7" s="35">
         <v>5</v>
       </c>
-      <c r="C7" s="46" t="s">
+      <c r="C7" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="46">
+      <c r="D7" s="35">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="46">
+      <c r="B8" s="35">
         <v>6</v>
       </c>
-      <c r="C8" s="46" t="s">
+      <c r="C8" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="46">
+      <c r="D8" s="35">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="41">
+      <c r="B9" s="30">
         <v>7</v>
       </c>
-      <c r="C9" s="41" t="s">
+      <c r="C9" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="41">
+      <c r="D9" s="30">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="41">
+      <c r="B10" s="30">
         <v>8</v>
       </c>
-      <c r="C10" s="41" t="s">
+      <c r="C10" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="41">
+      <c r="D10" s="30">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="42">
+      <c r="B11" s="31">
         <v>9</v>
       </c>
-      <c r="C11" s="42" t="s">
+      <c r="C11" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="42">
+      <c r="D11" s="31">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="42">
+      <c r="B12" s="31">
         <v>10</v>
       </c>
-      <c r="C12" s="42" t="s">
+      <c r="C12" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="42">
+      <c r="D12" s="31">
         <v>3</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="42">
+      <c r="B13" s="31">
         <v>11</v>
       </c>
-      <c r="C13" s="42" t="s">
+      <c r="C13" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="42">
+      <c r="D13" s="31">
         <v>2</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="42">
+      <c r="B14" s="31">
         <v>12</v>
       </c>
-      <c r="C14" s="42" t="s">
+      <c r="C14" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="42">
+      <c r="D14" s="31">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="42">
+      <c r="B15" s="31">
         <v>13</v>
       </c>
-      <c r="C15" s="43" t="s">
+      <c r="C15" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="42">
+      <c r="D15" s="31">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="42">
+      <c r="B16" s="31">
         <v>14</v>
       </c>
-      <c r="C16" s="43" t="s">
+      <c r="C16" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="42">
+      <c r="D16" s="31">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="44">
+      <c r="B17" s="33">
         <v>15</v>
       </c>
-      <c r="C17" s="45" t="s">
+      <c r="C17" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="44">
+      <c r="D17" s="33">
         <v>3</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="42">
+      <c r="B18" s="31">
         <v>16</v>
       </c>
-      <c r="C18" s="43" t="s">
+      <c r="C18" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="42">
+      <c r="D18" s="31">
         <v>5</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="44">
+      <c r="B19" s="33">
         <v>17</v>
       </c>
-      <c r="C19" s="45" t="s">
+      <c r="C19" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="44">
+      <c r="D19" s="33">
         <v>2</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="44">
+      <c r="B20" s="33">
         <v>18</v>
       </c>
-      <c r="C20" s="45" t="s">
+      <c r="C20" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="D20" s="44">
+      <c r="D20" s="33">
         <v>1</v>
       </c>
     </row>
@@ -3595,27 +3595,27 @@
       <c r="C2" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="32" t="s">
+      <c r="D2" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="32"/>
-      <c r="O2" s="32"/>
-      <c r="P2" s="32"/>
-      <c r="Q2" s="32"/>
-      <c r="R2" s="32"/>
-      <c r="S2" s="32"/>
-      <c r="T2" s="32"/>
-      <c r="U2" s="32"/>
-      <c r="V2" s="32"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="38"/>
+      <c r="P2" s="38"/>
+      <c r="Q2" s="38"/>
+      <c r="R2" s="38"/>
+      <c r="S2" s="38"/>
+      <c r="T2" s="38"/>
+      <c r="U2" s="38"/>
+      <c r="V2" s="38"/>
     </row>
     <row r="3" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B3" s="16"/>
@@ -3679,7 +3679,7 @@
       </c>
     </row>
     <row r="4" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="36" t="s">
         <v>22</v>
       </c>
       <c r="C4" s="6" t="s">
@@ -3744,7 +3744,7 @@
       </c>
     </row>
     <row r="5" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B5" s="33"/>
+      <c r="B5" s="39"/>
       <c r="C5" s="6" t="s">
         <v>47</v>
       </c>
@@ -3807,7 +3807,7 @@
       </c>
     </row>
     <row r="6" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B6" s="33"/>
+      <c r="B6" s="39"/>
       <c r="C6" s="2" t="s">
         <v>46</v>
       </c>
@@ -3870,7 +3870,7 @@
       </c>
     </row>
     <row r="7" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B7" s="31"/>
+      <c r="B7" s="37"/>
       <c r="C7" s="3" t="s">
         <v>45</v>
       </c>
@@ -3933,7 +3933,7 @@
       </c>
     </row>
     <row r="8" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="36" t="s">
         <v>23</v>
       </c>
       <c r="C8" s="8" t="s">
@@ -3998,7 +3998,7 @@
       </c>
     </row>
     <row r="9" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B9" s="33"/>
+      <c r="B9" s="39"/>
       <c r="C9" s="2" t="s">
         <v>30</v>
       </c>
@@ -4061,7 +4061,7 @@
       </c>
     </row>
     <row r="10" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B10" s="33"/>
+      <c r="B10" s="39"/>
       <c r="C10" s="2" t="s">
         <v>31</v>
       </c>
@@ -4124,7 +4124,7 @@
       </c>
     </row>
     <row r="11" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B11" s="33"/>
+      <c r="B11" s="39"/>
       <c r="C11" s="2" t="s">
         <v>32</v>
       </c>
@@ -4187,7 +4187,7 @@
       </c>
     </row>
     <row r="12" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B12" s="31"/>
+      <c r="B12" s="37"/>
       <c r="C12" s="3" t="s">
         <v>33</v>
       </c>
@@ -4250,7 +4250,7 @@
       </c>
     </row>
     <row r="13" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B13" s="30" t="s">
+      <c r="B13" s="36" t="s">
         <v>24</v>
       </c>
       <c r="C13" s="8" t="s">
@@ -4315,7 +4315,7 @@
       </c>
     </row>
     <row r="14" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B14" s="33"/>
+      <c r="B14" s="39"/>
       <c r="C14" s="2" t="s">
         <v>35</v>
       </c>
@@ -4378,7 +4378,7 @@
       </c>
     </row>
     <row r="15" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B15" s="33"/>
+      <c r="B15" s="39"/>
       <c r="C15" s="2" t="s">
         <v>36</v>
       </c>
@@ -4441,7 +4441,7 @@
       </c>
     </row>
     <row r="16" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B16" s="31"/>
+      <c r="B16" s="37"/>
       <c r="C16" s="3" t="s">
         <v>37</v>
       </c>
@@ -4504,7 +4504,7 @@
       </c>
     </row>
     <row r="17" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B17" s="30" t="s">
+      <c r="B17" s="36" t="s">
         <v>26</v>
       </c>
       <c r="C17" s="8" t="s">
@@ -4569,7 +4569,7 @@
       </c>
     </row>
     <row r="18" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B18" s="33"/>
+      <c r="B18" s="39"/>
       <c r="C18" s="2" t="s">
         <v>38</v>
       </c>
@@ -4632,7 +4632,7 @@
       </c>
     </row>
     <row r="19" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B19" s="31"/>
+      <c r="B19" s="37"/>
       <c r="C19" s="3" t="s">
         <v>39</v>
       </c>
@@ -4695,7 +4695,7 @@
       </c>
     </row>
     <row r="20" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B20" s="30" t="s">
+      <c r="B20" s="36" t="s">
         <v>27</v>
       </c>
       <c r="C20" s="8" t="s">
@@ -4760,7 +4760,7 @@
       </c>
     </row>
     <row r="21" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B21" s="31"/>
+      <c r="B21" s="37"/>
       <c r="C21" s="3" t="s">
         <v>41</v>
       </c>
@@ -4823,7 +4823,7 @@
       </c>
     </row>
     <row r="22" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B22" s="30" t="s">
+      <c r="B22" s="36" t="s">
         <v>28</v>
       </c>
       <c r="C22" s="8" t="s">
@@ -4888,7 +4888,7 @@
       </c>
     </row>
     <row r="23" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B23" s="31"/>
+      <c r="B23" s="37"/>
       <c r="C23" s="3" t="s">
         <v>43</v>
       </c>
@@ -5047,8 +5047,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B40D316F-9AC3-40B6-9034-2229B798232F}">
   <dimension ref="B2:AE24"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5092,14 +5092,14 @@
       <c r="U2" s="25"/>
       <c r="V2" s="25"/>
       <c r="W2" s="25"/>
-      <c r="X2" s="37"/>
-      <c r="Y2" s="37"/>
-      <c r="Z2" s="37"/>
-      <c r="AA2" s="37"/>
-      <c r="AB2" s="37"/>
-      <c r="AC2" s="37"/>
-      <c r="AD2" s="37"/>
-      <c r="AE2" s="37"/>
+      <c r="X2" s="43"/>
+      <c r="Y2" s="43"/>
+      <c r="Z2" s="43"/>
+      <c r="AA2" s="43"/>
+      <c r="AB2" s="43"/>
+      <c r="AC2" s="43"/>
+      <c r="AD2" s="43"/>
+      <c r="AE2" s="43"/>
     </row>
     <row r="3" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B3" s="16"/>
@@ -5186,10 +5186,10 @@
       </c>
     </row>
     <row r="4" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="40" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="38">
+      <c r="C4" s="44">
         <v>10</v>
       </c>
       <c r="D4" s="15" t="s">
@@ -5200,7 +5200,9 @@
       </c>
       <c r="F4" s="9"/>
       <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
+      <c r="N4" s="2">
+        <v>1</v>
+      </c>
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
@@ -5220,8 +5222,8 @@
       <c r="AE4" s="12"/>
     </row>
     <row r="5" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B5" s="35"/>
-      <c r="C5" s="39"/>
+      <c r="B5" s="41"/>
+      <c r="C5" s="45"/>
       <c r="D5" s="28" t="s">
         <v>62</v>
       </c>
@@ -5229,6 +5231,9 @@
         <v>56</v>
       </c>
       <c r="F5" s="10"/>
+      <c r="L5">
+        <v>1</v>
+      </c>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
@@ -5250,8 +5255,8 @@
       <c r="AE5" s="13"/>
     </row>
     <row r="6" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B6" s="35"/>
-      <c r="C6" s="39"/>
+      <c r="B6" s="41"/>
+      <c r="C6" s="45"/>
       <c r="D6" s="28" t="s">
         <v>63</v>
       </c>
@@ -5259,6 +5264,15 @@
         <v>57</v>
       </c>
       <c r="F6" s="10"/>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
@@ -5280,8 +5294,8 @@
       <c r="AE6" s="13"/>
     </row>
     <row r="7" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B7" s="36"/>
-      <c r="C7" s="40"/>
+      <c r="B7" s="42"/>
+      <c r="C7" s="46"/>
       <c r="D7" s="29" t="s">
         <v>64</v>
       </c>
@@ -5289,8 +5303,12 @@
         <v>57</v>
       </c>
       <c r="F7" s="11"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
+      <c r="G7" s="3">
+        <v>1</v>
+      </c>
+      <c r="H7" s="3">
+        <v>2</v>
+      </c>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
@@ -5316,10 +5334,10 @@
       <c r="AE7" s="14"/>
     </row>
     <row r="8" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="C8" s="38">
+      <c r="C8" s="44">
         <v>10</v>
       </c>
       <c r="D8" s="15" t="s">
@@ -5331,7 +5349,9 @@
       <c r="F8" s="9"/>
       <c r="M8" s="8"/>
       <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
+      <c r="O8" s="8">
+        <v>1</v>
+      </c>
       <c r="P8" s="8"/>
       <c r="Q8" s="8"/>
       <c r="R8" s="8"/>
@@ -5350,8 +5370,8 @@
       <c r="AE8" s="12"/>
     </row>
     <row r="9" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B9" s="35"/>
-      <c r="C9" s="39"/>
+      <c r="B9" s="41"/>
+      <c r="C9" s="45"/>
       <c r="D9" s="28" t="s">
         <v>66</v>
       </c>
@@ -5380,8 +5400,8 @@
       <c r="AE9" s="13"/>
     </row>
     <row r="10" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B10" s="35"/>
-      <c r="C10" s="39"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="45"/>
       <c r="D10" s="28" t="s">
         <v>67</v>
       </c>
@@ -5410,8 +5430,8 @@
       <c r="AE10" s="13"/>
     </row>
     <row r="11" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B11" s="35"/>
-      <c r="C11" s="39"/>
+      <c r="B11" s="41"/>
+      <c r="C11" s="45"/>
       <c r="D11" s="28" t="s">
         <v>68</v>
       </c>
@@ -5440,8 +5460,8 @@
       <c r="AE11" s="13"/>
     </row>
     <row r="12" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B12" s="36"/>
-      <c r="C12" s="40"/>
+      <c r="B12" s="42"/>
+      <c r="C12" s="46"/>
       <c r="D12" s="29" t="s">
         <v>69</v>
       </c>
@@ -5470,10 +5490,10 @@
       <c r="AE12" s="14"/>
     </row>
     <row r="13" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B13" s="34" t="s">
+      <c r="B13" s="40" t="s">
         <v>52</v>
       </c>
-      <c r="C13" s="38">
+      <c r="C13" s="44">
         <v>6</v>
       </c>
       <c r="D13" s="15" t="s">
@@ -5502,8 +5522,8 @@
       <c r="AE13" s="12"/>
     </row>
     <row r="14" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B14" s="35"/>
-      <c r="C14" s="39"/>
+      <c r="B14" s="41"/>
+      <c r="C14" s="45"/>
       <c r="D14" s="28" t="s">
         <v>71</v>
       </c>
@@ -5530,8 +5550,8 @@
       <c r="AE14" s="13"/>
     </row>
     <row r="15" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B15" s="35"/>
-      <c r="C15" s="39"/>
+      <c r="B15" s="41"/>
+      <c r="C15" s="45"/>
       <c r="D15" s="28" t="s">
         <v>72</v>
       </c>
@@ -5558,8 +5578,8 @@
       <c r="AE15" s="13"/>
     </row>
     <row r="16" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B16" s="36"/>
-      <c r="C16" s="40"/>
+      <c r="B16" s="42"/>
+      <c r="C16" s="46"/>
       <c r="D16" s="29" t="s">
         <v>73</v>
       </c>
@@ -5596,103 +5616,103 @@
       </c>
       <c r="G17" s="9">
         <f>F17-SUM(G4:G16)</f>
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H17" s="9">
         <f t="shared" ref="H17:X17" si="0">G17-SUM(H4:H16)</f>
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="I17" s="9">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="J17" s="9">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="K17" s="9">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="L17" s="9">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="M17" s="9">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="N17" s="9">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="O17" s="9">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="P17" s="9">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="Q17" s="9">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="R17" s="9">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="S17" s="9">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="T17" s="9">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="U17" s="9">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="V17" s="9">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="W17" s="9">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="X17" s="15">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="Y17" s="15">
         <f t="shared" ref="Y17" si="1">X17-SUM(Y4:Y16)</f>
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="Z17" s="15">
         <f t="shared" ref="Z17" si="2">Y17-SUM(Z4:Z16)</f>
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="AA17" s="15">
         <f t="shared" ref="AA17" si="3">Z17-SUM(AA4:AA16)</f>
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="AB17" s="15">
         <f t="shared" ref="AB17" si="4">AA17-SUM(AB4:AB16)</f>
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="AC17" s="15">
         <f t="shared" ref="AC17" si="5">AB17-SUM(AC4:AC16)</f>
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="AD17" s="15">
         <f t="shared" ref="AD17" si="6">AC17-SUM(AD4:AD16)</f>
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="AE17" s="15">
         <f t="shared" ref="AE17" si="7">AD17-SUM(AE4:AE16)</f>
-        <v>26</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="2:31" x14ac:dyDescent="0.25">
@@ -5887,21 +5907,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010007C60AE6480C8D49900E7A4362DC978A" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2c8c8df2ae4c8b52ea756b3d40f22f1c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="40d8dcd0-4b95-4e4d-9aa5-be2e8658acc5" xmlns:ns4="3244cbb2-9f52-4273-9113-8cc2cecf4979" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="54d9cecd5b552591da97f0387668823e" ns3:_="" ns4:_="">
     <xsd:import namespace="40d8dcd0-4b95-4e4d-9aa5-be2e8658acc5"/>
@@ -6124,32 +6129,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA34204B-E607-45A1-9498-394427B9D986}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="3244cbb2-9f52-4273-9113-8cc2cecf4979"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="40d8dcd0-4b95-4e4d-9aa5-be2e8658acc5"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B975CF3D-B020-4216-8822-B9E8F3D97495}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{308378B9-91A3-4988-8873-F75977EABA14}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6166,4 +6161,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B975CF3D-B020-4216-8822-B9E8F3D97495}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA34204B-E607-45A1-9498-394427B9D986}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="3244cbb2-9f52-4273-9113-8cc2cecf4979"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="40d8dcd0-4b95-4e4d-9aa5-be2e8658acc5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update: Seating page in need of icons
</commit_message>
<xml_diff>
--- a/Group C2-3 Scrum documentation.xlsx
+++ b/Group C2-3 Scrum documentation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johna\OneDrive\Documents\University\Year II\CO553 Agile Development and Software Security B\co553-c2-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18FA5D80-670D-4336-8E68-DCE011F037B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21DA1076-0990-497B-8ABD-AA37B7539C75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{0CC9FE5D-919A-41CA-B32D-5FFC3808111C}"/>
   </bookViews>
@@ -567,7 +567,7 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -606,9 +606,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -652,6 +649,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1451,55 +1452,55 @@
                   <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>17</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>17</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>17</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>17</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>17</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>17</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>17</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>17</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>17</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>17</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>17</c:v>
+                  <c:v>8.5</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>17</c:v>
+                  <c:v>8.5</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>17</c:v>
+                  <c:v>8.5</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>17</c:v>
+                  <c:v>8.5</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>17</c:v>
+                  <c:v>8.5</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>17</c:v>
+                  <c:v>8.5</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>17</c:v>
+                  <c:v>8.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3348,7 +3349,7 @@
   <dimension ref="B2:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="B12" sqref="B12:D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3368,200 +3369,200 @@
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="35">
+      <c r="B3" s="34">
         <v>1</v>
       </c>
-      <c r="C3" s="35" t="s">
+      <c r="C3" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="35">
+      <c r="D3" s="34">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="35">
+      <c r="B4" s="34">
         <v>2</v>
       </c>
-      <c r="C4" s="35" t="s">
+      <c r="C4" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="35">
+      <c r="D4" s="34">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="35">
+      <c r="B5" s="34">
         <v>3</v>
       </c>
-      <c r="C5" s="35" t="s">
+      <c r="C5" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="35">
+      <c r="D5" s="34">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="35">
+      <c r="B6" s="34">
         <v>4</v>
       </c>
-      <c r="C6" s="35" t="s">
+      <c r="C6" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="35">
+      <c r="D6" s="34">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="35">
+      <c r="B7" s="34">
         <v>5</v>
       </c>
-      <c r="C7" s="35" t="s">
+      <c r="C7" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="35">
+      <c r="D7" s="34">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="35">
+      <c r="B8" s="34">
         <v>6</v>
       </c>
-      <c r="C8" s="35" t="s">
+      <c r="C8" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="35">
+      <c r="D8" s="34">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="30">
+      <c r="B9" s="47">
         <v>7</v>
       </c>
-      <c r="C9" s="30" t="s">
+      <c r="C9" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="30">
+      <c r="D9" s="47">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="30">
+      <c r="B10" s="47">
         <v>8</v>
       </c>
-      <c r="C10" s="30" t="s">
+      <c r="C10" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="30">
+      <c r="D10" s="47">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="31">
+      <c r="B11" s="47">
         <v>9</v>
       </c>
-      <c r="C11" s="31" t="s">
+      <c r="C11" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="31">
+      <c r="D11" s="47">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="31">
+      <c r="B12" s="30">
         <v>10</v>
       </c>
-      <c r="C12" s="31" t="s">
+      <c r="C12" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="31">
+      <c r="D12" s="30">
         <v>3</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="31">
+      <c r="B13" s="30">
         <v>11</v>
       </c>
-      <c r="C13" s="31" t="s">
+      <c r="C13" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="31">
+      <c r="D13" s="30">
         <v>2</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="31">
+      <c r="B14" s="30">
         <v>12</v>
       </c>
-      <c r="C14" s="31" t="s">
+      <c r="C14" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="31">
+      <c r="D14" s="30">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="31">
+      <c r="B15" s="30">
         <v>13</v>
       </c>
-      <c r="C15" s="32" t="s">
+      <c r="C15" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="31">
+      <c r="D15" s="30">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="31">
+      <c r="B16" s="30">
         <v>14</v>
       </c>
-      <c r="C16" s="32" t="s">
+      <c r="C16" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="31">
+      <c r="D16" s="30">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="33">
+      <c r="B17" s="32">
         <v>15</v>
       </c>
-      <c r="C17" s="34" t="s">
+      <c r="C17" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="33">
+      <c r="D17" s="32">
         <v>3</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="31">
+      <c r="B18" s="30">
         <v>16</v>
       </c>
-      <c r="C18" s="32" t="s">
+      <c r="C18" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="31">
+      <c r="D18" s="30">
         <v>5</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="33">
+      <c r="B19" s="32">
         <v>17</v>
       </c>
-      <c r="C19" s="34" t="s">
+      <c r="C19" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="33">
+      <c r="D19" s="32">
         <v>2</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="33">
+      <c r="B20" s="32">
         <v>18</v>
       </c>
-      <c r="C20" s="34" t="s">
+      <c r="C20" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="D20" s="33">
+      <c r="D20" s="32">
         <v>1</v>
       </c>
     </row>
@@ -3595,27 +3596,27 @@
       <c r="C2" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="38" t="s">
+      <c r="D2" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
-      <c r="M2" s="38"/>
-      <c r="N2" s="38"/>
-      <c r="O2" s="38"/>
-      <c r="P2" s="38"/>
-      <c r="Q2" s="38"/>
-      <c r="R2" s="38"/>
-      <c r="S2" s="38"/>
-      <c r="T2" s="38"/>
-      <c r="U2" s="38"/>
-      <c r="V2" s="38"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="37"/>
+      <c r="O2" s="37"/>
+      <c r="P2" s="37"/>
+      <c r="Q2" s="37"/>
+      <c r="R2" s="37"/>
+      <c r="S2" s="37"/>
+      <c r="T2" s="37"/>
+      <c r="U2" s="37"/>
+      <c r="V2" s="37"/>
     </row>
     <row r="3" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B3" s="16"/>
@@ -3679,7 +3680,7 @@
       </c>
     </row>
     <row r="4" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="35" t="s">
         <v>22</v>
       </c>
       <c r="C4" s="6" t="s">
@@ -3744,7 +3745,7 @@
       </c>
     </row>
     <row r="5" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B5" s="39"/>
+      <c r="B5" s="38"/>
       <c r="C5" s="6" t="s">
         <v>47</v>
       </c>
@@ -3807,7 +3808,7 @@
       </c>
     </row>
     <row r="6" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B6" s="39"/>
+      <c r="B6" s="38"/>
       <c r="C6" s="2" t="s">
         <v>46</v>
       </c>
@@ -3870,7 +3871,7 @@
       </c>
     </row>
     <row r="7" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B7" s="37"/>
+      <c r="B7" s="36"/>
       <c r="C7" s="3" t="s">
         <v>45</v>
       </c>
@@ -3933,7 +3934,7 @@
       </c>
     </row>
     <row r="8" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="35" t="s">
         <v>23</v>
       </c>
       <c r="C8" s="8" t="s">
@@ -3998,7 +3999,7 @@
       </c>
     </row>
     <row r="9" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B9" s="39"/>
+      <c r="B9" s="38"/>
       <c r="C9" s="2" t="s">
         <v>30</v>
       </c>
@@ -4061,7 +4062,7 @@
       </c>
     </row>
     <row r="10" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B10" s="39"/>
+      <c r="B10" s="38"/>
       <c r="C10" s="2" t="s">
         <v>31</v>
       </c>
@@ -4124,7 +4125,7 @@
       </c>
     </row>
     <row r="11" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B11" s="39"/>
+      <c r="B11" s="38"/>
       <c r="C11" s="2" t="s">
         <v>32</v>
       </c>
@@ -4187,7 +4188,7 @@
       </c>
     </row>
     <row r="12" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B12" s="37"/>
+      <c r="B12" s="36"/>
       <c r="C12" s="3" t="s">
         <v>33</v>
       </c>
@@ -4250,7 +4251,7 @@
       </c>
     </row>
     <row r="13" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B13" s="36" t="s">
+      <c r="B13" s="35" t="s">
         <v>24</v>
       </c>
       <c r="C13" s="8" t="s">
@@ -4315,7 +4316,7 @@
       </c>
     </row>
     <row r="14" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B14" s="39"/>
+      <c r="B14" s="38"/>
       <c r="C14" s="2" t="s">
         <v>35</v>
       </c>
@@ -4378,7 +4379,7 @@
       </c>
     </row>
     <row r="15" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B15" s="39"/>
+      <c r="B15" s="38"/>
       <c r="C15" s="2" t="s">
         <v>36</v>
       </c>
@@ -4441,7 +4442,7 @@
       </c>
     </row>
     <row r="16" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B16" s="37"/>
+      <c r="B16" s="36"/>
       <c r="C16" s="3" t="s">
         <v>37</v>
       </c>
@@ -4504,7 +4505,7 @@
       </c>
     </row>
     <row r="17" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B17" s="36" t="s">
+      <c r="B17" s="35" t="s">
         <v>26</v>
       </c>
       <c r="C17" s="8" t="s">
@@ -4569,7 +4570,7 @@
       </c>
     </row>
     <row r="18" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B18" s="39"/>
+      <c r="B18" s="38"/>
       <c r="C18" s="2" t="s">
         <v>38</v>
       </c>
@@ -4632,7 +4633,7 @@
       </c>
     </row>
     <row r="19" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B19" s="37"/>
+      <c r="B19" s="36"/>
       <c r="C19" s="3" t="s">
         <v>39</v>
       </c>
@@ -4695,7 +4696,7 @@
       </c>
     </row>
     <row r="20" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B20" s="36" t="s">
+      <c r="B20" s="35" t="s">
         <v>27</v>
       </c>
       <c r="C20" s="8" t="s">
@@ -4760,7 +4761,7 @@
       </c>
     </row>
     <row r="21" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B21" s="37"/>
+      <c r="B21" s="36"/>
       <c r="C21" s="3" t="s">
         <v>41</v>
       </c>
@@ -4823,7 +4824,7 @@
       </c>
     </row>
     <row r="22" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B22" s="36" t="s">
+      <c r="B22" s="35" t="s">
         <v>28</v>
       </c>
       <c r="C22" s="8" t="s">
@@ -4888,7 +4889,7 @@
       </c>
     </row>
     <row r="23" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B23" s="37"/>
+      <c r="B23" s="36"/>
       <c r="C23" s="3" t="s">
         <v>43</v>
       </c>
@@ -5047,8 +5048,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B40D316F-9AC3-40B6-9034-2229B798232F}">
   <dimension ref="B2:AE24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5092,14 +5093,14 @@
       <c r="U2" s="25"/>
       <c r="V2" s="25"/>
       <c r="W2" s="25"/>
-      <c r="X2" s="43"/>
-      <c r="Y2" s="43"/>
-      <c r="Z2" s="43"/>
-      <c r="AA2" s="43"/>
-      <c r="AB2" s="43"/>
-      <c r="AC2" s="43"/>
-      <c r="AD2" s="43"/>
-      <c r="AE2" s="43"/>
+      <c r="X2" s="42"/>
+      <c r="Y2" s="42"/>
+      <c r="Z2" s="42"/>
+      <c r="AA2" s="42"/>
+      <c r="AB2" s="42"/>
+      <c r="AC2" s="42"/>
+      <c r="AD2" s="42"/>
+      <c r="AE2" s="42"/>
     </row>
     <row r="3" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B3" s="16"/>
@@ -5186,10 +5187,10 @@
       </c>
     </row>
     <row r="4" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="44">
+      <c r="C4" s="43">
         <v>10</v>
       </c>
       <c r="D4" s="15" t="s">
@@ -5200,13 +5201,15 @@
       </c>
       <c r="F4" s="9"/>
       <c r="M4" s="2"/>
-      <c r="N4" s="2">
+      <c r="N4" s="17">
         <v>1</v>
       </c>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
+      <c r="O4" s="17"/>
+      <c r="P4" s="17"/>
+      <c r="Q4" s="17"/>
+      <c r="R4" s="17">
+        <v>2</v>
+      </c>
       <c r="S4" s="2"/>
       <c r="T4" s="2"/>
       <c r="U4" s="2"/>
@@ -5222,8 +5225,8 @@
       <c r="AE4" s="12"/>
     </row>
     <row r="5" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B5" s="41"/>
-      <c r="C5" s="45"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="44"/>
       <c r="D5" s="28" t="s">
         <v>62</v>
       </c>
@@ -5231,7 +5234,7 @@
         <v>56</v>
       </c>
       <c r="F5" s="10"/>
-      <c r="L5">
+      <c r="L5" s="46">
         <v>1</v>
       </c>
       <c r="M5" s="2"/>
@@ -5255,8 +5258,8 @@
       <c r="AE5" s="13"/>
     </row>
     <row r="6" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B6" s="41"/>
-      <c r="C6" s="45"/>
+      <c r="B6" s="40"/>
+      <c r="C6" s="44"/>
       <c r="D6" s="28" t="s">
         <v>63</v>
       </c>
@@ -5264,13 +5267,14 @@
         <v>57</v>
       </c>
       <c r="F6" s="10"/>
-      <c r="I6">
+      <c r="I6" s="46">
         <v>1</v>
       </c>
-      <c r="K6">
+      <c r="J6" s="46"/>
+      <c r="K6" s="46">
         <v>1</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="46">
         <v>1</v>
       </c>
       <c r="M6" s="2"/>
@@ -5294,8 +5298,8 @@
       <c r="AE6" s="13"/>
     </row>
     <row r="7" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B7" s="42"/>
-      <c r="C7" s="46"/>
+      <c r="B7" s="41"/>
+      <c r="C7" s="45"/>
       <c r="D7" s="29" t="s">
         <v>64</v>
       </c>
@@ -5303,10 +5307,10 @@
         <v>57</v>
       </c>
       <c r="F7" s="11"/>
-      <c r="G7" s="3">
+      <c r="G7" s="22">
         <v>1</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="22">
         <v>2</v>
       </c>
       <c r="I7" s="3"/>
@@ -5334,10 +5338,10 @@
       <c r="AE7" s="14"/>
     </row>
     <row r="8" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B8" s="40" t="s">
+      <c r="B8" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="C8" s="44">
+      <c r="C8" s="43">
         <v>10</v>
       </c>
       <c r="D8" s="15" t="s">
@@ -5349,11 +5353,11 @@
       <c r="F8" s="9"/>
       <c r="M8" s="8"/>
       <c r="N8" s="8"/>
-      <c r="O8" s="8">
-        <v>1</v>
-      </c>
+      <c r="O8" s="8"/>
       <c r="P8" s="8"/>
-      <c r="Q8" s="8"/>
+      <c r="Q8" s="18">
+        <v>2</v>
+      </c>
       <c r="R8" s="8"/>
       <c r="S8" s="8"/>
       <c r="T8" s="8"/>
@@ -5370,8 +5374,8 @@
       <c r="AE8" s="12"/>
     </row>
     <row r="9" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B9" s="41"/>
-      <c r="C9" s="45"/>
+      <c r="B9" s="40"/>
+      <c r="C9" s="44"/>
       <c r="D9" s="28" t="s">
         <v>66</v>
       </c>
@@ -5400,8 +5404,8 @@
       <c r="AE9" s="13"/>
     </row>
     <row r="10" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B10" s="41"/>
-      <c r="C10" s="45"/>
+      <c r="B10" s="40"/>
+      <c r="C10" s="44"/>
       <c r="D10" s="28" t="s">
         <v>67</v>
       </c>
@@ -5430,8 +5434,8 @@
       <c r="AE10" s="13"/>
     </row>
     <row r="11" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B11" s="41"/>
-      <c r="C11" s="45"/>
+      <c r="B11" s="40"/>
+      <c r="C11" s="44"/>
       <c r="D11" s="28" t="s">
         <v>68</v>
       </c>
@@ -5460,8 +5464,8 @@
       <c r="AE11" s="13"/>
     </row>
     <row r="12" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B12" s="42"/>
-      <c r="C12" s="46"/>
+      <c r="B12" s="41"/>
+      <c r="C12" s="45"/>
       <c r="D12" s="29" t="s">
         <v>69</v>
       </c>
@@ -5490,10 +5494,10 @@
       <c r="AE12" s="14"/>
     </row>
     <row r="13" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B13" s="40" t="s">
+      <c r="B13" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="C13" s="44">
+      <c r="C13" s="43">
         <v>6</v>
       </c>
       <c r="D13" s="15" t="s">
@@ -5509,6 +5513,9 @@
       <c r="J13" s="8"/>
       <c r="K13" s="8"/>
       <c r="L13" s="8"/>
+      <c r="T13" s="46">
+        <v>1</v>
+      </c>
       <c r="U13" s="8"/>
       <c r="V13" s="8"/>
       <c r="W13" s="8"/>
@@ -5522,8 +5529,8 @@
       <c r="AE13" s="12"/>
     </row>
     <row r="14" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B14" s="41"/>
-      <c r="C14" s="45"/>
+      <c r="B14" s="40"/>
+      <c r="C14" s="44"/>
       <c r="D14" s="28" t="s">
         <v>71</v>
       </c>
@@ -5538,7 +5545,9 @@
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
       <c r="U14" s="2"/>
-      <c r="V14" s="2"/>
+      <c r="V14" s="17">
+        <v>1</v>
+      </c>
       <c r="W14" s="2"/>
       <c r="X14" s="2"/>
       <c r="Y14" s="2"/>
@@ -5550,8 +5559,8 @@
       <c r="AE14" s="13"/>
     </row>
     <row r="15" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B15" s="41"/>
-      <c r="C15" s="45"/>
+      <c r="B15" s="40"/>
+      <c r="C15" s="44"/>
       <c r="D15" s="28" t="s">
         <v>72</v>
       </c>
@@ -5568,8 +5577,12 @@
       <c r="U15" s="2"/>
       <c r="V15" s="2"/>
       <c r="W15" s="2"/>
-      <c r="X15" s="2"/>
-      <c r="Y15" s="2"/>
+      <c r="X15" s="17">
+        <v>2</v>
+      </c>
+      <c r="Y15" s="17">
+        <v>1</v>
+      </c>
       <c r="Z15" s="2"/>
       <c r="AA15" s="2"/>
       <c r="AB15" s="2"/>
@@ -5578,8 +5591,8 @@
       <c r="AE15" s="13"/>
     </row>
     <row r="16" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B16" s="42"/>
-      <c r="C16" s="46"/>
+      <c r="B16" s="41"/>
+      <c r="C16" s="45"/>
       <c r="D16" s="29" t="s">
         <v>73</v>
       </c>
@@ -5597,7 +5610,9 @@
       <c r="V16" s="2"/>
       <c r="W16" s="2"/>
       <c r="X16" s="3"/>
-      <c r="Y16" s="3"/>
+      <c r="Y16" s="22">
+        <v>0.5</v>
+      </c>
       <c r="Z16" s="3"/>
       <c r="AA16" s="3"/>
       <c r="AB16" s="3"/>
@@ -5648,71 +5663,71 @@
       </c>
       <c r="O17" s="9">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="P17" s="9">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="Q17" s="9">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="R17" s="9">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="S17" s="9">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="T17" s="9">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="U17" s="9">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="V17" s="9">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="W17" s="9">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="X17" s="15">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="Y17" s="15">
         <f t="shared" ref="Y17" si="1">X17-SUM(Y4:Y16)</f>
-        <v>17</v>
+        <v>8.5</v>
       </c>
       <c r="Z17" s="15">
         <f t="shared" ref="Z17" si="2">Y17-SUM(Z4:Z16)</f>
-        <v>17</v>
+        <v>8.5</v>
       </c>
       <c r="AA17" s="15">
         <f t="shared" ref="AA17" si="3">Z17-SUM(AA4:AA16)</f>
-        <v>17</v>
+        <v>8.5</v>
       </c>
       <c r="AB17" s="15">
         <f t="shared" ref="AB17" si="4">AA17-SUM(AB4:AB16)</f>
-        <v>17</v>
+        <v>8.5</v>
       </c>
       <c r="AC17" s="15">
         <f t="shared" ref="AC17" si="5">AB17-SUM(AC4:AC16)</f>
-        <v>17</v>
+        <v>8.5</v>
       </c>
       <c r="AD17" s="15">
         <f t="shared" ref="AD17" si="6">AC17-SUM(AD4:AD16)</f>
-        <v>17</v>
+        <v>8.5</v>
       </c>
       <c r="AE17" s="15">
         <f t="shared" ref="AE17" si="7">AD17-SUM(AE4:AE16)</f>
-        <v>17</v>
+        <v>8.5</v>
       </c>
     </row>
     <row r="18" spans="2:31" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update: Sprint 2 documentation
</commit_message>
<xml_diff>
--- a/Group C2-3 Scrum documentation.xlsx
+++ b/Group C2-3 Scrum documentation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johna\OneDrive\Documents\University\Year II\CO553 Agile Development and Software Security B\co553-c2-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21DA1076-0990-497B-8ABD-AA37B7539C75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A28A34BB-9C7D-4C69-AB7F-8E8CBDAF4809}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{0CC9FE5D-919A-41CA-B32D-5FFC3808111C}"/>
   </bookViews>
@@ -567,7 +567,7 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -617,6 +617,9 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -649,10 +652,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1464,43 +1463,43 @@
                   <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>14</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>13</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>13</c:v>
+                  <c:v>10.5</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>12</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>12</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>10</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>8.5</c:v>
+                  <c:v>5.5</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>8.5</c:v>
+                  <c:v>5.5</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>8.5</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>8.5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>8.5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>8.5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>8.5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3435,35 +3434,35 @@
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="47">
+      <c r="B9" s="35">
         <v>7</v>
       </c>
-      <c r="C9" s="47" t="s">
+      <c r="C9" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="47">
+      <c r="D9" s="35">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="47">
+      <c r="B10" s="35">
         <v>8</v>
       </c>
-      <c r="C10" s="47" t="s">
+      <c r="C10" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="47">
+      <c r="D10" s="35">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="47">
+      <c r="B11" s="35">
         <v>9</v>
       </c>
-      <c r="C11" s="47" t="s">
+      <c r="C11" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="47">
+      <c r="D11" s="35">
         <v>5</v>
       </c>
     </row>
@@ -3596,27 +3595,27 @@
       <c r="C2" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="37" t="s">
+      <c r="D2" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37"/>
-      <c r="O2" s="37"/>
-      <c r="P2" s="37"/>
-      <c r="Q2" s="37"/>
-      <c r="R2" s="37"/>
-      <c r="S2" s="37"/>
-      <c r="T2" s="37"/>
-      <c r="U2" s="37"/>
-      <c r="V2" s="37"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="38"/>
+      <c r="P2" s="38"/>
+      <c r="Q2" s="38"/>
+      <c r="R2" s="38"/>
+      <c r="S2" s="38"/>
+      <c r="T2" s="38"/>
+      <c r="U2" s="38"/>
+      <c r="V2" s="38"/>
     </row>
     <row r="3" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B3" s="16"/>
@@ -3680,7 +3679,7 @@
       </c>
     </row>
     <row r="4" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="36" t="s">
         <v>22</v>
       </c>
       <c r="C4" s="6" t="s">
@@ -3745,7 +3744,7 @@
       </c>
     </row>
     <row r="5" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B5" s="38"/>
+      <c r="B5" s="39"/>
       <c r="C5" s="6" t="s">
         <v>47</v>
       </c>
@@ -3808,7 +3807,7 @@
       </c>
     </row>
     <row r="6" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B6" s="38"/>
+      <c r="B6" s="39"/>
       <c r="C6" s="2" t="s">
         <v>46</v>
       </c>
@@ -3871,7 +3870,7 @@
       </c>
     </row>
     <row r="7" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B7" s="36"/>
+      <c r="B7" s="37"/>
       <c r="C7" s="3" t="s">
         <v>45</v>
       </c>
@@ -3934,7 +3933,7 @@
       </c>
     </row>
     <row r="8" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B8" s="35" t="s">
+      <c r="B8" s="36" t="s">
         <v>23</v>
       </c>
       <c r="C8" s="8" t="s">
@@ -3999,7 +3998,7 @@
       </c>
     </row>
     <row r="9" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B9" s="38"/>
+      <c r="B9" s="39"/>
       <c r="C9" s="2" t="s">
         <v>30</v>
       </c>
@@ -4062,7 +4061,7 @@
       </c>
     </row>
     <row r="10" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B10" s="38"/>
+      <c r="B10" s="39"/>
       <c r="C10" s="2" t="s">
         <v>31</v>
       </c>
@@ -4125,7 +4124,7 @@
       </c>
     </row>
     <row r="11" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B11" s="38"/>
+      <c r="B11" s="39"/>
       <c r="C11" s="2" t="s">
         <v>32</v>
       </c>
@@ -4188,7 +4187,7 @@
       </c>
     </row>
     <row r="12" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B12" s="36"/>
+      <c r="B12" s="37"/>
       <c r="C12" s="3" t="s">
         <v>33</v>
       </c>
@@ -4251,7 +4250,7 @@
       </c>
     </row>
     <row r="13" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B13" s="35" t="s">
+      <c r="B13" s="36" t="s">
         <v>24</v>
       </c>
       <c r="C13" s="8" t="s">
@@ -4316,7 +4315,7 @@
       </c>
     </row>
     <row r="14" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B14" s="38"/>
+      <c r="B14" s="39"/>
       <c r="C14" s="2" t="s">
         <v>35</v>
       </c>
@@ -4379,7 +4378,7 @@
       </c>
     </row>
     <row r="15" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B15" s="38"/>
+      <c r="B15" s="39"/>
       <c r="C15" s="2" t="s">
         <v>36</v>
       </c>
@@ -4442,7 +4441,7 @@
       </c>
     </row>
     <row r="16" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B16" s="36"/>
+      <c r="B16" s="37"/>
       <c r="C16" s="3" t="s">
         <v>37</v>
       </c>
@@ -4505,7 +4504,7 @@
       </c>
     </row>
     <row r="17" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B17" s="35" t="s">
+      <c r="B17" s="36" t="s">
         <v>26</v>
       </c>
       <c r="C17" s="8" t="s">
@@ -4570,7 +4569,7 @@
       </c>
     </row>
     <row r="18" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B18" s="38"/>
+      <c r="B18" s="39"/>
       <c r="C18" s="2" t="s">
         <v>38</v>
       </c>
@@ -4633,7 +4632,7 @@
       </c>
     </row>
     <row r="19" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B19" s="36"/>
+      <c r="B19" s="37"/>
       <c r="C19" s="3" t="s">
         <v>39</v>
       </c>
@@ -4696,7 +4695,7 @@
       </c>
     </row>
     <row r="20" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B20" s="35" t="s">
+      <c r="B20" s="36" t="s">
         <v>27</v>
       </c>
       <c r="C20" s="8" t="s">
@@ -4761,7 +4760,7 @@
       </c>
     </row>
     <row r="21" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B21" s="36"/>
+      <c r="B21" s="37"/>
       <c r="C21" s="3" t="s">
         <v>41</v>
       </c>
@@ -4824,7 +4823,7 @@
       </c>
     </row>
     <row r="22" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B22" s="35" t="s">
+      <c r="B22" s="36" t="s">
         <v>28</v>
       </c>
       <c r="C22" s="8" t="s">
@@ -4889,7 +4888,7 @@
       </c>
     </row>
     <row r="23" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B23" s="36"/>
+      <c r="B23" s="37"/>
       <c r="C23" s="3" t="s">
         <v>43</v>
       </c>
@@ -5048,8 +5047,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B40D316F-9AC3-40B6-9034-2229B798232F}">
   <dimension ref="B2:AE24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="Z20" sqref="Z20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5093,14 +5092,14 @@
       <c r="U2" s="25"/>
       <c r="V2" s="25"/>
       <c r="W2" s="25"/>
-      <c r="X2" s="42"/>
-      <c r="Y2" s="42"/>
-      <c r="Z2" s="42"/>
-      <c r="AA2" s="42"/>
-      <c r="AB2" s="42"/>
-      <c r="AC2" s="42"/>
-      <c r="AD2" s="42"/>
-      <c r="AE2" s="42"/>
+      <c r="X2" s="43"/>
+      <c r="Y2" s="43"/>
+      <c r="Z2" s="43"/>
+      <c r="AA2" s="43"/>
+      <c r="AB2" s="43"/>
+      <c r="AC2" s="43"/>
+      <c r="AD2" s="43"/>
+      <c r="AE2" s="43"/>
     </row>
     <row r="3" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B3" s="16"/>
@@ -5187,10 +5186,10 @@
       </c>
     </row>
     <row r="4" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="40" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="43">
+      <c r="C4" s="44">
         <v>10</v>
       </c>
       <c r="D4" s="15" t="s">
@@ -5201,13 +5200,10 @@
       </c>
       <c r="F4" s="9"/>
       <c r="M4" s="2"/>
-      <c r="N4" s="17">
+      <c r="N4">
         <v>1</v>
       </c>
-      <c r="O4" s="17"/>
-      <c r="P4" s="17"/>
-      <c r="Q4" s="17"/>
-      <c r="R4" s="17">
+      <c r="R4">
         <v>2</v>
       </c>
       <c r="S4" s="2"/>
@@ -5225,8 +5221,8 @@
       <c r="AE4" s="12"/>
     </row>
     <row r="5" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B5" s="40"/>
-      <c r="C5" s="44"/>
+      <c r="B5" s="41"/>
+      <c r="C5" s="45"/>
       <c r="D5" s="28" t="s">
         <v>62</v>
       </c>
@@ -5234,7 +5230,7 @@
         <v>56</v>
       </c>
       <c r="F5" s="10"/>
-      <c r="L5" s="46">
+      <c r="L5">
         <v>1</v>
       </c>
       <c r="M5" s="2"/>
@@ -5258,8 +5254,8 @@
       <c r="AE5" s="13"/>
     </row>
     <row r="6" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B6" s="40"/>
-      <c r="C6" s="44"/>
+      <c r="B6" s="41"/>
+      <c r="C6" s="45"/>
       <c r="D6" s="28" t="s">
         <v>63</v>
       </c>
@@ -5267,14 +5263,13 @@
         <v>57</v>
       </c>
       <c r="F6" s="10"/>
-      <c r="I6" s="46">
+      <c r="I6">
         <v>1</v>
       </c>
-      <c r="J6" s="46"/>
-      <c r="K6" s="46">
+      <c r="K6">
         <v>1</v>
       </c>
-      <c r="L6" s="46">
+      <c r="L6">
         <v>1</v>
       </c>
       <c r="M6" s="2"/>
@@ -5298,8 +5293,8 @@
       <c r="AE6" s="13"/>
     </row>
     <row r="7" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B7" s="41"/>
-      <c r="C7" s="45"/>
+      <c r="B7" s="42"/>
+      <c r="C7" s="46"/>
       <c r="D7" s="29" t="s">
         <v>64</v>
       </c>
@@ -5307,10 +5302,10 @@
         <v>57</v>
       </c>
       <c r="F7" s="11"/>
-      <c r="G7" s="22">
+      <c r="G7" s="3">
         <v>1</v>
       </c>
-      <c r="H7" s="22">
+      <c r="H7" s="3">
         <v>2</v>
       </c>
       <c r="I7" s="3"/>
@@ -5338,10 +5333,10 @@
       <c r="AE7" s="14"/>
     </row>
     <row r="8" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B8" s="39" t="s">
+      <c r="B8" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="C8" s="43">
+      <c r="C8" s="44">
         <v>10</v>
       </c>
       <c r="D8" s="15" t="s">
@@ -5355,7 +5350,7 @@
       <c r="N8" s="8"/>
       <c r="O8" s="8"/>
       <c r="P8" s="8"/>
-      <c r="Q8" s="18">
+      <c r="Q8">
         <v>2</v>
       </c>
       <c r="R8" s="8"/>
@@ -5374,8 +5369,8 @@
       <c r="AE8" s="12"/>
     </row>
     <row r="9" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B9" s="40"/>
-      <c r="C9" s="44"/>
+      <c r="B9" s="41"/>
+      <c r="C9" s="45"/>
       <c r="D9" s="28" t="s">
         <v>66</v>
       </c>
@@ -5389,9 +5384,12 @@
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
       <c r="R9" s="2"/>
-      <c r="S9" s="2"/>
-      <c r="T9" s="2"/>
-      <c r="U9" s="2"/>
+      <c r="S9">
+        <v>1</v>
+      </c>
+      <c r="U9">
+        <v>1.5</v>
+      </c>
       <c r="V9" s="2"/>
       <c r="W9" s="2"/>
       <c r="X9" s="2"/>
@@ -5404,8 +5402,8 @@
       <c r="AE9" s="13"/>
     </row>
     <row r="10" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B10" s="40"/>
-      <c r="C10" s="44"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="45"/>
       <c r="D10" s="28" t="s">
         <v>67</v>
       </c>
@@ -5430,12 +5428,14 @@
       <c r="AA10" s="2"/>
       <c r="AB10" s="2"/>
       <c r="AC10" s="2"/>
-      <c r="AD10" s="2"/>
+      <c r="AD10">
+        <v>1</v>
+      </c>
       <c r="AE10" s="13"/>
     </row>
     <row r="11" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B11" s="40"/>
-      <c r="C11" s="44"/>
+      <c r="B11" s="41"/>
+      <c r="C11" s="45"/>
       <c r="D11" s="28" t="s">
         <v>68</v>
       </c>
@@ -5453,19 +5453,20 @@
       <c r="T11" s="2"/>
       <c r="U11" s="2"/>
       <c r="V11" s="2"/>
-      <c r="W11" s="2"/>
       <c r="X11" s="2"/>
       <c r="Y11" s="2"/>
       <c r="Z11" s="2"/>
-      <c r="AA11" s="2"/>
+      <c r="AA11">
+        <v>0.5</v>
+      </c>
       <c r="AB11" s="2"/>
       <c r="AC11" s="2"/>
       <c r="AD11" s="2"/>
       <c r="AE11" s="13"/>
     </row>
     <row r="12" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B12" s="41"/>
-      <c r="C12" s="45"/>
+      <c r="B12" s="42"/>
+      <c r="C12" s="46"/>
       <c r="D12" s="29" t="s">
         <v>69</v>
       </c>
@@ -5484,20 +5485,21 @@
       <c r="U12" s="3"/>
       <c r="V12" s="3"/>
       <c r="W12" s="3"/>
-      <c r="X12" s="3"/>
       <c r="Y12" s="3"/>
       <c r="Z12" s="3"/>
       <c r="AA12" s="3"/>
-      <c r="AB12" s="3"/>
+      <c r="AB12">
+        <v>1</v>
+      </c>
       <c r="AC12" s="3"/>
       <c r="AD12" s="3"/>
       <c r="AE12" s="14"/>
     </row>
     <row r="13" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B13" s="39" t="s">
+      <c r="B13" s="40" t="s">
         <v>52</v>
       </c>
-      <c r="C13" s="43">
+      <c r="C13" s="44">
         <v>6</v>
       </c>
       <c r="D13" s="15" t="s">
@@ -5513,7 +5515,7 @@
       <c r="J13" s="8"/>
       <c r="K13" s="8"/>
       <c r="L13" s="8"/>
-      <c r="T13" s="46">
+      <c r="T13">
         <v>1</v>
       </c>
       <c r="U13" s="8"/>
@@ -5529,8 +5531,8 @@
       <c r="AE13" s="12"/>
     </row>
     <row r="14" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B14" s="40"/>
-      <c r="C14" s="44"/>
+      <c r="B14" s="41"/>
+      <c r="C14" s="45"/>
       <c r="D14" s="28" t="s">
         <v>71</v>
       </c>
@@ -5545,10 +5547,12 @@
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
       <c r="U14" s="2"/>
-      <c r="V14" s="17">
+      <c r="V14">
         <v>1</v>
       </c>
-      <c r="W14" s="2"/>
+      <c r="W14" s="2">
+        <v>0.5</v>
+      </c>
       <c r="X14" s="2"/>
       <c r="Y14" s="2"/>
       <c r="Z14" s="2"/>
@@ -5559,8 +5563,8 @@
       <c r="AE14" s="13"/>
     </row>
     <row r="15" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B15" s="40"/>
-      <c r="C15" s="44"/>
+      <c r="B15" s="41"/>
+      <c r="C15" s="45"/>
       <c r="D15" s="28" t="s">
         <v>72</v>
       </c>
@@ -5577,10 +5581,10 @@
       <c r="U15" s="2"/>
       <c r="V15" s="2"/>
       <c r="W15" s="2"/>
-      <c r="X15" s="17">
+      <c r="X15">
         <v>2</v>
       </c>
-      <c r="Y15" s="17">
+      <c r="Y15">
         <v>1</v>
       </c>
       <c r="Z15" s="2"/>
@@ -5591,8 +5595,8 @@
       <c r="AE15" s="13"/>
     </row>
     <row r="16" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B16" s="41"/>
-      <c r="C16" s="45"/>
+      <c r="B16" s="42"/>
+      <c r="C16" s="46"/>
       <c r="D16" s="29" t="s">
         <v>73</v>
       </c>
@@ -5610,7 +5614,7 @@
       <c r="V16" s="2"/>
       <c r="W16" s="2"/>
       <c r="X16" s="3"/>
-      <c r="Y16" s="22">
+      <c r="Y16">
         <v>0.5</v>
       </c>
       <c r="Z16" s="3"/>
@@ -5679,55 +5683,55 @@
       </c>
       <c r="S17" s="9">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="T17" s="9">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="U17" s="9">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>10.5</v>
       </c>
       <c r="V17" s="9">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>9.5</v>
       </c>
       <c r="W17" s="9">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="X17" s="15">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="Y17" s="15">
         <f t="shared" ref="Y17" si="1">X17-SUM(Y4:Y16)</f>
-        <v>8.5</v>
+        <v>5.5</v>
       </c>
       <c r="Z17" s="15">
         <f t="shared" ref="Z17" si="2">Y17-SUM(Z4:Z16)</f>
-        <v>8.5</v>
+        <v>5.5</v>
       </c>
       <c r="AA17" s="15">
         <f t="shared" ref="AA17" si="3">Z17-SUM(AA4:AA16)</f>
-        <v>8.5</v>
+        <v>5</v>
       </c>
       <c r="AB17" s="15">
         <f t="shared" ref="AB17" si="4">AA17-SUM(AB4:AB16)</f>
-        <v>8.5</v>
+        <v>4</v>
       </c>
       <c r="AC17" s="15">
         <f t="shared" ref="AC17" si="5">AB17-SUM(AC4:AC16)</f>
-        <v>8.5</v>
+        <v>4</v>
       </c>
       <c r="AD17" s="15">
         <f t="shared" ref="AD17" si="6">AC17-SUM(AD4:AD16)</f>
-        <v>8.5</v>
+        <v>3</v>
       </c>
       <c r="AE17" s="15">
         <f t="shared" ref="AE17" si="7">AD17-SUM(AE4:AE16)</f>
-        <v>8.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="2:31" x14ac:dyDescent="0.25">
@@ -5922,6 +5926,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010007C60AE6480C8D49900E7A4362DC978A" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2c8c8df2ae4c8b52ea756b3d40f22f1c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="40d8dcd0-4b95-4e4d-9aa5-be2e8658acc5" xmlns:ns4="3244cbb2-9f52-4273-9113-8cc2cecf4979" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="54d9cecd5b552591da97f0387668823e" ns3:_="" ns4:_="">
     <xsd:import namespace="40d8dcd0-4b95-4e4d-9aa5-be2e8658acc5"/>
@@ -6144,22 +6163,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA34204B-E607-45A1-9498-394427B9D986}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="3244cbb2-9f52-4273-9113-8cc2cecf4979"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="40d8dcd0-4b95-4e4d-9aa5-be2e8658acc5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B975CF3D-B020-4216-8822-B9E8F3D97495}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{308378B9-91A3-4988-8873-F75977EABA14}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6176,29 +6205,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B975CF3D-B020-4216-8822-B9E8F3D97495}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA34204B-E607-45A1-9498-394427B9D986}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="3244cbb2-9f52-4273-9113-8cc2cecf4979"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="40d8dcd0-4b95-4e4d-9aa5-be2e8658acc5"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update: Sprint 2 Documentation Revised
</commit_message>
<xml_diff>
--- a/Group C2-3 Scrum documentation.xlsx
+++ b/Group C2-3 Scrum documentation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johna\OneDrive\Documents\University\Year II\CO553 Agile Development and Software Security B\co553-c2-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A28A34BB-9C7D-4C69-AB7F-8E8CBDAF4809}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F94B983F-E502-4760-BE80-7DD49E410D82}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{0CC9FE5D-919A-41CA-B32D-5FFC3808111C}"/>
   </bookViews>
@@ -300,7 +300,7 @@
     <t>Create table with the information inputted [3]</t>
   </si>
   <si>
-    <t>Proceed with the booking confirmation [0.5]</t>
+    <t>Proceed to the booking confirmation [0.5]</t>
   </si>
 </sst>
 </file>
@@ -1496,10 +1496,10 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5048,7 +5048,7 @@
   <dimension ref="B2:AE24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="Z20" sqref="Z20"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5429,9 +5429,11 @@
       <c r="AB10" s="2"/>
       <c r="AC10" s="2"/>
       <c r="AD10">
-        <v>1</v>
-      </c>
-      <c r="AE10" s="13"/>
+        <v>2</v>
+      </c>
+      <c r="AE10" s="13">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B11" s="41"/>
@@ -5727,11 +5729,11 @@
       </c>
       <c r="AD17" s="15">
         <f t="shared" ref="AD17" si="6">AC17-SUM(AD4:AD16)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AE17" s="15">
         <f t="shared" ref="AE17" si="7">AD17-SUM(AE4:AE16)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="2:31" x14ac:dyDescent="0.25">
@@ -5926,21 +5928,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010007C60AE6480C8D49900E7A4362DC978A" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2c8c8df2ae4c8b52ea756b3d40f22f1c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="40d8dcd0-4b95-4e4d-9aa5-be2e8658acc5" xmlns:ns4="3244cbb2-9f52-4273-9113-8cc2cecf4979" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="54d9cecd5b552591da97f0387668823e" ns3:_="" ns4:_="">
     <xsd:import namespace="40d8dcd0-4b95-4e4d-9aa5-be2e8658acc5"/>
@@ -6163,32 +6150,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA34204B-E607-45A1-9498-394427B9D986}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="3244cbb2-9f52-4273-9113-8cc2cecf4979"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="40d8dcd0-4b95-4e4d-9aa5-be2e8658acc5"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B975CF3D-B020-4216-8822-B9E8F3D97495}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{308378B9-91A3-4988-8873-F75977EABA14}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6205,4 +6182,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B975CF3D-B020-4216-8822-B9E8F3D97495}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA34204B-E607-45A1-9498-394427B9D986}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="3244cbb2-9f52-4273-9113-8cc2cecf4979"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="40d8dcd0-4b95-4e4d-9aa5-be2e8658acc5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update: Payment and Confirmation
</commit_message>
<xml_diff>
--- a/Group C2-3 Scrum documentation.xlsx
+++ b/Group C2-3 Scrum documentation.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johna\OneDrive\Documents\University\Year II\CO553 Agile Development and Software Security B\co553-c2-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F94B983F-E502-4760-BE80-7DD49E410D82}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6F9C3BC0-A61B-406C-9E17-020980602E16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{0CC9FE5D-919A-41CA-B32D-5FFC3808111C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{0CC9FE5D-919A-41CA-B32D-5FFC3808111C}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
     <sheet name="Group C2-3 Sprint 1" sheetId="2" r:id="rId2"/>
     <sheet name="Group C2-3 Sprint 2" sheetId="5" r:id="rId3"/>
+    <sheet name="Group C2-3 Sprint 3" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="79">
   <si>
     <t>ID</t>
   </si>
@@ -47,51 +48,6 @@
   </si>
   <si>
     <t>Create databases on MySQL</t>
-  </si>
-  <si>
-    <t>As a customer i would like the films to be displayed, so that i can select the films that appeal to me</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a customer I would like to be able to buy tickets, so that I can watch movies </t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a customer i would like there to be a login option so i can easily access my account </t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a customer I want there to be a sign out option so that i can exit my session. </t>
-  </si>
-  <si>
-    <t>As a customer i would like to select my seat/seats so that i know where i will sit when i enter the screening room.</t>
-  </si>
-  <si>
-    <t>As a customer i want to have a payment selection section so that i can pay for my tickets</t>
-  </si>
-  <si>
-    <t>As customer I would like to have a booking confirmation sent to my email address so that I am assured that the payment has gone through the system</t>
-  </si>
-  <si>
-    <t>As a customer i would like there to be a guest checkout option, so that i don't have to go through the process of creating an account since i'm not a frequent customer</t>
-  </si>
-  <si>
-    <t>As a customer i would like to post my own reviews of movies so that i can inform other users who may be wanting to watch the movie.</t>
-  </si>
-  <si>
-    <t>As a customer i would like to view reviews from other users so that i can decide on whether a movie appeals to me or not.</t>
-  </si>
-  <si>
-    <t>As a customer i want to be able to edit my reviews so that i can correct any mistakes i made.</t>
-  </si>
-  <si>
-    <t>As a customer I would like to have a Membership card feature so that I can find better seats and have priority over people who hasn't bought a membership</t>
-  </si>
-  <si>
-    <t>As a customer i would like to be able to view a trending page  that shows a user the current trending movies for a week so that they can make their selection easier.</t>
-  </si>
-  <si>
-    <t>As a customer I would like technical support on the website to be available so that i can report any issues that i have</t>
-  </si>
-  <si>
-    <t>As a customer i would like to use discount codes so that i can get a percentage off a movie ticket</t>
   </si>
   <si>
     <t>As a customer I would like to be able to see the booking history of the tickets so that i can see what tickets i've previously purchased.</t>
@@ -110,9 +66,6 @@
   </si>
   <si>
     <t>As a customer I would like to be able to buy tickets so that I can watch movies [10 points]</t>
-  </si>
-  <si>
-    <t>As a customer i would like to register for an account so that I can use it to make my transactions</t>
   </si>
   <si>
     <t>As a customer i would like to register for an account so that I can use it to make my transactions [2 points]</t>
@@ -302,6 +255,69 @@
   <si>
     <t>Proceed to the booking confirmation [0.5]</t>
   </si>
+  <si>
+    <t>As a customer, I would like to post and edit reviews as well as see reviews from other viewers, so that I can inform other users who may be wanting to watch the movie and to decide on whether a movie appeals to me or not.</t>
+  </si>
+  <si>
+    <t>Add an edit button so that a user can change a review(1)</t>
+  </si>
+  <si>
+    <t>Add a post button that will upload a user review(1.5)</t>
+  </si>
+  <si>
+    <t>Create a review page(0.5)</t>
+  </si>
+  <si>
+    <t>Create a booking history page(0.5)</t>
+  </si>
+  <si>
+    <t>Retrieve booking number from database to show booking confirmation(1.5)</t>
+  </si>
+  <si>
+    <t>As a customer, I would like the films to be displayed, so that i can select the films that appeal to me</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a customer, I would like to be able to buy tickets, so that I can watch movies </t>
+  </si>
+  <si>
+    <t>As a customer, I would like to register for an account, so that I can use it to make my transactions</t>
+  </si>
+  <si>
+    <t>As a customer, I would like to select my seat/seats, so that i know where i will sit when i enter the screening room.</t>
+  </si>
+  <si>
+    <t>As a customer, I want to have a payment selection section, so that i can pay for my tickets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a customer, I want there to be a sign out option, so that i can exit my session. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a customer, I would like there to be a login option, so i can easily access my account </t>
+  </si>
+  <si>
+    <t>As a customer I would like to be able to see the booking history of the tickets, so that i can see what tickets i've previously purchased.</t>
+  </si>
+  <si>
+    <t>As a customer, I would like to be able to view a trending page  that shows a user the current trending movies for a week, so that they can make their selection easier.</t>
+  </si>
+  <si>
+    <t>As a customer, I would like to use discount codes, so that i can get a percentage off a movie ticket.</t>
+  </si>
+  <si>
+    <t>As customer, I would like to have a booking confirmation displayed, so that I am assured that the payment has gone through the system.</t>
+  </si>
+  <si>
+    <t>Create a booking page(1)</t>
+  </si>
+  <si>
+    <t>Message that includes all the booking details (database retrieval)(2)</t>
+  </si>
+  <si>
+    <t>Kezia/Sukh</t>
+  </si>
+  <si>
+    <t>Allow all users to manage their bookings(2)</t>
+  </si>
 </sst>
 </file>
 
@@ -358,7 +374,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -400,6 +416,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -567,7 +595,7 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -614,11 +642,26 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -651,6 +694,24 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1854,6 +1915,572 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" b="1"/>
+              <a:t>Burndown Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Group C2-3 Sprint 3'!$F$3:$W$3</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>44277</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44278</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44279</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44280</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44281</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44282</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44283</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44284</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44285</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44286</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44287</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44288</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>44289</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>44290</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>44291</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>44292</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>44293</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>44294</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Group C2-3 Sprint 3'!$F$12:$W$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>6.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2B48-430E-8E3E-D510A4208B87}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="668577120"/>
+        <c:axId val="668577448"/>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="668577120"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Sprint</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> Duration</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.49371158094218992"/>
+              <c:y val="0.92824013749550338"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="668577448"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="668577448"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Points Remaining</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="1.0741688844810507E-2"/>
+              <c:y val="0.4091653010378779"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="668577120"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1934,6 +2561,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -2451,6 +3118,522 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3032,6 +4215,49 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2000252</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2952751</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A8272CB-45E1-4843-8C39-BC3833B4DC8D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -3345,10 +4571,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F2ABAF1-62E6-41B4-BC47-CFBA7BD3B611}">
-  <dimension ref="B2:D21"/>
+  <dimension ref="B1:D15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:D14"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3356,221 +4582,166 @@
     <col min="3" max="3" width="149.5703125" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="B2" s="39">
         <v>1</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>2</v>
+      <c r="C2" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="39">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="34">
-        <v>1</v>
-      </c>
-      <c r="C3" s="34" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="34">
-        <v>1</v>
+      <c r="B3" s="39">
+        <v>2</v>
+      </c>
+      <c r="C3" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="39">
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="34">
-        <v>2</v>
-      </c>
-      <c r="C4" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="34">
-        <v>8</v>
+      <c r="B4" s="39">
+        <v>3</v>
+      </c>
+      <c r="C4" s="39" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" s="39">
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="34">
-        <v>3</v>
-      </c>
-      <c r="C5" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="34">
-        <v>10</v>
+      <c r="B5" s="39">
+        <v>4</v>
+      </c>
+      <c r="C5" s="39" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" s="39">
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="34">
-        <v>4</v>
-      </c>
-      <c r="C6" s="34" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="34">
-        <v>2</v>
+      <c r="B6" s="39">
+        <v>5</v>
+      </c>
+      <c r="C6" s="39" t="s">
+        <v>70</v>
+      </c>
+      <c r="D6" s="39">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="34">
-        <v>5</v>
-      </c>
-      <c r="C7" s="34" t="s">
+      <c r="B7" s="39">
         <v>6</v>
       </c>
-      <c r="D7" s="34">
+      <c r="C7" s="39" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" s="39">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="34">
-        <v>6</v>
-      </c>
-      <c r="C8" s="34" t="s">
+      <c r="B8" s="38">
         <v>7</v>
       </c>
-      <c r="D8" s="34">
-        <v>1</v>
+      <c r="C8" s="38" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" s="38">
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="35">
-        <v>7</v>
-      </c>
-      <c r="C9" s="35" t="s">
+      <c r="B9" s="38">
         <v>8</v>
       </c>
-      <c r="D9" s="35">
-        <v>8</v>
+      <c r="C9" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" s="38">
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="35">
-        <v>8</v>
-      </c>
-      <c r="C10" s="35" t="s">
+      <c r="B10" s="36">
         <v>9</v>
       </c>
-      <c r="D10" s="35">
+      <c r="C10" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="D10" s="36">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B11" s="35">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="35">
-        <v>9</v>
-      </c>
-      <c r="C11" s="35" t="s">
-        <v>10</v>
+      <c r="C11" s="37" t="s">
+        <v>58</v>
       </c>
       <c r="D11" s="35">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="30">
-        <v>10</v>
-      </c>
-      <c r="C12" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="30">
-        <v>3</v>
+      <c r="B12" s="35">
+        <v>11</v>
+      </c>
+      <c r="C12" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" s="35">
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="30">
-        <v>11</v>
-      </c>
-      <c r="C13" s="30" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="C13" s="31" t="s">
+        <v>72</v>
       </c>
       <c r="D13" s="30">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" s="30">
-        <v>12</v>
-      </c>
-      <c r="C14" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" s="30">
+        <v>13</v>
+      </c>
+      <c r="C14" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="D14" s="32">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="30">
-        <v>13</v>
-      </c>
-      <c r="C15" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" s="30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="30">
-        <v>14</v>
-      </c>
-      <c r="C16" s="31" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" s="30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="32">
-        <v>15</v>
-      </c>
-      <c r="C17" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="D17" s="32">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="30">
-        <v>16</v>
-      </c>
-      <c r="C18" s="31" t="s">
-        <v>16</v>
-      </c>
-      <c r="D18" s="30">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="32">
-        <v>17</v>
-      </c>
-      <c r="C19" s="33" t="s">
-        <v>17</v>
-      </c>
-      <c r="D19" s="32">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="32">
-        <v>18</v>
-      </c>
-      <c r="C20" s="33" t="s">
-        <v>18</v>
-      </c>
-      <c r="D20" s="32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="1"/>
+      <c r="B15" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3590,32 +4761,32 @@
   <sheetData>
     <row r="2" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="38" t="s">
-        <v>44</v>
-      </c>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
-      <c r="M2" s="38"/>
-      <c r="N2" s="38"/>
-      <c r="O2" s="38"/>
-      <c r="P2" s="38"/>
-      <c r="Q2" s="38"/>
-      <c r="R2" s="38"/>
-      <c r="S2" s="38"/>
-      <c r="T2" s="38"/>
-      <c r="U2" s="38"/>
-      <c r="V2" s="38"/>
+        <v>6</v>
+      </c>
+      <c r="D2" s="43" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="43"/>
+      <c r="L2" s="43"/>
+      <c r="M2" s="43"/>
+      <c r="N2" s="43"/>
+      <c r="O2" s="43"/>
+      <c r="P2" s="43"/>
+      <c r="Q2" s="43"/>
+      <c r="R2" s="43"/>
+      <c r="S2" s="43"/>
+      <c r="T2" s="43"/>
+      <c r="U2" s="43"/>
+      <c r="V2" s="43"/>
     </row>
     <row r="3" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B3" s="16"/>
@@ -3679,11 +4850,11 @@
       </c>
     </row>
     <row r="4" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B4" s="36" t="s">
-        <v>22</v>
+      <c r="B4" s="41" t="s">
+        <v>7</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="D4" s="9">
         <v>0</v>
@@ -3744,9 +4915,9 @@
       </c>
     </row>
     <row r="5" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B5" s="39"/>
+      <c r="B5" s="44"/>
       <c r="C5" s="6" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="D5" s="10">
         <v>0</v>
@@ -3807,9 +4978,9 @@
       </c>
     </row>
     <row r="6" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B6" s="39"/>
+      <c r="B6" s="44"/>
       <c r="C6" s="2" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="D6" s="10">
         <v>0</v>
@@ -3870,9 +5041,9 @@
       </c>
     </row>
     <row r="7" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B7" s="37"/>
+      <c r="B7" s="42"/>
       <c r="C7" s="3" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="D7" s="11">
         <v>0</v>
@@ -3933,11 +5104,11 @@
       </c>
     </row>
     <row r="8" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B8" s="36" t="s">
-        <v>23</v>
+      <c r="B8" s="41" t="s">
+        <v>8</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="D8" s="9">
         <v>0</v>
@@ -3998,9 +5169,9 @@
       </c>
     </row>
     <row r="9" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B9" s="39"/>
+      <c r="B9" s="44"/>
       <c r="C9" s="2" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="D9" s="10">
         <v>0</v>
@@ -4061,9 +5232,9 @@
       </c>
     </row>
     <row r="10" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B10" s="39"/>
+      <c r="B10" s="44"/>
       <c r="C10" s="2" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="D10" s="10">
         <v>0</v>
@@ -4124,9 +5295,9 @@
       </c>
     </row>
     <row r="11" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B11" s="39"/>
+      <c r="B11" s="44"/>
       <c r="C11" s="2" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="D11" s="10">
         <v>0</v>
@@ -4187,9 +5358,9 @@
       </c>
     </row>
     <row r="12" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B12" s="37"/>
+      <c r="B12" s="42"/>
       <c r="C12" s="3" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="D12" s="11">
         <v>0</v>
@@ -4250,11 +5421,11 @@
       </c>
     </row>
     <row r="13" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B13" s="36" t="s">
-        <v>24</v>
+      <c r="B13" s="41" t="s">
+        <v>9</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="D13" s="9">
         <v>0</v>
@@ -4315,9 +5486,9 @@
       </c>
     </row>
     <row r="14" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B14" s="39"/>
+      <c r="B14" s="44"/>
       <c r="C14" s="2" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="D14" s="10">
         <v>0</v>
@@ -4378,9 +5549,9 @@
       </c>
     </row>
     <row r="15" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B15" s="39"/>
+      <c r="B15" s="44"/>
       <c r="C15" s="2" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="D15" s="10">
         <v>0</v>
@@ -4441,9 +5612,9 @@
       </c>
     </row>
     <row r="16" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B16" s="37"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="3" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="D16" s="11">
         <v>0</v>
@@ -4504,11 +5675,11 @@
       </c>
     </row>
     <row r="17" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B17" s="36" t="s">
-        <v>26</v>
+      <c r="B17" s="41" t="s">
+        <v>10</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="D17" s="9">
         <v>0</v>
@@ -4569,9 +5740,9 @@
       </c>
     </row>
     <row r="18" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B18" s="39"/>
+      <c r="B18" s="44"/>
       <c r="C18" s="2" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="D18" s="10">
         <v>0</v>
@@ -4632,9 +5803,9 @@
       </c>
     </row>
     <row r="19" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B19" s="37"/>
+      <c r="B19" s="42"/>
       <c r="C19" s="3" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="D19" s="11">
         <v>0</v>
@@ -4695,11 +5866,11 @@
       </c>
     </row>
     <row r="20" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B20" s="36" t="s">
-        <v>27</v>
+      <c r="B20" s="41" t="s">
+        <v>11</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="D20" s="9">
         <v>0</v>
@@ -4760,9 +5931,9 @@
       </c>
     </row>
     <row r="21" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B21" s="37"/>
+      <c r="B21" s="42"/>
       <c r="C21" s="3" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="D21" s="11">
         <v>0</v>
@@ -4823,11 +5994,11 @@
       </c>
     </row>
     <row r="22" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B22" s="36" t="s">
-        <v>28</v>
+      <c r="B22" s="41" t="s">
+        <v>12</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="D22" s="9">
         <v>0</v>
@@ -4888,9 +6059,9 @@
       </c>
     </row>
     <row r="23" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B23" s="37"/>
+      <c r="B23" s="42"/>
       <c r="C23" s="3" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="D23" s="11">
         <v>0</v>
@@ -5038,7 +6209,7 @@
     <mergeCell ref="B17:B19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -5047,7 +6218,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B40D316F-9AC3-40B6-9034-2229B798232F}">
   <dimension ref="B2:AE24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
@@ -5061,19 +6232,19 @@
   <sheetData>
     <row r="2" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="F2" s="25" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="G2" s="25"/>
       <c r="H2" s="25"/>
@@ -5092,14 +6263,14 @@
       <c r="U2" s="25"/>
       <c r="V2" s="25"/>
       <c r="W2" s="25"/>
-      <c r="X2" s="43"/>
-      <c r="Y2" s="43"/>
-      <c r="Z2" s="43"/>
-      <c r="AA2" s="43"/>
-      <c r="AB2" s="43"/>
-      <c r="AC2" s="43"/>
-      <c r="AD2" s="43"/>
-      <c r="AE2" s="43"/>
+      <c r="X2" s="48"/>
+      <c r="Y2" s="48"/>
+      <c r="Z2" s="48"/>
+      <c r="AA2" s="48"/>
+      <c r="AB2" s="48"/>
+      <c r="AC2" s="48"/>
+      <c r="AD2" s="48"/>
+      <c r="AE2" s="48"/>
     </row>
     <row r="3" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B3" s="16"/>
@@ -5186,17 +6357,17 @@
       </c>
     </row>
     <row r="4" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B4" s="40" t="s">
-        <v>50</v>
-      </c>
-      <c r="C4" s="44">
+      <c r="B4" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="49">
         <v>10</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="F4" s="9"/>
       <c r="M4" s="2"/>
@@ -5221,13 +6392,13 @@
       <c r="AE4" s="12"/>
     </row>
     <row r="5" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B5" s="41"/>
-      <c r="C5" s="45"/>
+      <c r="B5" s="46"/>
+      <c r="C5" s="50"/>
       <c r="D5" s="28" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="F5" s="10"/>
       <c r="L5">
@@ -5254,13 +6425,13 @@
       <c r="AE5" s="13"/>
     </row>
     <row r="6" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B6" s="41"/>
-      <c r="C6" s="45"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="50"/>
       <c r="D6" s="28" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="E6" s="27" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="F6" s="10"/>
       <c r="I6">
@@ -5293,13 +6464,13 @@
       <c r="AE6" s="13"/>
     </row>
     <row r="7" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B7" s="42"/>
-      <c r="C7" s="46"/>
+      <c r="B7" s="47"/>
+      <c r="C7" s="51"/>
       <c r="D7" s="29" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="F7" s="11"/>
       <c r="G7" s="3">
@@ -5333,17 +6504,17 @@
       <c r="AE7" s="14"/>
     </row>
     <row r="8" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B8" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="C8" s="44">
+      <c r="B8" s="45" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="49">
         <v>10</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="F8" s="9"/>
       <c r="M8" s="8"/>
@@ -5369,13 +6540,13 @@
       <c r="AE8" s="12"/>
     </row>
     <row r="9" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B9" s="41"/>
-      <c r="C9" s="45"/>
+      <c r="B9" s="46"/>
+      <c r="C9" s="50"/>
       <c r="D9" s="28" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="E9" s="27" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="F9" s="10"/>
       <c r="M9" s="2"/>
@@ -5402,13 +6573,13 @@
       <c r="AE9" s="13"/>
     </row>
     <row r="10" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B10" s="41"/>
-      <c r="C10" s="45"/>
+      <c r="B10" s="46"/>
+      <c r="C10" s="50"/>
       <c r="D10" s="28" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="E10" s="27" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="F10" s="10"/>
       <c r="M10" s="2"/>
@@ -5436,13 +6607,13 @@
       </c>
     </row>
     <row r="11" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B11" s="41"/>
-      <c r="C11" s="45"/>
+      <c r="B11" s="46"/>
+      <c r="C11" s="50"/>
       <c r="D11" s="28" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="E11" s="27" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="F11" s="10"/>
       <c r="M11" s="2"/>
@@ -5467,13 +6638,13 @@
       <c r="AE11" s="13"/>
     </row>
     <row r="12" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B12" s="42"/>
-      <c r="C12" s="46"/>
+      <c r="B12" s="47"/>
+      <c r="C12" s="51"/>
       <c r="D12" s="29" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="F12" s="11"/>
       <c r="M12" s="3"/>
@@ -5498,17 +6669,17 @@
       <c r="AE12" s="14"/>
     </row>
     <row r="13" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B13" s="40" t="s">
-        <v>52</v>
-      </c>
-      <c r="C13" s="44">
+      <c r="B13" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="49">
         <v>6</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="F13" s="9"/>
       <c r="G13" s="8"/>
@@ -5533,13 +6704,13 @@
       <c r="AE13" s="12"/>
     </row>
     <row r="14" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B14" s="41"/>
-      <c r="C14" s="45"/>
+      <c r="B14" s="46"/>
+      <c r="C14" s="50"/>
       <c r="D14" s="28" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="E14" s="27" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="F14" s="10"/>
       <c r="G14" s="2"/>
@@ -5565,13 +6736,13 @@
       <c r="AE14" s="13"/>
     </row>
     <row r="15" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B15" s="41"/>
-      <c r="C15" s="45"/>
+      <c r="B15" s="46"/>
+      <c r="C15" s="50"/>
       <c r="D15" s="28" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="E15" s="27" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="F15" s="10"/>
       <c r="G15" s="2"/>
@@ -5597,13 +6768,13 @@
       <c r="AE15" s="13"/>
     </row>
     <row r="16" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B16" s="42"/>
-      <c r="C16" s="46"/>
+      <c r="B16" s="47"/>
+      <c r="C16" s="51"/>
       <c r="D16" s="29" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="E16" s="27" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="F16" s="10"/>
       <c r="G16" s="2"/>
@@ -5922,12 +7093,586 @@
     <mergeCell ref="C13:C16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEB650AB-BCC2-4621-B350-229143F7398D}">
+  <dimension ref="B2:W19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="109.85546875" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" customWidth="1"/>
+    <col min="4" max="4" width="99.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="25"/>
+      <c r="N2" s="25"/>
+      <c r="O2" s="25"/>
+      <c r="P2" s="25"/>
+      <c r="Q2" s="25"/>
+      <c r="R2" s="25"/>
+      <c r="S2" s="25"/>
+      <c r="T2" s="25"/>
+      <c r="U2" s="25"/>
+      <c r="V2" s="25"/>
+      <c r="W2" s="25"/>
+    </row>
+    <row r="3" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="5">
+        <v>44277</v>
+      </c>
+      <c r="G3" s="5">
+        <v>44278</v>
+      </c>
+      <c r="H3" s="5">
+        <v>44279</v>
+      </c>
+      <c r="I3" s="5">
+        <v>44280</v>
+      </c>
+      <c r="J3" s="5">
+        <v>44281</v>
+      </c>
+      <c r="K3" s="5">
+        <v>44282</v>
+      </c>
+      <c r="L3" s="5">
+        <v>44283</v>
+      </c>
+      <c r="M3" s="5">
+        <v>44284</v>
+      </c>
+      <c r="N3" s="5">
+        <v>44285</v>
+      </c>
+      <c r="O3" s="5">
+        <v>44286</v>
+      </c>
+      <c r="P3" s="5">
+        <v>44287</v>
+      </c>
+      <c r="Q3" s="5">
+        <v>44288</v>
+      </c>
+      <c r="R3" s="5">
+        <v>44289</v>
+      </c>
+      <c r="S3" s="5">
+        <v>44290</v>
+      </c>
+      <c r="T3" s="5">
+        <v>44291</v>
+      </c>
+      <c r="U3" s="5">
+        <v>44292</v>
+      </c>
+      <c r="V3" s="5">
+        <v>44293</v>
+      </c>
+      <c r="W3" s="5">
+        <v>44294</v>
+      </c>
+    </row>
+    <row r="4" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="54" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" s="56">
+        <v>5</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" s="9">
+        <v>1</v>
+      </c>
+      <c r="M4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2"/>
+      <c r="W4" s="12"/>
+    </row>
+    <row r="5" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B5" s="55"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" s="10"/>
+      <c r="H5">
+        <v>2</v>
+      </c>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="13"/>
+    </row>
+    <row r="6" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B6" s="55"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="E6" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="F6" s="11"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3">
+        <v>1</v>
+      </c>
+      <c r="K6" s="3">
+        <v>1</v>
+      </c>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="14"/>
+    </row>
+    <row r="7" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B7" s="52" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" s="49">
+        <v>3</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="10"/>
+      <c r="M7" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+      <c r="U7" s="2"/>
+      <c r="V7" s="2"/>
+      <c r="W7" s="13"/>
+    </row>
+    <row r="8" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B8" s="53"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="10"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="V8" s="2"/>
+      <c r="W8" s="13"/>
+    </row>
+    <row r="9" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B9" s="53"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="E9" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="11"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
+      <c r="T9" s="3"/>
+      <c r="U9" s="3"/>
+      <c r="V9" s="3"/>
+      <c r="W9" s="14"/>
+    </row>
+    <row r="10" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B10" s="52" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="49">
+        <v>2</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10" s="10"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="U10" s="2"/>
+      <c r="V10" s="2"/>
+      <c r="W10" s="13"/>
+    </row>
+    <row r="11" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B11" s="53"/>
+      <c r="C11" s="50"/>
+      <c r="D11" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="E11" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="10"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="U11" s="2"/>
+      <c r="W11" s="13"/>
+    </row>
+    <row r="12" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="8">
+        <f>12 - SUM(F4:F11)</f>
+        <v>11</v>
+      </c>
+      <c r="G12" s="9">
+        <f t="shared" ref="G12:W12" si="0">F12-SUM(G4:G11)</f>
+        <v>11</v>
+      </c>
+      <c r="H12" s="9">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="I12" s="9">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="J12" s="9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="K12" s="9">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="L12" s="9">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="M12" s="9">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="N12" s="9">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="O12" s="9">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="P12" s="9">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="Q12" s="9">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="R12" s="9">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="S12" s="9">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="T12" s="9">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="U12" s="9">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="V12" s="9">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="W12" s="15">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="13" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B13" s="34"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="2"/>
+      <c r="S13" s="2"/>
+      <c r="T13" s="2"/>
+      <c r="U13" s="2"/>
+      <c r="V13" s="2"/>
+      <c r="W13" s="2"/>
+    </row>
+    <row r="14" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B14" s="34"/>
+      <c r="C14" s="34"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="2"/>
+      <c r="S14" s="2"/>
+      <c r="T14" s="2"/>
+      <c r="U14" s="2"/>
+      <c r="V14" s="2"/>
+      <c r="W14" s="2"/>
+    </row>
+    <row r="15" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B15" s="34"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2"/>
+      <c r="R15" s="2"/>
+      <c r="S15" s="2"/>
+      <c r="T15" s="2"/>
+      <c r="U15" s="2"/>
+      <c r="V15" s="2"/>
+      <c r="W15" s="2"/>
+    </row>
+    <row r="16" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2"/>
+      <c r="R16" s="2"/>
+      <c r="S16" s="2"/>
+      <c r="T16" s="2"/>
+      <c r="U16" s="2"/>
+      <c r="V16" s="2"/>
+      <c r="W16" s="2"/>
+    </row>
+    <row r="17" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B17" s="34"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+      <c r="P17" s="2"/>
+      <c r="Q17" s="2"/>
+      <c r="R17" s="2"/>
+      <c r="S17" s="2"/>
+      <c r="T17" s="2"/>
+      <c r="U17" s="2"/>
+      <c r="V17" s="2"/>
+      <c r="W17" s="2"/>
+    </row>
+    <row r="18" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B18" s="34"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
+      <c r="R18" s="2"/>
+      <c r="S18" s="2"/>
+      <c r="T18" s="2"/>
+      <c r="U18" s="2"/>
+      <c r="V18" s="2"/>
+      <c r="W18" s="2"/>
+    </row>
+    <row r="19" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="2"/>
+      <c r="R19" s="2"/>
+      <c r="S19" s="2"/>
+      <c r="T19" s="2"/>
+      <c r="U19" s="2"/>
+      <c r="V19" s="2"/>
+      <c r="W19" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="C4:C6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010007C60AE6480C8D49900E7A4362DC978A" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2c8c8df2ae4c8b52ea756b3d40f22f1c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="40d8dcd0-4b95-4e4d-9aa5-be2e8658acc5" xmlns:ns4="3244cbb2-9f52-4273-9113-8cc2cecf4979" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="54d9cecd5b552591da97f0387668823e" ns3:_="" ns4:_="">
     <xsd:import namespace="40d8dcd0-4b95-4e4d-9aa5-be2e8658acc5"/>
@@ -6150,7 +7895,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -6159,13 +7904,24 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA34204B-E607-45A1-9498-394427B9D986}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="3244cbb2-9f52-4273-9113-8cc2cecf4979"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="40d8dcd0-4b95-4e4d-9aa5-be2e8658acc5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{308378B9-91A3-4988-8873-F75977EABA14}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6184,27 +7940,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B975CF3D-B020-4216-8822-B9E8F3D97495}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA34204B-E607-45A1-9498-394427B9D986}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="3244cbb2-9f52-4273-9113-8cc2cecf4979"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="40d8dcd0-4b95-4e4d-9aa5-be2e8658acc5"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update: Changes made to the sprint documentation
</commit_message>
<xml_diff>
--- a/Group C2-3 Scrum documentation.xlsx
+++ b/Group C2-3 Scrum documentation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johna\OneDrive\Documents\University\Year II\CO553 Agile Development and Software Security B\co553-c2-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6F9C3BC0-A61B-406C-9E17-020980602E16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88D1FE26-7432-46AC-B5E3-C03F3D9264D0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{0CC9FE5D-919A-41CA-B32D-5FFC3808111C}"/>
   </bookViews>
@@ -2108,25 +2108,25 @@
                   <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6.5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6.5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6.5</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>6.5</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>6.5</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>6.5</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>6.5</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7103,7 +7103,7 @@
   <dimension ref="B2:W19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+      <selection activeCell="S44" sqref="S44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7382,6 +7382,9 @@
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
+      <c r="Q10">
+        <v>0.5</v>
+      </c>
       <c r="U10" s="2"/>
       <c r="V10" s="2"/>
       <c r="W10" s="13"/>
@@ -7402,6 +7405,9 @@
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
+      <c r="S11">
+        <v>1</v>
+      </c>
       <c r="U11" s="2"/>
       <c r="W11" s="13"/>
     </row>
@@ -7456,31 +7462,31 @@
       </c>
       <c r="Q12" s="9">
         <f t="shared" si="0"/>
-        <v>6.5</v>
+        <v>6</v>
       </c>
       <c r="R12" s="9">
         <f t="shared" si="0"/>
-        <v>6.5</v>
+        <v>6</v>
       </c>
       <c r="S12" s="9">
         <f t="shared" si="0"/>
-        <v>6.5</v>
+        <v>5</v>
       </c>
       <c r="T12" s="9">
         <f t="shared" si="0"/>
-        <v>6.5</v>
+        <v>5</v>
       </c>
       <c r="U12" s="9">
         <f t="shared" si="0"/>
-        <v>6.5</v>
+        <v>5</v>
       </c>
       <c r="V12" s="9">
         <f t="shared" si="0"/>
-        <v>6.5</v>
+        <v>5</v>
       </c>
       <c r="W12" s="15">
         <f t="shared" si="0"/>
-        <v>6.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="2:23" x14ac:dyDescent="0.25">
@@ -7667,9 +7673,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7896,27 +7905,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA34204B-E607-45A1-9498-394427B9D986}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B975CF3D-B020-4216-8822-B9E8F3D97495}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="3244cbb2-9f52-4273-9113-8cc2cecf4979"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="40d8dcd0-4b95-4e4d-9aa5-be2e8658acc5"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -7941,9 +7938,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B975CF3D-B020-4216-8822-B9E8F3D97495}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA34204B-E607-45A1-9498-394427B9D986}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="3244cbb2-9f52-4273-9113-8cc2cecf4979"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="40d8dcd0-4b95-4e4d-9aa5-be2e8658acc5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update: Final Submission Reel Website
</commit_message>
<xml_diff>
--- a/Group C2-3 Scrum documentation.xlsx
+++ b/Group C2-3 Scrum documentation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johna\OneDrive\Documents\University\Year II\CO553 Agile Development and Software Security B\co553-c2-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88D1FE26-7432-46AC-B5E3-C03F3D9264D0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA16CBC1-C8BE-4338-89CB-690AF5D0A5E3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{0CC9FE5D-919A-41CA-B32D-5FFC3808111C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="77">
   <si>
     <t>ID</t>
   </si>
@@ -259,9 +259,6 @@
     <t>As a customer, I would like to post and edit reviews as well as see reviews from other viewers, so that I can inform other users who may be wanting to watch the movie and to decide on whether a movie appeals to me or not.</t>
   </si>
   <si>
-    <t>Add an edit button so that a user can change a review(1)</t>
-  </si>
-  <si>
     <t>Add a post button that will upload a user review(1.5)</t>
   </si>
   <si>
@@ -298,12 +295,6 @@
     <t>As a customer I would like to be able to see the booking history of the tickets, so that i can see what tickets i've previously purchased.</t>
   </si>
   <si>
-    <t>As a customer, I would like to be able to view a trending page  that shows a user the current trending movies for a week, so that they can make their selection easier.</t>
-  </si>
-  <si>
-    <t>As a customer, I would like to use discount codes, so that i can get a percentage off a movie ticket.</t>
-  </si>
-  <si>
     <t>As customer, I would like to have a booking confirmation displayed, so that I am assured that the payment has gone through the system.</t>
   </si>
   <si>
@@ -317,6 +308,9 @@
   </si>
   <si>
     <t>Allow all users to manage their bookings(2)</t>
+  </si>
+  <si>
+    <t>Indicate whether the user is an account holder or guest in the review(1)</t>
   </si>
 </sst>
 </file>
@@ -374,7 +368,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -416,18 +410,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -595,7 +577,7 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -637,31 +619,20 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -713,6 +684,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -2075,58 +2049,58 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>11</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.5</c:v>
+                  <c:v>4.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6.5</c:v>
+                  <c:v>4.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6.5</c:v>
+                  <c:v>4.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>6.5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5</c:v>
+                  <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>5</c:v>
+                  <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>5</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4236,15 +4210,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>2000252</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>184150</xdr:rowOff>
+      <xdr:colOff>2013859</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>102507</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>2952751</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:colOff>2966358</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>45357</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4571,10 +4545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F2ABAF1-62E6-41B4-BC47-CFBA7BD3B611}">
-  <dimension ref="B1:D15"/>
+  <dimension ref="B1:E15"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4582,7 +4556,7 @@
     <col min="3" max="3" width="149.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
@@ -4593,150 +4567,134 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="39">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B2" s="33">
         <v>1</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="39">
+      <c r="D2" s="33">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="39">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="33">
         <v>2</v>
       </c>
-      <c r="C3" s="39" t="s">
+      <c r="C3" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3" s="33">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="33">
+        <v>3</v>
+      </c>
+      <c r="C4" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="D3" s="39">
+      <c r="D4" s="33">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="33">
+        <v>4</v>
+      </c>
+      <c r="C5" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="D5" s="33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="33">
+        <v>5</v>
+      </c>
+      <c r="C6" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="33">
+        <v>6</v>
+      </c>
+      <c r="C7" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="34">
+        <v>7</v>
+      </c>
+      <c r="C8" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="D8" s="34">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="39">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="34">
+        <v>8</v>
+      </c>
+      <c r="C9" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="D9" s="34">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="34">
+        <v>9</v>
+      </c>
+      <c r="C10" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="D10" s="34">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B11" s="30">
+        <v>10</v>
+      </c>
+      <c r="C11" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" s="30">
         <v>3</v>
       </c>
-      <c r="C4" s="39" t="s">
-        <v>65</v>
-      </c>
-      <c r="D4" s="39">
-        <v>10</v>
-      </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="39">
-        <v>4</v>
-      </c>
-      <c r="C5" s="39" t="s">
-        <v>66</v>
-      </c>
-      <c r="D5" s="39">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="53">
+        <v>11</v>
+      </c>
+      <c r="C12" s="53" t="s">
+        <v>70</v>
+      </c>
+      <c r="D12" s="53">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="39">
-        <v>5</v>
-      </c>
-      <c r="C6" s="39" t="s">
-        <v>70</v>
-      </c>
-      <c r="D6" s="39">
-        <v>1</v>
-      </c>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E13" s="2"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="39">
-        <v>6</v>
-      </c>
-      <c r="C7" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="D7" s="39">
-        <v>1</v>
-      </c>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E14" s="2"/>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="38">
-        <v>7</v>
-      </c>
-      <c r="C8" s="38" t="s">
-        <v>67</v>
-      </c>
-      <c r="D8" s="38">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="38">
-        <v>8</v>
-      </c>
-      <c r="C9" s="38" t="s">
-        <v>68</v>
-      </c>
-      <c r="D9" s="38">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="36">
-        <v>9</v>
-      </c>
-      <c r="C10" s="36" t="s">
-        <v>74</v>
-      </c>
-      <c r="D10" s="36">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B11" s="35">
-        <v>10</v>
-      </c>
-      <c r="C11" s="37" t="s">
-        <v>58</v>
-      </c>
-      <c r="D11" s="35">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="35">
-        <v>11</v>
-      </c>
-      <c r="C12" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="D12" s="35">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="30">
-        <v>12</v>
-      </c>
-      <c r="C13" s="31" t="s">
-        <v>72</v>
-      </c>
-      <c r="D13" s="30">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="30">
-        <v>13</v>
-      </c>
-      <c r="C14" s="33" t="s">
-        <v>73</v>
-      </c>
-      <c r="D14" s="32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
     </row>
   </sheetData>
@@ -4766,27 +4724,27 @@
       <c r="C2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="43" t="s">
+      <c r="D2" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
-      <c r="K2" s="43"/>
-      <c r="L2" s="43"/>
-      <c r="M2" s="43"/>
-      <c r="N2" s="43"/>
-      <c r="O2" s="43"/>
-      <c r="P2" s="43"/>
-      <c r="Q2" s="43"/>
-      <c r="R2" s="43"/>
-      <c r="S2" s="43"/>
-      <c r="T2" s="43"/>
-      <c r="U2" s="43"/>
-      <c r="V2" s="43"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="38"/>
+      <c r="P2" s="38"/>
+      <c r="Q2" s="38"/>
+      <c r="R2" s="38"/>
+      <c r="S2" s="38"/>
+      <c r="T2" s="38"/>
+      <c r="U2" s="38"/>
+      <c r="V2" s="38"/>
     </row>
     <row r="3" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B3" s="16"/>
@@ -4850,7 +4808,7 @@
       </c>
     </row>
     <row r="4" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="36" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="6" t="s">
@@ -4915,7 +4873,7 @@
       </c>
     </row>
     <row r="5" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B5" s="44"/>
+      <c r="B5" s="39"/>
       <c r="C5" s="6" t="s">
         <v>31</v>
       </c>
@@ -4978,7 +4936,7 @@
       </c>
     </row>
     <row r="6" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B6" s="44"/>
+      <c r="B6" s="39"/>
       <c r="C6" s="2" t="s">
         <v>30</v>
       </c>
@@ -5041,7 +4999,7 @@
       </c>
     </row>
     <row r="7" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B7" s="42"/>
+      <c r="B7" s="37"/>
       <c r="C7" s="3" t="s">
         <v>29</v>
       </c>
@@ -5104,7 +5062,7 @@
       </c>
     </row>
     <row r="8" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B8" s="41" t="s">
+      <c r="B8" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="8" t="s">
@@ -5169,7 +5127,7 @@
       </c>
     </row>
     <row r="9" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B9" s="44"/>
+      <c r="B9" s="39"/>
       <c r="C9" s="2" t="s">
         <v>14</v>
       </c>
@@ -5232,7 +5190,7 @@
       </c>
     </row>
     <row r="10" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B10" s="44"/>
+      <c r="B10" s="39"/>
       <c r="C10" s="2" t="s">
         <v>15</v>
       </c>
@@ -5295,7 +5253,7 @@
       </c>
     </row>
     <row r="11" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B11" s="44"/>
+      <c r="B11" s="39"/>
       <c r="C11" s="2" t="s">
         <v>16</v>
       </c>
@@ -5358,7 +5316,7 @@
       </c>
     </row>
     <row r="12" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B12" s="42"/>
+      <c r="B12" s="37"/>
       <c r="C12" s="3" t="s">
         <v>17</v>
       </c>
@@ -5421,7 +5379,7 @@
       </c>
     </row>
     <row r="13" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B13" s="41" t="s">
+      <c r="B13" s="36" t="s">
         <v>9</v>
       </c>
       <c r="C13" s="8" t="s">
@@ -5486,7 +5444,7 @@
       </c>
     </row>
     <row r="14" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B14" s="44"/>
+      <c r="B14" s="39"/>
       <c r="C14" s="2" t="s">
         <v>19</v>
       </c>
@@ -5549,7 +5507,7 @@
       </c>
     </row>
     <row r="15" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B15" s="44"/>
+      <c r="B15" s="39"/>
       <c r="C15" s="2" t="s">
         <v>20</v>
       </c>
@@ -5612,7 +5570,7 @@
       </c>
     </row>
     <row r="16" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B16" s="42"/>
+      <c r="B16" s="37"/>
       <c r="C16" s="3" t="s">
         <v>21</v>
       </c>
@@ -5675,7 +5633,7 @@
       </c>
     </row>
     <row r="17" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B17" s="41" t="s">
+      <c r="B17" s="36" t="s">
         <v>10</v>
       </c>
       <c r="C17" s="8" t="s">
@@ -5740,7 +5698,7 @@
       </c>
     </row>
     <row r="18" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B18" s="44"/>
+      <c r="B18" s="39"/>
       <c r="C18" s="2" t="s">
         <v>22</v>
       </c>
@@ -5803,7 +5761,7 @@
       </c>
     </row>
     <row r="19" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B19" s="42"/>
+      <c r="B19" s="37"/>
       <c r="C19" s="3" t="s">
         <v>23</v>
       </c>
@@ -5866,7 +5824,7 @@
       </c>
     </row>
     <row r="20" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B20" s="41" t="s">
+      <c r="B20" s="36" t="s">
         <v>11</v>
       </c>
       <c r="C20" s="8" t="s">
@@ -5931,7 +5889,7 @@
       </c>
     </row>
     <row r="21" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B21" s="42"/>
+      <c r="B21" s="37"/>
       <c r="C21" s="3" t="s">
         <v>25</v>
       </c>
@@ -5994,7 +5952,7 @@
       </c>
     </row>
     <row r="22" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B22" s="41" t="s">
+      <c r="B22" s="36" t="s">
         <v>12</v>
       </c>
       <c r="C22" s="8" t="s">
@@ -6059,7 +6017,7 @@
       </c>
     </row>
     <row r="23" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B23" s="42"/>
+      <c r="B23" s="37"/>
       <c r="C23" s="3" t="s">
         <v>27</v>
       </c>
@@ -6263,14 +6221,14 @@
       <c r="U2" s="25"/>
       <c r="V2" s="25"/>
       <c r="W2" s="25"/>
-      <c r="X2" s="48"/>
-      <c r="Y2" s="48"/>
-      <c r="Z2" s="48"/>
-      <c r="AA2" s="48"/>
-      <c r="AB2" s="48"/>
-      <c r="AC2" s="48"/>
-      <c r="AD2" s="48"/>
-      <c r="AE2" s="48"/>
+      <c r="X2" s="43"/>
+      <c r="Y2" s="43"/>
+      <c r="Z2" s="43"/>
+      <c r="AA2" s="43"/>
+      <c r="AB2" s="43"/>
+      <c r="AC2" s="43"/>
+      <c r="AD2" s="43"/>
+      <c r="AE2" s="43"/>
     </row>
     <row r="3" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B3" s="16"/>
@@ -6357,10 +6315,10 @@
       </c>
     </row>
     <row r="4" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="49">
+      <c r="C4" s="44">
         <v>10</v>
       </c>
       <c r="D4" s="15" t="s">
@@ -6392,8 +6350,8 @@
       <c r="AE4" s="12"/>
     </row>
     <row r="5" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B5" s="46"/>
-      <c r="C5" s="50"/>
+      <c r="B5" s="41"/>
+      <c r="C5" s="45"/>
       <c r="D5" s="28" t="s">
         <v>46</v>
       </c>
@@ -6425,8 +6383,8 @@
       <c r="AE5" s="13"/>
     </row>
     <row r="6" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B6" s="46"/>
-      <c r="C6" s="50"/>
+      <c r="B6" s="41"/>
+      <c r="C6" s="45"/>
       <c r="D6" s="28" t="s">
         <v>47</v>
       </c>
@@ -6464,8 +6422,8 @@
       <c r="AE6" s="13"/>
     </row>
     <row r="7" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B7" s="47"/>
-      <c r="C7" s="51"/>
+      <c r="B7" s="42"/>
+      <c r="C7" s="46"/>
       <c r="D7" s="29" t="s">
         <v>48</v>
       </c>
@@ -6504,10 +6462,10 @@
       <c r="AE7" s="14"/>
     </row>
     <row r="8" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B8" s="45" t="s">
+      <c r="B8" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="49">
+      <c r="C8" s="44">
         <v>10</v>
       </c>
       <c r="D8" s="15" t="s">
@@ -6540,8 +6498,8 @@
       <c r="AE8" s="12"/>
     </row>
     <row r="9" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B9" s="46"/>
-      <c r="C9" s="50"/>
+      <c r="B9" s="41"/>
+      <c r="C9" s="45"/>
       <c r="D9" s="28" t="s">
         <v>50</v>
       </c>
@@ -6573,8 +6531,8 @@
       <c r="AE9" s="13"/>
     </row>
     <row r="10" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B10" s="46"/>
-      <c r="C10" s="50"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="45"/>
       <c r="D10" s="28" t="s">
         <v>51</v>
       </c>
@@ -6607,8 +6565,8 @@
       </c>
     </row>
     <row r="11" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B11" s="46"/>
-      <c r="C11" s="50"/>
+      <c r="B11" s="41"/>
+      <c r="C11" s="45"/>
       <c r="D11" s="28" t="s">
         <v>52</v>
       </c>
@@ -6638,8 +6596,8 @@
       <c r="AE11" s="13"/>
     </row>
     <row r="12" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B12" s="47"/>
-      <c r="C12" s="51"/>
+      <c r="B12" s="42"/>
+      <c r="C12" s="46"/>
       <c r="D12" s="29" t="s">
         <v>53</v>
       </c>
@@ -6669,10 +6627,10 @@
       <c r="AE12" s="14"/>
     </row>
     <row r="13" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B13" s="45" t="s">
+      <c r="B13" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="49">
+      <c r="C13" s="44">
         <v>6</v>
       </c>
       <c r="D13" s="15" t="s">
@@ -6704,8 +6662,8 @@
       <c r="AE13" s="12"/>
     </row>
     <row r="14" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B14" s="46"/>
-      <c r="C14" s="50"/>
+      <c r="B14" s="41"/>
+      <c r="C14" s="45"/>
       <c r="D14" s="28" t="s">
         <v>55</v>
       </c>
@@ -6736,8 +6694,8 @@
       <c r="AE14" s="13"/>
     </row>
     <row r="15" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B15" s="46"/>
-      <c r="C15" s="50"/>
+      <c r="B15" s="41"/>
+      <c r="C15" s="45"/>
       <c r="D15" s="28" t="s">
         <v>56</v>
       </c>
@@ -6768,8 +6726,8 @@
       <c r="AE15" s="13"/>
     </row>
     <row r="16" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B16" s="47"/>
-      <c r="C16" s="51"/>
+      <c r="B16" s="42"/>
+      <c r="C16" s="46"/>
       <c r="D16" s="29" t="s">
         <v>57</v>
       </c>
@@ -7102,8 +7060,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEB650AB-BCC2-4621-B350-229143F7398D}">
   <dimension ref="B2:W19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="S44" sqref="S44"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7209,14 +7167,14 @@
       </c>
     </row>
     <row r="4" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="54" t="s">
-        <v>74</v>
-      </c>
-      <c r="C4" s="56">
+      <c r="B4" s="49" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" s="51">
         <v>5</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>41</v>
@@ -7232,10 +7190,10 @@
       <c r="W4" s="12"/>
     </row>
     <row r="5" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B5" s="55"/>
-      <c r="C5" s="57"/>
+      <c r="B5" s="50"/>
+      <c r="C5" s="52"/>
       <c r="D5" s="28" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>39</v>
@@ -7257,13 +7215,13 @@
       <c r="W5" s="13"/>
     </row>
     <row r="6" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B6" s="55"/>
-      <c r="C6" s="57"/>
+      <c r="B6" s="50"/>
+      <c r="C6" s="52"/>
       <c r="D6" s="28" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E6" s="27" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F6" s="11"/>
       <c r="G6" s="3"/>
@@ -7289,14 +7247,14 @@
       <c r="W6" s="14"/>
     </row>
     <row r="7" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B7" s="52" t="s">
+      <c r="B7" s="47" t="s">
         <v>58</v>
       </c>
-      <c r="C7" s="49">
+      <c r="C7" s="44">
         <v>3</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>40</v>
@@ -7316,10 +7274,10 @@
       <c r="W7" s="13"/>
     </row>
     <row r="8" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B8" s="53"/>
-      <c r="C8" s="50"/>
+      <c r="B8" s="48"/>
+      <c r="C8" s="45"/>
       <c r="D8" s="28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E8" s="27" t="s">
         <v>42</v>
@@ -7328,17 +7286,19 @@
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
+      <c r="P8" s="2">
+        <v>1.5</v>
+      </c>
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
       <c r="V8" s="2"/>
       <c r="W8" s="13"/>
     </row>
     <row r="9" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B9" s="53"/>
-      <c r="C9" s="50"/>
+      <c r="B9" s="48"/>
+      <c r="C9" s="45"/>
       <c r="D9" s="28" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="E9" s="27" t="s">
         <v>42</v>
@@ -7359,18 +7319,20 @@
       <c r="S9" s="3"/>
       <c r="T9" s="3"/>
       <c r="U9" s="3"/>
-      <c r="V9" s="3"/>
+      <c r="V9" s="3">
+        <v>1</v>
+      </c>
       <c r="W9" s="14"/>
     </row>
     <row r="10" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B10" s="52" t="s">
+      <c r="B10" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="49">
+      <c r="C10" s="44">
         <v>2</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E10" s="8" t="s">
         <v>39</v>
@@ -7390,10 +7352,10 @@
       <c r="W10" s="13"/>
     </row>
     <row r="11" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B11" s="53"/>
-      <c r="C11" s="50"/>
-      <c r="D11" s="40" t="s">
-        <v>63</v>
+      <c r="B11" s="48"/>
+      <c r="C11" s="45"/>
+      <c r="D11" s="32" t="s">
+        <v>62</v>
       </c>
       <c r="E11" s="27" t="s">
         <v>41</v>
@@ -7408,7 +7370,9 @@
       <c r="S11">
         <v>1</v>
       </c>
-      <c r="U11" s="2"/>
+      <c r="U11" s="2">
+        <v>0.5</v>
+      </c>
       <c r="W11" s="13"/>
     </row>
     <row r="12" spans="2:23" x14ac:dyDescent="0.25">
@@ -7417,81 +7381,81 @@
       <c r="D12" s="8"/>
       <c r="E12" s="12"/>
       <c r="F12" s="8">
-        <f>12 - SUM(F4:F11)</f>
-        <v>11</v>
+        <f>10 - SUM(F4:F11)</f>
+        <v>9</v>
       </c>
       <c r="G12" s="9">
         <f t="shared" ref="G12:W12" si="0">F12-SUM(G4:G11)</f>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H12" s="9">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I12" s="9">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="J12" s="9">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K12" s="9">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="L12" s="9">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="M12" s="9">
         <f t="shared" si="0"/>
-        <v>6.5</v>
+        <v>4.5</v>
       </c>
       <c r="N12" s="9">
         <f t="shared" si="0"/>
-        <v>6.5</v>
+        <v>4.5</v>
       </c>
       <c r="O12" s="9">
         <f t="shared" si="0"/>
-        <v>6.5</v>
+        <v>4.5</v>
       </c>
       <c r="P12" s="9">
         <f t="shared" si="0"/>
-        <v>6.5</v>
+        <v>3</v>
       </c>
       <c r="Q12" s="9">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>2.5</v>
       </c>
       <c r="R12" s="9">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>2.5</v>
       </c>
       <c r="S12" s="9">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>1.5</v>
       </c>
       <c r="T12" s="9">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>1.5</v>
       </c>
       <c r="U12" s="9">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="V12" s="9">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="W12" s="15">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B13" s="34"/>
-      <c r="C13" s="34"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="31"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
@@ -7514,8 +7478,8 @@
       <c r="W13" s="2"/>
     </row>
     <row r="14" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B14" s="34"/>
-      <c r="C14" s="34"/>
+      <c r="B14" s="31"/>
+      <c r="C14" s="31"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
@@ -7538,8 +7502,8 @@
       <c r="W14" s="2"/>
     </row>
     <row r="15" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B15" s="34"/>
-      <c r="C15" s="34"/>
+      <c r="B15" s="31"/>
+      <c r="C15" s="31"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
@@ -7562,8 +7526,8 @@
       <c r="W15" s="2"/>
     </row>
     <row r="16" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B16" s="34"/>
-      <c r="C16" s="34"/>
+      <c r="B16" s="31"/>
+      <c r="C16" s="31"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
@@ -7586,8 +7550,8 @@
       <c r="W16" s="2"/>
     </row>
     <row r="17" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B17" s="34"/>
-      <c r="C17" s="34"/>
+      <c r="B17" s="31"/>
+      <c r="C17" s="31"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
@@ -7610,8 +7574,8 @@
       <c r="W17" s="2"/>
     </row>
     <row r="18" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B18" s="34"/>
-      <c r="C18" s="34"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="31"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
@@ -7673,12 +7637,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7905,15 +7866,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B975CF3D-B020-4216-8822-B9E8F3D97495}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA34204B-E607-45A1-9498-394427B9D986}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="3244cbb2-9f52-4273-9113-8cc2cecf4979"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="40d8dcd0-4b95-4e4d-9aa5-be2e8658acc5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -7938,18 +7911,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA34204B-E607-45A1-9498-394427B9D986}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B975CF3D-B020-4216-8822-B9E8F3D97495}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="3244cbb2-9f52-4273-9113-8cc2cecf4979"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="40d8dcd0-4b95-4e4d-9aa5-be2e8658acc5"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>